<commit_message>
new admin helper,testdata and testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07BEC07-E808-4557-A115-D96C9BD6E2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33F0B0-0C9B-4C86-9651-9EE00241D915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="1020" windowWidth="15360" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="115">
   <si>
     <t>DataSet</t>
   </si>
@@ -351,6 +350,30 @@
   </si>
   <si>
     <t>https://mcloud-na-stage.hydroflask.com/</t>
+  </si>
+  <si>
+    <t>videoUrl</t>
+  </si>
+  <si>
+    <t>https://youtu.be/tysrAXqAP1k</t>
+  </si>
+  <si>
+    <t>mobilelayout</t>
+  </si>
+  <si>
+    <t>Stacked</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>#343434</t>
+  </si>
+  <si>
+    <t>TextColor</t>
   </si>
 </sst>
 </file>
@@ -360,7 +383,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -444,6 +467,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -725,13 +749,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN33"/>
+  <dimension ref="A1:AR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM19" sqref="AM19"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO5" sqref="AO5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
@@ -766,7 +790,7 @@
     <col min="37" max="37" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="9.140625" bestFit="1" customWidth="1"/>
@@ -814,7 +838,7 @@
     <col min="86" max="86" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -935,8 +959,20 @@
       <c r="AN1" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:40">
+      <c r="AO1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -970,7 +1006,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1003,7 +1039,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="7"/>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1040,7 +1076,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:40" ht="24.75" customHeight="1">
+    <row r="5" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1068,7 +1104,7 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="8"/>
     </row>
-    <row r="6" spans="1:40" ht="13.5" customHeight="1">
+    <row r="6" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1098,7 +1134,7 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1123,7 +1159,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1148,7 +1184,7 @@
       <c r="R8" s="5"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1167,7 +1203,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1190,7 +1226,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:40" s="2" customFormat="1">
+    <row r="11" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -1210,7 +1246,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1235,7 +1271,7 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:40" ht="14.25" customHeight="1">
+    <row r="13" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1258,7 +1294,7 @@
       <c r="AI13" s="1"/>
       <c r="AJ13" s="8"/>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1296,7 +1332,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1319,7 +1355,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -1327,7 +1363,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -1335,7 +1371,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="14.25" customHeight="1">
+    <row r="18" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1345,7 +1381,7 @@
       </c>
       <c r="AJ18" s="8"/>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -1379,12 +1415,24 @@
       <c r="AN19" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="20" spans="1:40">
+      <c r="AO19" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AF20" s="6"/>
       <c r="AG20" s="7"/>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1398,7 +1446,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1413,7 +1461,7 @@
       <c r="Q22" s="4"/>
       <c r="AF22" s="9"/>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1428,7 +1476,7 @@
       <c r="Q24" s="4"/>
       <c r="X24" s="4"/>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="E25" s="10"/>
       <c r="F25" s="4"/>
@@ -1446,7 +1494,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1460,7 +1508,7 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="33" spans="3:17">
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1485,8 +1533,9 @@
     <hyperlink ref="B2" r:id="rId6" xr:uid="{A6EF088F-EADE-4859-A9B4-308887E697F1}"/>
     <hyperlink ref="F14" r:id="rId7" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
     <hyperlink ref="AN19" r:id="rId8" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="AO19" r:id="rId9" xr:uid="{CA5410D8-F4B4-4C34-89E0-72BD40B5E41B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
country selector new admin test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33F0B0-0C9B-4C86-9651-9EE00241D915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84555974-D3BB-4E9A-A0DA-FB9B2D5B9DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="122">
   <si>
     <t>DataSet</t>
   </si>
@@ -374,6 +374,27 @@
   </si>
   <si>
     <t>TextColor</t>
+  </si>
+  <si>
+    <t>IsEnabled</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com//</t>
   </si>
 </sst>
 </file>
@@ -749,9 +770,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR33"/>
+  <dimension ref="A1:AU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AO5" sqref="AO5"/>
     </sheetView>
   </sheetViews>
@@ -778,67 +799,69 @@
     <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="11.28515625" customWidth="1"/>
+    <col min="30" max="30" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" customWidth="1"/>
+    <col min="36" max="36" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="161.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="146.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="15" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="8" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="14" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="161.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="146.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="17" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="14" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -921,58 +944,67 @@
         <v>26</v>
       </c>
       <c r="AB1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1006,7 +1038,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1036,10 +1068,11 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="7"/>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="7"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1073,10 +1106,11 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="7"/>
-    </row>
-    <row r="5" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="7"/>
+    </row>
+    <row r="5" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1101,10 +1135,10 @@
       <c r="P5" t="s">
         <v>54</v>
       </c>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="8"/>
-    </row>
-    <row r="6" spans="1:44" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="8"/>
+    </row>
+    <row r="6" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1134,7 +1168,7 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1159,7 +1193,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1184,7 +1218,7 @@
       <c r="R8" s="5"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1203,7 +1237,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1226,7 +1260,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -1246,7 +1280,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1271,7 +1305,7 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1291,10 +1325,10 @@
       <c r="L13" t="s">
         <v>77</v>
       </c>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="8"/>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="8"/>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1331,57 +1365,74 @@
       <c r="AA14" s="12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
+      <c r="I15" t="s">
+        <v>74</v>
+      </c>
       <c r="W15" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="AB15" s="5" t="s">
+      <c r="AB15" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AC15" s="5" t="s">
+      <c r="AE15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AD15" s="9" t="s">
+      <c r="AF15" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AE15" s="14" t="s">
+      <c r="AG15" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AF15" s="13" t="s">
+      <c r="AH15" s="13" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AI15" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ15" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>
-      <c r="AG16" s="9" t="s">
+      <c r="AJ16" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
-      <c r="AH17" s="9" t="s">
+      <c r="AK17" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>99</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="AI18" t="s">
+      <c r="AL18" t="s">
         <v>100</v>
       </c>
-      <c r="AJ18" s="8"/>
-    </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AM18" s="8"/>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -1399,40 +1450,41 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
-      <c r="AI19" s="1"/>
-      <c r="AJ19" t="s">
+      <c r="AL19" s="1"/>
+      <c r="AM19" t="s">
         <v>102</v>
       </c>
-      <c r="AK19" t="s">
+      <c r="AN19" t="s">
         <v>103</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AO19" t="s">
         <v>104</v>
       </c>
-      <c r="AM19" t="s">
+      <c r="AP19" t="s">
         <v>105</v>
       </c>
-      <c r="AN19" s="4" t="s">
+      <c r="AQ19" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AO19" s="15" t="s">
+      <c r="AR19" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="AP19" t="s">
+      <c r="AS19" t="s">
         <v>110</v>
       </c>
-      <c r="AQ19" t="s">
+      <c r="AT19" t="s">
         <v>112</v>
       </c>
-      <c r="AR19" t="s">
+      <c r="AU19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AF20" s="6"/>
-      <c r="AG20" s="7"/>
-    </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="7"/>
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1446,7 +1498,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1459,9 +1511,10 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
-      <c r="AF22" s="9"/>
-    </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1476,7 +1529,7 @@
       <c r="Q24" s="4"/>
       <c r="X24" s="4"/>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="E25" s="10"/>
       <c r="F25" s="4"/>
@@ -1494,7 +1547,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1532,10 +1585,11 @@
     <hyperlink ref="B4" r:id="rId5" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
     <hyperlink ref="B2" r:id="rId6" xr:uid="{A6EF088F-EADE-4859-A9B4-308887E697F1}"/>
     <hyperlink ref="F14" r:id="rId7" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
-    <hyperlink ref="AN19" r:id="rId8" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="AO19" r:id="rId9" xr:uid="{CA5410D8-F4B4-4C34-89E0-72BD40B5E41B}"/>
+    <hyperlink ref="AQ19" r:id="rId8" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="AR19" r:id="rId9" xr:uid="{CA5410D8-F4B4-4C34-89E0-72BD40B5E41B}"/>
+    <hyperlink ref="AQ15" r:id="rId10" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
admin promo media card content
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84555974-D3BB-4E9A-A0DA-FB9B2D5B9DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177260C3-2A69-4E8A-BA17-D3F3634B3D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="129">
   <si>
     <t>DataSet</t>
   </si>
@@ -346,55 +346,76 @@
     <t>Fixed</t>
   </si>
   <si>
+    <t>https://mcloud-na-stage.hydroflask.com/</t>
+  </si>
+  <si>
+    <t>videoUrl</t>
+  </si>
+  <si>
+    <t>https://youtu.be/tysrAXqAP1k</t>
+  </si>
+  <si>
+    <t>mobilelayout</t>
+  </si>
+  <si>
+    <t>Stacked</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>#343434</t>
+  </si>
+  <si>
+    <t>TextColor</t>
+  </si>
+  <si>
+    <t>IsEnabled</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com//</t>
+  </si>
+  <si>
+    <t>CTA Type</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>CTA Link</t>
+  </si>
+  <si>
+    <t>CTA Edit</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com/QATestingHydro</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>W32075</t>
+  </si>
+  <si>
     <t>qaFlask</t>
-  </si>
-  <si>
-    <t>https://mcloud-na-stage.hydroflask.com/</t>
-  </si>
-  <si>
-    <t>videoUrl</t>
-  </si>
-  <si>
-    <t>https://youtu.be/tysrAXqAP1k</t>
-  </si>
-  <si>
-    <t>mobilelayout</t>
-  </si>
-  <si>
-    <t>Stacked</t>
-  </si>
-  <si>
-    <t>heading</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>#343434</t>
-  </si>
-  <si>
-    <t>TextColor</t>
-  </si>
-  <si>
-    <t>IsEnabled</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>North America</t>
-  </si>
-  <si>
-    <t>https://mcloud-na-stage.hydroflask.com//</t>
   </si>
 </sst>
 </file>
@@ -770,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU33"/>
+  <dimension ref="A1:AW33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO5" sqref="AO5"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AP19" sqref="AP19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +833,7 @@
     <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -861,7 +882,7 @@
     <col min="89" max="89" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -944,10 +965,10 @@
         <v>26</v>
       </c>
       <c r="AB1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>27</v>
@@ -965,7 +986,7 @@
         <v>31</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AJ1" s="3" t="s">
         <v>32</v>
@@ -992,19 +1013,25 @@
         <v>39</v>
       </c>
       <c r="AR1" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AS1" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AT1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AU1" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1038,7 +1065,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1072,7 +1099,7 @@
       <c r="AI3" s="6"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1110,7 +1137,7 @@
       <c r="AI4" s="6"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1138,7 +1165,7 @@
       <c r="AL5" s="1"/>
       <c r="AM5" s="8"/>
     </row>
-    <row r="6" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1168,7 +1195,7 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1193,7 +1220,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1218,7 +1245,7 @@
       <c r="R8" s="5"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1237,7 +1264,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1260,7 +1287,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -1280,7 +1307,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1305,7 +1332,7 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1328,7 +1355,7 @@
       <c r="AL13" s="1"/>
       <c r="AM13" s="8"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1368,7 +1395,7 @@
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1379,10 +1406,10 @@
         <v>90</v>
       </c>
       <c r="AB15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC15" t="s">
         <v>117</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>118</v>
       </c>
       <c r="AD15" s="5" t="s">
         <v>91</v>
@@ -1400,13 +1427,13 @@
         <v>84</v>
       </c>
       <c r="AI15" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ15" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AQ15" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -1414,7 +1441,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -1422,7 +1449,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1432,7 +1459,7 @@
       </c>
       <c r="AM18" s="8"/>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -1461,30 +1488,54 @@
         <v>104</v>
       </c>
       <c r="AP19" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ19" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AQ19" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="AR19" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AS19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AT19" t="s">
+        <v>111</v>
+      </c>
+      <c r="AU19" t="s">
         <v>112</v>
       </c>
-      <c r="AU19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="7"/>
-    </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AK20" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ20" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV20" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1498,7 +1549,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1514,7 +1565,7 @@
       <c r="AH22" s="9"/>
       <c r="AI22" s="9"/>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1529,7 +1580,7 @@
       <c r="Q24" s="4"/>
       <c r="X24" s="4"/>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="E25" s="10"/>
       <c r="F25" s="4"/>
@@ -1547,7 +1598,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1588,8 +1639,9 @@
     <hyperlink ref="AQ19" r:id="rId8" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
     <hyperlink ref="AR19" r:id="rId9" xr:uid="{CA5410D8-F4B4-4C34-89E0-72BD40B5E41B}"/>
     <hyperlink ref="AQ15" r:id="rId10" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="AQ20" r:id="rId11" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gold Admim PromoBlock Component test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177260C3-2A69-4E8A-BA17-D3F3634B3D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8BE8FE-8969-41EC-A369-5974216EC868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="136">
   <si>
     <t>DataSet</t>
   </si>
@@ -154,12 +154,6 @@
     <t>AccountDetails</t>
   </si>
   <si>
-    <t>avayugundla@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Axnstqjguhqy1!</t>
-  </si>
-  <si>
     <t>Dashboard / Magento Admin</t>
   </si>
   <si>
@@ -416,6 +410,33 @@
   </si>
   <si>
     <t>qaFlask</t>
+  </si>
+  <si>
+    <t>EditContentSection</t>
+  </si>
+  <si>
+    <t>QA Testing on Promo Block Components-Content Changes</t>
+  </si>
+  <si>
+    <t>QA Test/Promo Block-Content</t>
+  </si>
+  <si>
+    <t>CTAElements</t>
+  </si>
+  <si>
+    <t>QATESTINGHYDRO</t>
+  </si>
+  <si>
+    <t>QAHYDRO</t>
+  </si>
+  <si>
+    <t>QA test for the hydrflask and promo content</t>
+  </si>
+  <si>
+    <t>CTAText</t>
+  </si>
+  <si>
+    <t>CTAurl</t>
   </si>
 </sst>
 </file>
@@ -791,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW33"/>
+  <dimension ref="A1:AY33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AP19" sqref="AP19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +862,7 @@
     <col min="48" max="48" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="161.42578125" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -882,7 +903,7 @@
     <col min="89" max="89" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -965,10 +986,10 @@
         <v>26</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>27</v>
@@ -986,7 +1007,7 @@
         <v>31</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AJ1" s="3" t="s">
         <v>32</v>
@@ -1013,34 +1034,36 @@
         <v>39</v>
       </c>
       <c r="AR1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AT1" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="AU1" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AV1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AW1" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1054,7 +1077,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
@@ -1065,9 +1088,9 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4"/>
       <c r="F3" s="4"/>
@@ -1083,10 +1106,10 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
@@ -1099,18 +1122,18 @@
       <c r="AI3" s="6"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1122,7 +1145,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R4" s="5"/>
       <c r="S4" s="4"/>
@@ -1137,18 +1160,18 @@
       <c r="AI4" s="6"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:49" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1160,18 +1183,18 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL5" s="1"/>
       <c r="AM5" s="8"/>
     </row>
-    <row r="6" spans="1:49" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1183,7 +1206,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -1195,9 +1218,9 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="4"/>
       <c r="F7" s="4"/>
@@ -1213,16 +1236,16 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1232,28 +1255,28 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="5"/>
@@ -1264,52 +1287,52 @@
       <c r="R9" s="5"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" t="s">
+      <c r="Q10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10" t="s">
         <v>65</v>
       </c>
-      <c r="M10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="R11" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>68</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>70</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1319,149 +1342,149 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" s="4"/>
       <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" t="s">
         <v>73</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>74</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>75</v>
-      </c>
-      <c r="K13" t="s">
-        <v>76</v>
-      </c>
-      <c r="L13" t="s">
-        <v>77</v>
       </c>
       <c r="AL13" s="1"/>
       <c r="AM13" s="8"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
         <v>78</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E14" t="s">
+      <c r="T14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="V14" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="T14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="U14" s="5" t="s">
+      <c r="W14" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="V14" s="12" t="s">
+      <c r="X14" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="W14" s="13" t="s">
+      <c r="Y14" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="X14" s="13" t="s">
+      <c r="Z14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Y14" s="13" t="s">
+      <c r="AA14" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="Z14" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA14" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" t="s">
+        <v>72</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I15" t="s">
-        <v>74</v>
-      </c>
-      <c r="W15" s="13" t="s">
+      <c r="AE15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AB15" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC15" t="s">
+      <c r="AF15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG15" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH15" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI15" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="AD15" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF15" s="9" t="s">
+      <c r="AQ15" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="AG15" s="14" t="s">
+      <c r="AJ16" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AH15" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI15" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ15" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="AJ16" s="9" t="s">
+      <c r="AK17" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>97</v>
-      </c>
-      <c r="AK17" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>99</v>
       </c>
       <c r="C18" s="4"/>
       <c r="AL18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AM18" s="8"/>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1475,81 +1498,94 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="R19" t="s">
+        <v>133</v>
+      </c>
       <c r="S19" s="4"/>
       <c r="AL19" s="1"/>
       <c r="AM19" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO19" t="s">
         <v>102</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="AP19" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AO19" t="s">
-        <v>104</v>
-      </c>
-      <c r="AP19" t="s">
-        <v>128</v>
-      </c>
-      <c r="AQ19" s="4" t="s">
+      <c r="AR19" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="AR19" s="15" t="s">
+      <c r="AS19" t="s">
         <v>107</v>
       </c>
-      <c r="AS19" t="s">
+      <c r="AT19" t="s">
         <v>109</v>
       </c>
-      <c r="AT19" t="s">
-        <v>111</v>
-      </c>
       <c r="AU19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="7"/>
       <c r="AK20" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AQ20" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AR20" t="s">
         <v>39</v>
       </c>
       <c r="AS20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AT20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AV20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AW20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1564,8 +1600,20 @@
       <c r="Q22" s="4"/>
       <c r="AH22" s="9"/>
       <c r="AI22" s="9"/>
-    </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AP22" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ22" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY22" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1580,7 +1628,7 @@
       <c r="Q24" s="4"/>
       <c r="X24" s="4"/>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="E25" s="10"/>
       <c r="F25" s="4"/>
@@ -1598,7 +1646,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1634,14 +1682,15 @@
     <hyperlink ref="F5" r:id="rId3" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{A6EF088F-EADE-4859-A9B4-308887E697F1}"/>
-    <hyperlink ref="F14" r:id="rId7" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
-    <hyperlink ref="AQ19" r:id="rId8" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="AR19" r:id="rId9" xr:uid="{CA5410D8-F4B4-4C34-89E0-72BD40B5E41B}"/>
-    <hyperlink ref="AQ15" r:id="rId10" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="AQ20" r:id="rId11" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="F14" r:id="rId6" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
+    <hyperlink ref="AQ19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="AR19" r:id="rId8" xr:uid="{CA5410D8-F4B4-4C34-89E0-72BD40B5E41B}"/>
+    <hyperlink ref="AQ15" r:id="rId9" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="AQ20" r:id="rId10" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="AQ22" r:id="rId11" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="AY22" r:id="rId12" xr:uid="{ED44CB44-A563-49C0-BA70-BC4941FCD5E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Admin testcase product tile, chat bot, authenticated user HF Commit.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,33 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8BE8FE-8969-41EC-A369-5974216EC868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B3F6C6-CB49-4EB5-9DFA-040BDC8A6238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="199">
   <si>
     <t>DataSet</t>
   </si>
@@ -343,27 +334,12 @@
     <t>https://mcloud-na-stage.hydroflask.com/</t>
   </si>
   <si>
-    <t>videoUrl</t>
-  </si>
-  <si>
-    <t>https://youtu.be/tysrAXqAP1k</t>
-  </si>
-  <si>
     <t>mobilelayout</t>
   </si>
   <si>
-    <t>Stacked</t>
-  </si>
-  <si>
     <t>heading</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>#343434</t>
-  </si>
-  <si>
     <t>TextColor</t>
   </si>
   <si>
@@ -403,9 +379,6 @@
     <t>https://mcloud-na-stage.hydroflask.com/QATestingHydro</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>W32075</t>
   </si>
   <si>
@@ -418,25 +391,232 @@
     <t>QA Testing on Promo Block Components-Content Changes</t>
   </si>
   <si>
-    <t>QA Test/Promo Block-Content</t>
-  </si>
-  <si>
     <t>CTAElements</t>
   </si>
   <si>
     <t>QATESTINGHYDRO</t>
   </si>
   <si>
-    <t>QAHYDRO</t>
-  </si>
-  <si>
-    <t>QA test for the hydrflask and promo content</t>
-  </si>
-  <si>
     <t>CTAText</t>
   </si>
   <si>
     <t>CTAurl</t>
+  </si>
+  <si>
+    <t>skatipelli@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Aoypzjceqraq1!</t>
+  </si>
+  <si>
+    <t>Tiletext</t>
+  </si>
+  <si>
+    <t>textbutton</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>CategorySelect</t>
+  </si>
+  <si>
+    <t>productnames</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>VideoURL</t>
+  </si>
+  <si>
+    <t>CardTitle</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Buttontext</t>
+  </si>
+  <si>
+    <t>Buttontype</t>
+  </si>
+  <si>
+    <t>ButtonLinknavigation</t>
+  </si>
+  <si>
+    <t>Categorydisplay</t>
+  </si>
+  <si>
+    <t>No.ofproductsdisplay</t>
+  </si>
+  <si>
+    <t>productcategory</t>
+  </si>
+  <si>
+    <t>Editpagetitle</t>
+  </si>
+  <si>
+    <t>datacontenttype</t>
+  </si>
+  <si>
+    <t>Deletcomponent</t>
+  </si>
+  <si>
+    <t>LOTUSQATITLE</t>
+  </si>
+  <si>
+    <t>LOTUSQABUTTON</t>
+  </si>
+  <si>
+    <t>m-media-card</t>
+  </si>
+  <si>
+    <t>tiles__wrapper</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>W32075,W32410,W32520,1115580,1165700,1071499B</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Copper Brown,32 oz Wide Mouth - Everest Blue,32 oz Wide Mouth - Acai Purple</t>
+  </si>
+  <si>
+    <t>Price: high to low</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/V_58eaD1NII</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVE</t>
+  </si>
+  <si>
+    <t>QATesting</t>
+  </si>
+  <si>
+    <t>#a8d098</t>
+  </si>
+  <si>
+    <t>demo-desktop_3.png</t>
+  </si>
+  <si>
+    <t>QATEST</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Shop,Bottles</t>
+  </si>
+  <si>
+    <t>Bottles</t>
+  </si>
+  <si>
+    <t>Edit Card Tiles</t>
+  </si>
+  <si>
+    <t>hot_card_tiles</t>
+  </si>
+  <si>
+    <t>hot-card-tiles</t>
+  </si>
+  <si>
+    <t>OXO 10-Piece POP Container Set,3-Piece Mixing Bowl Set,Cherry &amp; Olive Pitter</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.oxo.com/</t>
+  </si>
+  <si>
+    <t>#a8d099</t>
+  </si>
+  <si>
+    <t>plp-block</t>
+  </si>
+  <si>
+    <t>c-plp-cms-block</t>
+  </si>
+  <si>
+    <t>Phone.png</t>
+  </si>
+  <si>
+    <t>Edit PLP Block</t>
+  </si>
+  <si>
+    <t>hot_plp_block</t>
+  </si>
+  <si>
+    <t>type-wrapper</t>
+  </si>
+  <si>
+    <t>c-clp-hero</t>
+  </si>
+  <si>
+    <t>Lotusqa.png</t>
+  </si>
+  <si>
+    <t>Edit CLP Hero Banner</t>
+  </si>
+  <si>
+    <t>hot_clp_banner</t>
+  </si>
+  <si>
+    <t>The page is for Testing only.</t>
+  </si>
+  <si>
+    <t>Lotus Testing the CLP Hero banner</t>
+  </si>
+  <si>
+    <t>The page has been deleted.</t>
+  </si>
+  <si>
+    <t>headingtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description Type</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>QALOTUSTEST</t>
+  </si>
+  <si>
+    <t>ProductcardTile</t>
+  </si>
+  <si>
+    <t>OXOproducttile</t>
+  </si>
+  <si>
+    <t>PLPBLOCK</t>
+  </si>
+  <si>
+    <t>Qatest2</t>
+  </si>
+  <si>
+    <t>message_3.png</t>
+  </si>
+  <si>
+    <t>CLPHerobanner</t>
+  </si>
+  <si>
+    <t>OXOCLPHerobanner</t>
+  </si>
+  <si>
+    <t>mkoppanadam@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Acyqadtkonic1!</t>
   </si>
 </sst>
 </file>
@@ -446,7 +626,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,13 +638,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1F497D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -520,17 +693,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -812,98 +987,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY33"/>
+  <dimension ref="A1:BT33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="B2:D2"/>
+    <sheetView tabSelected="1" topLeftCell="BH7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BL10" sqref="BL10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.42578125" customWidth="1"/>
-    <col min="12" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" customWidth="1"/>
-    <col min="17" max="17" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="68.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="11.28515625" customWidth="1"/>
-    <col min="30" max="30" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.140625" customWidth="1"/>
-    <col min="36" max="36" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="161.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="146.85546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="17" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="14" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7265625" customWidth="1"/>
+    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.453125" customWidth="1"/>
+    <col min="12" max="12" width="49.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7265625" customWidth="1"/>
+    <col min="16" max="16" width="89.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7265625" customWidth="1"/>
+    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17" customWidth="1"/>
+    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="17.54296875" customWidth="1"/>
+    <col min="29" max="29" width="14.7265625" customWidth="1"/>
+    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.7265625" customWidth="1"/>
+    <col min="34" max="34" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.7265625" customWidth="1"/>
+    <col min="36" max="36" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="68.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="38" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="11.26953125" customWidth="1"/>
+    <col min="52" max="52" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.1796875" customWidth="1"/>
+    <col min="58" max="58" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="49.6328125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="161.453125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="146.81640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="15" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="12" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="17" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="14" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="5" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -922,22 +1116,22 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
@@ -953,117 +1147,184 @@
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BH1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="BR1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="AJ1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="AY1" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BS1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1076,9 +1337,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
@@ -1087,12 +1346,41 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="4"/>
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1105,12 +1393,8 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
@@ -1118,11 +1402,37 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="7"/>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6"/>
+      <c r="BF3" s="7"/>
+    </row>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1147,7 +1457,8 @@
       <c r="P4" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="5"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -1156,11 +1467,30 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
-      <c r="AJ4" s="7"/>
-    </row>
-    <row r="5" spans="1:51" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="4"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="BD4" s="6"/>
+      <c r="BE4" s="6"/>
+      <c r="BF4" s="7"/>
+    </row>
+    <row r="5" spans="1:72" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1185,10 +1515,30 @@
       <c r="P5" t="s">
         <v>52</v>
       </c>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="8"/>
-    </row>
-    <row r="6" spans="1:51" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="8"/>
+    </row>
+    <row r="6" spans="1:72" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1208,6 +1558,7 @@
       <c r="P6" t="s">
         <v>52</v>
       </c>
+      <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -1217,8 +1568,27 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="4"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="4"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+    </row>
+    <row r="7" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1235,15 +1605,37 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO7" s="4"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+    </row>
+    <row r="8" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1262,13 +1654,35 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="R8" s="5"/>
-      <c r="S8" s="4"/>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="4"/>
+    </row>
+    <row r="9" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1283,11 +1697,33 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
       <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="4"/>
+    </row>
+    <row r="10" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1303,14 +1739,16 @@
       <c r="O10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="R10" t="s">
+      <c r="AN10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1323,14 +1761,16 @@
       <c r="O11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="AN11" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1349,13 +1789,35 @@
         <v>69</v>
       </c>
       <c r="P12" s="4"/>
-      <c r="Q12" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="1:51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="4"/>
+    </row>
+    <row r="13" spans="1:72" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1375,10 +1837,10 @@
       <c r="L13" t="s">
         <v>75</v>
       </c>
-      <c r="AL13" s="1"/>
-      <c r="AM13" s="8"/>
-    </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BH13" s="1"/>
+      <c r="BI13" s="8"/>
+    </row>
+    <row r="14" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1391,98 +1853,117 @@
       <c r="F14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="Q14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AP14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="AQ14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V14" s="12" t="s">
+      <c r="AR14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="W14" s="13" t="s">
+      <c r="AS14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="X14" s="13" t="s">
+      <c r="AT14" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="Y14" s="13" t="s">
+      <c r="AU14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="Z14" s="13" t="s">
+      <c r="AV14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AA14" s="12" t="s">
+      <c r="AW14" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
-    </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AX14" s="11"/>
+      <c r="AY14" s="11"/>
+    </row>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
       <c r="I15" t="s">
         <v>72</v>
       </c>
-      <c r="W15" s="13" t="s">
+      <c r="AS15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AB15" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD15" s="5" t="s">
+      <c r="AX15" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AZ15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AE15" s="5" t="s">
+      <c r="BA15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AF15" s="9" t="s">
+      <c r="BB15" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AG15" s="14" t="s">
+      <c r="BC15" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="AH15" s="13" t="s">
+      <c r="BD15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="AI15" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ15" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BE15" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="BM15" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:72" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="AJ16" s="9" t="s">
+      <c r="BF16" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="AK17" s="9" t="s">
+      <c r="BG17" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:67" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="AL18" t="s">
+      <c r="BH18" t="s">
         <v>98</v>
       </c>
-      <c r="AM18" s="8"/>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BI18" s="8"/>
+    </row>
+    <row r="19" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1495,74 +1976,76 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="O19" t="s">
+        <v>185</v>
+      </c>
       <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" t="s">
-        <v>133</v>
-      </c>
-      <c r="S19" s="4"/>
-      <c r="AL19" s="1"/>
-      <c r="AM19" t="s">
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
+      <c r="AM19" s="4"/>
+      <c r="AO19" s="4"/>
+      <c r="BH19" s="1"/>
+      <c r="BI19" t="s">
         <v>100</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="BJ19" t="s">
         <v>101</v>
       </c>
-      <c r="AO19" t="s">
+      <c r="BK19" t="s">
         <v>102</v>
       </c>
-      <c r="AP19" t="s">
-        <v>126</v>
-      </c>
-      <c r="AQ19" s="4" t="s">
+      <c r="BL19" t="s">
+        <v>120</v>
+      </c>
+      <c r="BM19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AR19" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS19" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT19" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>122</v>
-      </c>
-      <c r="AH20" s="6"/>
-      <c r="AI20" s="6"/>
-      <c r="AJ20" s="7"/>
-      <c r="AK20" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="AQ20" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR20" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS20" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT20" t="s">
-        <v>124</v>
-      </c>
-      <c r="AV20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
+      <c r="BD20" s="6"/>
+      <c r="BE20" s="6"/>
+      <c r="BF20" s="7"/>
+      <c r="BG20" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="BM20" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1571,20 +2054,36 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="4"/>
+      <c r="AL21" s="4"/>
+      <c r="AM21" s="4"/>
+    </row>
+    <row r="22" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1597,70 +2096,361 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="AH22" s="9"/>
-      <c r="AI22" s="9"/>
-      <c r="AP22" t="s">
-        <v>131</v>
-      </c>
-      <c r="AQ22" s="15" t="s">
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="4"/>
+      <c r="AM22" s="4"/>
+      <c r="BD22" s="9"/>
+      <c r="BE22" s="9"/>
+      <c r="BL22" t="s">
+        <v>124</v>
+      </c>
+      <c r="BM22" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AX22" t="s">
-        <v>132</v>
-      </c>
-      <c r="AY22" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+    </row>
+    <row r="23" spans="1:67" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>190</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="O23" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>149</v>
+      </c>
+      <c r="R23" t="s">
+        <v>150</v>
+      </c>
+      <c r="S23" t="s">
+        <v>151</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="W23" t="s">
+        <v>156</v>
+      </c>
+      <c r="X23" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y23" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA23" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB23" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD23" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE23" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF23" s="4">
+        <v>3</v>
+      </c>
+      <c r="AG23" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH23" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AI23" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ23" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AO23" s="4"/>
+      <c r="AR23" t="s">
+        <v>185</v>
+      </c>
+      <c r="BG23" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BI23" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK23" s="6"/>
+      <c r="BL23" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM23" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:67" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>191</v>
+      </c>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="X24" s="4"/>
-    </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="C25" s="4"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="Q24" t="s">
+        <v>149</v>
+      </c>
+      <c r="R24" t="s">
+        <v>150</v>
+      </c>
+      <c r="S24" t="s">
+        <v>151</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="V24" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="W24" t="s">
+        <v>156</v>
+      </c>
+      <c r="X24" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y24" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA24" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB24" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC24" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD24" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF24" s="4">
+        <v>3</v>
+      </c>
+      <c r="AG24" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH24" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AI24" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ24" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AO24" s="4"/>
+      <c r="BI24" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="BK24" s="6"/>
+      <c r="BL24" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM24" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>192</v>
+      </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
       <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-    </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-    </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>149</v>
+      </c>
+      <c r="R25" t="s">
+        <v>150</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI25" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ25" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="4"/>
+      <c r="AN25" s="4"/>
+      <c r="AO25" s="4"/>
+      <c r="AP25" s="4"/>
+      <c r="AQ25" s="4"/>
+      <c r="AR25" s="4"/>
+      <c r="AS25" s="4"/>
+      <c r="AT25" s="4"/>
+      <c r="AU25" s="4"/>
+      <c r="AV25" s="4"/>
+      <c r="BL25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BN25" t="s">
+        <v>193</v>
+      </c>
+      <c r="BO25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>195</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="P26" s="4"/>
+      <c r="Q26" t="s">
+        <v>149</v>
+      </c>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA26" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI26" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AJ26" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK26" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AL26" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AN26" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO26" s="4"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="4"/>
+      <c r="AR26" s="4"/>
+      <c r="AS26" s="4"/>
+      <c r="AT26" s="4"/>
+      <c r="AU26" s="4"/>
+      <c r="AV26" s="4"/>
+      <c r="BK26" s="9"/>
+      <c r="BL26" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM26" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>196</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>149</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AO27" s="4"/>
+    </row>
+    <row r="33" spans="3:39" x14ac:dyDescent="0.35">
       <c r="C33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1674,6 +2464,28 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="4"/>
+      <c r="AI33" s="4"/>
+      <c r="AJ33" s="4"/>
+      <c r="AK33" s="4"/>
+      <c r="AL33" s="4"/>
+      <c r="AM33" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1683,14 +2495,21 @@
     <hyperlink ref="C4" r:id="rId4" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
     <hyperlink ref="F14" r:id="rId6" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
-    <hyperlink ref="AQ19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="AR19" r:id="rId8" xr:uid="{CA5410D8-F4B4-4C34-89E0-72BD40B5E41B}"/>
-    <hyperlink ref="AQ15" r:id="rId9" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="AQ20" r:id="rId10" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
-    <hyperlink ref="AQ22" r:id="rId11" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="AY22" r:id="rId12" xr:uid="{ED44CB44-A563-49C0-BA70-BC4941FCD5E3}"/>
+    <hyperlink ref="BM19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="BM15" r:id="rId8" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="BM20" r:id="rId9" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="BM22" r:id="rId10" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="B2" r:id="rId11" xr:uid="{93DFD34B-00AC-4EAF-86FA-A13945460604}"/>
+    <hyperlink ref="Y23" r:id="rId12" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="Y25" r:id="rId13" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y24" r:id="rId14" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="B3" r:id="rId15" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
+    <hyperlink ref="BM23" r:id="rId16" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="BM25" r:id="rId17" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BM26" r:id="rId18" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BM24" r:id="rId19" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new excel changes and helper class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B3F6C6-CB49-4EB5-9DFA-040BDC8A6238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8194B9D0-365F-46AF-A527-E6093D8AE754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="205">
   <si>
     <t>DataSet</t>
   </si>
@@ -394,229 +394,247 @@
     <t>CTAElements</t>
   </si>
   <si>
-    <t>QATESTINGHYDRO</t>
-  </si>
-  <si>
     <t>CTAText</t>
   </si>
   <si>
     <t>CTAurl</t>
   </si>
   <si>
+    <t>Tiletext</t>
+  </si>
+  <si>
+    <t>textbutton</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>CategorySelect</t>
+  </si>
+  <si>
+    <t>productnames</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>VideoURL</t>
+  </si>
+  <si>
+    <t>CardTitle</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Buttontext</t>
+  </si>
+  <si>
+    <t>Buttontype</t>
+  </si>
+  <si>
+    <t>ButtonLinknavigation</t>
+  </si>
+  <si>
+    <t>Categorydisplay</t>
+  </si>
+  <si>
+    <t>No.ofproductsdisplay</t>
+  </si>
+  <si>
+    <t>productcategory</t>
+  </si>
+  <si>
+    <t>Editpagetitle</t>
+  </si>
+  <si>
+    <t>datacontenttype</t>
+  </si>
+  <si>
+    <t>Deletcomponent</t>
+  </si>
+  <si>
+    <t>LOTUSQATITLE</t>
+  </si>
+  <si>
+    <t>LOTUSQABUTTON</t>
+  </si>
+  <si>
+    <t>m-media-card</t>
+  </si>
+  <si>
+    <t>tiles__wrapper</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>W32075,W32410,W32520,1115580,1165700,1071499B</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Copper Brown,32 oz Wide Mouth - Everest Blue,32 oz Wide Mouth - Acai Purple</t>
+  </si>
+  <si>
+    <t>Price: high to low</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/V_58eaD1NII</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVE</t>
+  </si>
+  <si>
+    <t>QATesting</t>
+  </si>
+  <si>
+    <t>#a8d098</t>
+  </si>
+  <si>
+    <t>demo-desktop_3.png</t>
+  </si>
+  <si>
+    <t>QATEST</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Shop,Bottles</t>
+  </si>
+  <si>
+    <t>Bottles</t>
+  </si>
+  <si>
+    <t>Edit Card Tiles</t>
+  </si>
+  <si>
+    <t>hot_card_tiles</t>
+  </si>
+  <si>
+    <t>hot-card-tiles</t>
+  </si>
+  <si>
+    <t>OXO 10-Piece POP Container Set,3-Piece Mixing Bowl Set,Cherry &amp; Olive Pitter</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.oxo.com/</t>
+  </si>
+  <si>
+    <t>#a8d099</t>
+  </si>
+  <si>
+    <t>plp-block</t>
+  </si>
+  <si>
+    <t>c-plp-cms-block</t>
+  </si>
+  <si>
+    <t>Phone.png</t>
+  </si>
+  <si>
+    <t>Edit PLP Block</t>
+  </si>
+  <si>
+    <t>hot_plp_block</t>
+  </si>
+  <si>
+    <t>type-wrapper</t>
+  </si>
+  <si>
+    <t>c-clp-hero</t>
+  </si>
+  <si>
+    <t>Lotusqa.png</t>
+  </si>
+  <si>
+    <t>Edit CLP Hero Banner</t>
+  </si>
+  <si>
+    <t>hot_clp_banner</t>
+  </si>
+  <si>
+    <t>The page is for Testing only.</t>
+  </si>
+  <si>
+    <t>Lotus Testing the CLP Hero banner</t>
+  </si>
+  <si>
+    <t>The page has been deleted.</t>
+  </si>
+  <si>
+    <t>headingtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description Type</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>QALOTUSTEST</t>
+  </si>
+  <si>
+    <t>ProductcardTile</t>
+  </si>
+  <si>
+    <t>OXOproducttile</t>
+  </si>
+  <si>
+    <t>PLPBLOCK</t>
+  </si>
+  <si>
+    <t>Qatest2</t>
+  </si>
+  <si>
+    <t>message_3.png</t>
+  </si>
+  <si>
+    <t>CLPHerobanner</t>
+  </si>
+  <si>
+    <t>OXOCLPHerobanner</t>
+  </si>
+  <si>
+    <t>mkoppanadam@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Acyqadtkonic1!</t>
+  </si>
+  <si>
+    <t>Stacked</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>#343434</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>QA test for the hydrflask and promo content</t>
+  </si>
+  <si>
+    <t>QA Test/Promo Block-Content</t>
+  </si>
+  <si>
+    <t>QAHYDRO</t>
+  </si>
+  <si>
     <t>skatipelli@helenoftroy.com</t>
   </si>
   <si>
     <t>Aoypzjceqraq1!</t>
-  </si>
-  <si>
-    <t>Tiletext</t>
-  </si>
-  <si>
-    <t>textbutton</t>
-  </si>
-  <si>
-    <t>component</t>
-  </si>
-  <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>CategorySelect</t>
-  </si>
-  <si>
-    <t>productnames</t>
-  </si>
-  <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>VideoURL</t>
-  </si>
-  <si>
-    <t>CardTitle</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>Buttontext</t>
-  </si>
-  <si>
-    <t>Buttontype</t>
-  </si>
-  <si>
-    <t>ButtonLinknavigation</t>
-  </si>
-  <si>
-    <t>Categorydisplay</t>
-  </si>
-  <si>
-    <t>No.ofproductsdisplay</t>
-  </si>
-  <si>
-    <t>productcategory</t>
-  </si>
-  <si>
-    <t>Editpagetitle</t>
-  </si>
-  <si>
-    <t>datacontenttype</t>
-  </si>
-  <si>
-    <t>Deletcomponent</t>
-  </si>
-  <si>
-    <t>LOTUSQATITLE</t>
-  </si>
-  <si>
-    <t>LOTUSQABUTTON</t>
-  </si>
-  <si>
-    <t>m-media-card</t>
-  </si>
-  <si>
-    <t>tiles__wrapper</t>
-  </si>
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>W32075,W32410,W32520,1115580,1165700,1071499B</t>
-  </si>
-  <si>
-    <t>32 oz Wide Mouth - Copper Brown,32 oz Wide Mouth - Everest Blue,32 oz Wide Mouth - Acai Purple</t>
-  </si>
-  <si>
-    <t>Price: high to low</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/V_58eaD1NII</t>
-  </si>
-  <si>
-    <t>QATESTINGLOTUSWAVE</t>
-  </si>
-  <si>
-    <t>QATesting</t>
-  </si>
-  <si>
-    <t>#a8d098</t>
-  </si>
-  <si>
-    <t>demo-desktop_3.png</t>
-  </si>
-  <si>
-    <t>QATEST</t>
-  </si>
-  <si>
-    <t>Page</t>
-  </si>
-  <si>
-    <t>Shop,Bottles</t>
-  </si>
-  <si>
-    <t>Bottles</t>
-  </si>
-  <si>
-    <t>Edit Card Tiles</t>
-  </si>
-  <si>
-    <t>hot_card_tiles</t>
-  </si>
-  <si>
-    <t>hot-card-tiles</t>
-  </si>
-  <si>
-    <t>OXO 10-Piece POP Container Set,3-Piece Mixing Bowl Set,Cherry &amp; Olive Pitter</t>
-  </si>
-  <si>
-    <t>https://mcloud-na-stage.oxo.com/</t>
-  </si>
-  <si>
-    <t>#a8d099</t>
-  </si>
-  <si>
-    <t>plp-block</t>
-  </si>
-  <si>
-    <t>c-plp-cms-block</t>
-  </si>
-  <si>
-    <t>Phone.png</t>
-  </si>
-  <si>
-    <t>Edit PLP Block</t>
-  </si>
-  <si>
-    <t>hot_plp_block</t>
-  </si>
-  <si>
-    <t>type-wrapper</t>
-  </si>
-  <si>
-    <t>c-clp-hero</t>
-  </si>
-  <si>
-    <t>Lotusqa.png</t>
-  </si>
-  <si>
-    <t>Edit CLP Hero Banner</t>
-  </si>
-  <si>
-    <t>hot_clp_banner</t>
-  </si>
-  <si>
-    <t>The page is for Testing only.</t>
-  </si>
-  <si>
-    <t>Lotus Testing the CLP Hero banner</t>
-  </si>
-  <si>
-    <t>The page has been deleted.</t>
-  </si>
-  <si>
-    <t>headingtype</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Description Type</t>
-  </si>
-  <si>
-    <t>H6</t>
-  </si>
-  <si>
-    <t>QALOTUSTEST</t>
-  </si>
-  <si>
-    <t>ProductcardTile</t>
-  </si>
-  <si>
-    <t>OXOproducttile</t>
-  </si>
-  <si>
-    <t>PLPBLOCK</t>
-  </si>
-  <si>
-    <t>Qatest2</t>
-  </si>
-  <si>
-    <t>message_3.png</t>
-  </si>
-  <si>
-    <t>CLPHerobanner</t>
-  </si>
-  <si>
-    <t>OXOCLPHerobanner</t>
-  </si>
-  <si>
-    <t>mkoppanadam@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Acyqadtkonic1!</t>
   </si>
 </sst>
 </file>
@@ -989,115 +1007,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BL10" sqref="BL10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7265625" customWidth="1"/>
-    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.453125" customWidth="1"/>
-    <col min="12" max="12" width="49.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="30.7265625" customWidth="1"/>
-    <col min="16" max="16" width="89.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7265625" customWidth="1"/>
-    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.42578125" customWidth="1"/>
+    <col min="12" max="12" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="17.54296875" customWidth="1"/>
-    <col min="29" max="29" width="14.7265625" customWidth="1"/>
+    <col min="25" max="25" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="17.5703125" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" customWidth="1"/>
     <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7265625" customWidth="1"/>
-    <col min="34" max="34" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.7265625" customWidth="1"/>
-    <col min="36" max="36" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="45.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="68.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.7109375" customWidth="1"/>
+    <col min="34" max="34" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" customWidth="1"/>
+    <col min="36" max="36" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="68.5703125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="38" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="11.26953125" customWidth="1"/>
-    <col min="52" max="52" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="11.28515625" customWidth="1"/>
+    <col min="52" max="52" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="8" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.1796875" customWidth="1"/>
-    <col min="58" max="58" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="49.6328125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="161.453125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="146.81640625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.140625" customWidth="1"/>
+    <col min="58" max="58" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="161.42578125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="146.85546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="15" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="12" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="17" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="8" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="14" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="5" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1147,70 +1165,70 @@
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="AH1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="AK1" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AM1" s="3" t="s">
         <v>16</v>
@@ -1309,21 +1327,21 @@
         <v>116</v>
       </c>
       <c r="BS1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BT1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="BT1" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>127</v>
+        <v>203</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>204</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1371,15 +1389,15 @@
       <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1432,7 +1450,7 @@
       <c r="BE3" s="6"/>
       <c r="BF3" s="7"/>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1490,7 +1508,7 @@
       <c r="BE4" s="6"/>
       <c r="BF4" s="7"/>
     </row>
-    <row r="5" spans="1:72" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:72" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1538,7 +1556,7 @@
       <c r="BH5" s="1"/>
       <c r="BI5" s="8"/>
     </row>
-    <row r="6" spans="1:72" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1588,7 +1606,7 @@
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1635,7 +1653,7 @@
       <c r="AQ7" s="4"/>
       <c r="AR7" s="4"/>
     </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1682,7 +1700,7 @@
       <c r="AN8" s="5"/>
       <c r="AO8" s="4"/>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1723,7 +1741,7 @@
       <c r="AN9" s="5"/>
       <c r="AO9" s="4"/>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1748,7 +1766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1770,7 +1788,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1817,7 +1835,7 @@
       <c r="AN12" s="4"/>
       <c r="AO12" s="4"/>
     </row>
-    <row r="13" spans="1:72" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1840,7 +1858,7 @@
       <c r="BH13" s="1"/>
       <c r="BI13" s="8"/>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1899,7 +1917,7 @@
       <c r="AX14" s="11"/>
       <c r="AY14" s="11"/>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -1937,7 +1955,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -1945,7 +1963,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1953,7 +1971,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:67" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1963,7 +1981,7 @@
       </c>
       <c r="BI18" s="8"/>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1977,13 +1995,15 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
-      <c r="Y19" s="4"/>
+      <c r="Y19" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="Z19" s="4"/>
       <c r="AA19" s="15"/>
       <c r="AB19" s="15"/>
@@ -1996,6 +2016,9 @@
       <c r="AI19" s="4"/>
       <c r="AJ19" s="4"/>
       <c r="AM19" s="4"/>
+      <c r="AN19" t="s">
+        <v>200</v>
+      </c>
       <c r="AO19" s="4"/>
       <c r="BH19" s="1"/>
       <c r="BI19" t="s">
@@ -2013,15 +2036,26 @@
       <c r="BM19" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BN19" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="BO19" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="BP19" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>117</v>
       </c>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="Y20" s="4"/>
+      <c r="Y20" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="Z20" s="4"/>
       <c r="AA20" s="15"/>
       <c r="AB20" s="15"/>
@@ -2042,8 +2076,20 @@
       <c r="BM20" s="14" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BN20" t="s">
+        <v>196</v>
+      </c>
+      <c r="BO20" t="s">
+        <v>199</v>
+      </c>
+      <c r="BQ20" t="s">
+        <v>115</v>
+      </c>
+      <c r="BR20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -2080,8 +2126,11 @@
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
-    </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="AN21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -2121,207 +2170,213 @@
       <c r="BD22" s="9"/>
       <c r="BE22" s="9"/>
       <c r="BL22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="BM22" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:67" ht="29" x14ac:dyDescent="0.35">
+      <c r="BS22" t="s">
+        <v>202</v>
+      </c>
+      <c r="BT22" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:72" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="O23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q23" t="s">
+        <v>146</v>
+      </c>
+      <c r="R23" t="s">
+        <v>147</v>
+      </c>
+      <c r="S23" t="s">
+        <v>148</v>
+      </c>
+      <c r="T23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="R23" t="s">
+      <c r="U23" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="S23" t="s">
-        <v>151</v>
-      </c>
-      <c r="T23" s="4" t="s">
+      <c r="V23" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="U23" s="4" t="s">
+      <c r="W23" t="s">
         <v>153</v>
       </c>
-      <c r="V23" s="4" t="s">
+      <c r="X23" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y23" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="W23" t="s">
-        <v>156</v>
-      </c>
-      <c r="X23" t="s">
+      <c r="Z23" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="Y23" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z23" s="4" t="s">
+      <c r="AA23" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB23" s="15" t="s">
         <v>160</v>
-      </c>
-      <c r="AA23" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB23" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="AC23" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AD23" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AE23" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AF23" s="4">
         <v>3</v>
       </c>
       <c r="AG23" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH23" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI23" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AJ23" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="AH23" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="AI23" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AJ23" s="4" t="s">
-        <v>169</v>
       </c>
       <c r="AO23" s="4"/>
       <c r="AR23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BG23" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="BI23" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="BK23" s="6"/>
       <c r="BL23" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BM23" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:67" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:72" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L24" s="4"/>
       <c r="Q24" t="s">
+        <v>146</v>
+      </c>
+      <c r="R24" t="s">
+        <v>147</v>
+      </c>
+      <c r="S24" t="s">
+        <v>148</v>
+      </c>
+      <c r="T24" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="R24" t="s">
+      <c r="U24" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="S24" t="s">
-        <v>151</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="U24" s="4" t="s">
+      <c r="V24" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="W24" t="s">
         <v>153</v>
       </c>
-      <c r="V24" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="W24" t="s">
-        <v>156</v>
-      </c>
       <c r="X24" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y24" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z24" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="Y24" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z24" s="4" t="s">
+      <c r="AA24" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB24" s="15" t="s">
         <v>160</v>
-      </c>
-      <c r="AA24" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB24" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="AC24" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AD24" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AE24" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AF24" s="4">
         <v>3</v>
       </c>
       <c r="AG24" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH24" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AJ24" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="AH24" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="AI24" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AJ24" s="4" t="s">
-        <v>169</v>
       </c>
       <c r="AO24" s="4"/>
       <c r="BI24" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="BK24" s="6"/>
       <c r="BL24" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BM24" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="R25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Z25" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AA25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
@@ -2330,13 +2385,13 @@
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
       <c r="AH25" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AI25" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AJ25" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
@@ -2351,35 +2406,35 @@
       <c r="AU25" s="4"/>
       <c r="AV25" s="4"/>
       <c r="BL25" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BM25" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BN25" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="BO25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="R26" s="4"/>
       <c r="S26" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
@@ -2387,10 +2442,10 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
@@ -2399,22 +2454,22 @@
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AI26" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AJ26" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AK26" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AL26" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AN26" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AO26" s="4"/>
       <c r="AP26" s="4"/>
@@ -2426,31 +2481,31 @@
       <c r="AV26" s="4"/>
       <c r="BK26" s="9"/>
       <c r="BL26" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="BM26" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Q27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AO27" s="4"/>
     </row>
-    <row r="33" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:39" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2499,17 +2554,18 @@
     <hyperlink ref="BM15" r:id="rId8" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
     <hyperlink ref="BM20" r:id="rId9" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
     <hyperlink ref="BM22" r:id="rId10" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="B2" r:id="rId11" xr:uid="{93DFD34B-00AC-4EAF-86FA-A13945460604}"/>
-    <hyperlink ref="Y23" r:id="rId12" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
-    <hyperlink ref="Y25" r:id="rId13" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
-    <hyperlink ref="Y24" r:id="rId14" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
-    <hyperlink ref="B3" r:id="rId15" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="BM23" r:id="rId16" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
-    <hyperlink ref="BM25" r:id="rId17" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BM26" r:id="rId18" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BM24" r:id="rId19" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="Y23" r:id="rId11" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="Y25" r:id="rId12" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y24" r:id="rId13" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
+    <hyperlink ref="BM23" r:id="rId15" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="BM25" r:id="rId16" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BM26" r:id="rId17" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BM24" r:id="rId18" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="Y19" r:id="rId19" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
+    <hyperlink ref="BT22" r:id="rId20" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Normal path Admin Testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8194B9D0-365F-46AF-A527-E6093D8AE754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D04A80-D6FB-4DB0-85FE-A32C683FCD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="208">
   <si>
     <t>DataSet</t>
   </si>
@@ -635,6 +635,15 @@
   </si>
   <si>
     <t>Aoypzjceqraq1!</t>
+  </si>
+  <si>
+    <t>Categorydetails</t>
+  </si>
+  <si>
+    <t>categoryname</t>
+  </si>
+  <si>
+    <t>HYDROFLASK</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BT33"/>
+  <dimension ref="A1:BU33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1124,7 @@
     <col min="110" max="110" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1332,8 +1341,11 @@
       <c r="BT1" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="BU1" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1389,7 +1401,7 @@
       <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1450,7 +1462,7 @@
       <c r="BE3" s="6"/>
       <c r="BF3" s="7"/>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1508,7 +1520,7 @@
       <c r="BE4" s="6"/>
       <c r="BF4" s="7"/>
     </row>
-    <row r="5" spans="1:72" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1556,7 +1568,7 @@
       <c r="BH5" s="1"/>
       <c r="BI5" s="8"/>
     </row>
-    <row r="6" spans="1:72" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1606,7 +1618,7 @@
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1653,7 +1665,7 @@
       <c r="AQ7" s="4"/>
       <c r="AR7" s="4"/>
     </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1700,7 +1712,7 @@
       <c r="AN8" s="5"/>
       <c r="AO8" s="4"/>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1741,7 +1753,7 @@
       <c r="AN9" s="5"/>
       <c r="AO9" s="4"/>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1766,7 +1778,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:72" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:73" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1788,7 +1800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1835,7 +1847,7 @@
       <c r="AN12" s="4"/>
       <c r="AO12" s="4"/>
     </row>
-    <row r="13" spans="1:72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1858,7 +1870,7 @@
       <c r="BH13" s="1"/>
       <c r="BI13" s="8"/>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1917,7 +1929,7 @@
       <c r="AX14" s="11"/>
       <c r="AY14" s="11"/>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -1955,7 +1967,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -1963,7 +1975,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1971,7 +1983,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1981,7 +1993,7 @@
       </c>
       <c r="BI18" s="8"/>
     </row>
-    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2046,7 +2058,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -2089,7 +2101,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -2130,7 +2142,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -2182,7 +2194,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:72" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:73" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -2270,7 +2282,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:72" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:73" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>188</v>
       </c>
@@ -2347,7 +2359,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -2418,7 +2430,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>192</v>
       </c>
@@ -2487,7 +2499,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>193</v>
       </c>
@@ -2504,6 +2516,14 @@
         <v>176</v>
       </c>
       <c r="AO27" s="4"/>
+    </row>
+    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>205</v>
+      </c>
+      <c r="BU28" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="33" spans="3:39" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>

</xml_diff>

<commit_message>
Admin testcase and Storelocater test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D04A80-D6FB-4DB0-85FE-A32C683FCD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDD0029-6737-4F5C-89E9-ADCD3FA5ADB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="217">
   <si>
     <t>DataSet</t>
   </si>
@@ -644,6 +644,33 @@
   </si>
   <si>
     <t>HYDROFLASK</t>
+  </si>
+  <si>
+    <t>mrgtop</t>
+  </si>
+  <si>
+    <t>mrgright</t>
+  </si>
+  <si>
+    <t>mrgbottom</t>
+  </si>
+  <si>
+    <t>mrgleft</t>
+  </si>
+  <si>
+    <t>paddingtop</t>
+  </si>
+  <si>
+    <t>paddingright</t>
+  </si>
+  <si>
+    <t>paddingbottom</t>
+  </si>
+  <si>
+    <t>paddingleft</t>
+  </si>
+  <si>
+    <t>CSSclasses</t>
   </si>
 </sst>
 </file>
@@ -653,7 +680,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,6 +709,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -697,10 +730,36 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD1D1D1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD1D1D1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD1D1D1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD1D1D1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD1D1D1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD1D1D1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -710,7 +769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -732,6 +791,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1014,117 +1079,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BU33"/>
+  <dimension ref="A1:CD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="BU1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CE6" sqref="CE6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.42578125" customWidth="1"/>
-    <col min="12" max="12" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7265625" customWidth="1"/>
+    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.453125" customWidth="1"/>
+    <col min="12" max="12" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7265625" customWidth="1"/>
+    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7265625" customWidth="1"/>
+    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="17.5703125" customWidth="1"/>
-    <col min="29" max="29" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="17.54296875" customWidth="1"/>
+    <col min="29" max="29" width="14.7265625" customWidth="1"/>
     <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7109375" customWidth="1"/>
-    <col min="34" max="34" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" customWidth="1"/>
-    <col min="36" max="36" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.7265625" customWidth="1"/>
+    <col min="34" max="34" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.7265625" customWidth="1"/>
+    <col min="36" max="36" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="68.54296875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="38" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="11.28515625" customWidth="1"/>
-    <col min="52" max="52" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="11.26953125" customWidth="1"/>
+    <col min="52" max="52" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="8" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.140625" customWidth="1"/>
-    <col min="58" max="58" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="161.42578125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="146.85546875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.1796875" customWidth="1"/>
+    <col min="58" max="58" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="14.54296875" customWidth="1"/>
+    <col min="74" max="74" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="146.81640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="15" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="12" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="17" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="8" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="14" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="5" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1344,8 +1409,35 @@
       <c r="BU1" s="3" t="s">
         <v>206</v>
       </c>
+      <c r="BV1" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="BW1" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="BX1" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="BY1" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="BZ1" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="CA1" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="CB1" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="CC1" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="CD1" s="17" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1401,7 +1493,7 @@
       <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1462,7 +1554,7 @@
       <c r="BE3" s="6"/>
       <c r="BF3" s="7"/>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1520,7 +1612,7 @@
       <c r="BE4" s="6"/>
       <c r="BF4" s="7"/>
     </row>
-    <row r="5" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1568,7 +1660,7 @@
       <c r="BH5" s="1"/>
       <c r="BI5" s="8"/>
     </row>
-    <row r="6" spans="1:73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1618,7 +1710,7 @@
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1665,7 +1757,7 @@
       <c r="AQ7" s="4"/>
       <c r="AR7" s="4"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1712,7 +1804,7 @@
       <c r="AN8" s="5"/>
       <c r="AO8" s="4"/>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1753,7 +1845,7 @@
       <c r="AN9" s="5"/>
       <c r="AO9" s="4"/>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1778,7 +1870,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:73" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1800,7 +1892,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1847,7 +1939,7 @@
       <c r="AN12" s="4"/>
       <c r="AO12" s="4"/>
     </row>
-    <row r="13" spans="1:73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1870,7 +1962,7 @@
       <c r="BH13" s="1"/>
       <c r="BI13" s="8"/>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1929,7 +2021,7 @@
       <c r="AX14" s="11"/>
       <c r="AY14" s="11"/>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -1967,7 +2059,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -1975,7 +2067,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1983,7 +2075,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1993,7 +2085,7 @@
       </c>
       <c r="BI18" s="8"/>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2057,8 +2149,35 @@
       <c r="BP19" s="5" t="s">
         <v>198</v>
       </c>
+      <c r="BV19">
+        <v>40</v>
+      </c>
+      <c r="BW19">
+        <v>27</v>
+      </c>
+      <c r="BX19">
+        <v>55</v>
+      </c>
+      <c r="BY19">
+        <v>48</v>
+      </c>
+      <c r="BZ19">
+        <v>100</v>
+      </c>
+      <c r="CA19">
+        <v>278</v>
+      </c>
+      <c r="CB19">
+        <v>300</v>
+      </c>
+      <c r="CC19">
+        <v>129</v>
+      </c>
+      <c r="CD19" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -2101,7 +2220,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -2142,7 +2261,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -2194,7 +2313,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:73" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:82" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -2281,8 +2400,35 @@
       <c r="BM23" s="4" t="s">
         <v>103</v>
       </c>
+      <c r="BV23">
+        <v>40</v>
+      </c>
+      <c r="BW23">
+        <v>27</v>
+      </c>
+      <c r="BX23">
+        <v>55</v>
+      </c>
+      <c r="BY23">
+        <v>48</v>
+      </c>
+      <c r="BZ23">
+        <v>100</v>
+      </c>
+      <c r="CA23">
+        <v>278</v>
+      </c>
+      <c r="CB23">
+        <v>300</v>
+      </c>
+      <c r="CC23">
+        <v>129</v>
+      </c>
+      <c r="CD23" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="24" spans="1:73" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:82" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>188</v>
       </c>
@@ -2358,8 +2504,35 @@
       <c r="BM24" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="BV24">
+        <v>40</v>
+      </c>
+      <c r="BW24">
+        <v>27</v>
+      </c>
+      <c r="BX24">
+        <v>55</v>
+      </c>
+      <c r="BY24">
+        <v>48</v>
+      </c>
+      <c r="BZ24">
+        <v>100</v>
+      </c>
+      <c r="CA24">
+        <v>278</v>
+      </c>
+      <c r="CB24">
+        <v>300</v>
+      </c>
+      <c r="CC24">
+        <v>129</v>
+      </c>
+      <c r="CD24" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -2429,8 +2602,35 @@
       <c r="BO25" t="s">
         <v>191</v>
       </c>
+      <c r="BV25">
+        <v>40</v>
+      </c>
+      <c r="BW25">
+        <v>27</v>
+      </c>
+      <c r="BX25">
+        <v>55</v>
+      </c>
+      <c r="BY25">
+        <v>48</v>
+      </c>
+      <c r="BZ25">
+        <v>100</v>
+      </c>
+      <c r="CA25">
+        <v>278</v>
+      </c>
+      <c r="CB25">
+        <v>300</v>
+      </c>
+      <c r="CC25">
+        <v>129</v>
+      </c>
+      <c r="CD25" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>192</v>
       </c>
@@ -2498,8 +2698,35 @@
       <c r="BM26" s="4" t="s">
         <v>103</v>
       </c>
+      <c r="BV26">
+        <v>40</v>
+      </c>
+      <c r="BW26">
+        <v>27</v>
+      </c>
+      <c r="BX26">
+        <v>55</v>
+      </c>
+      <c r="BY26">
+        <v>48</v>
+      </c>
+      <c r="BZ26">
+        <v>100</v>
+      </c>
+      <c r="CA26">
+        <v>278</v>
+      </c>
+      <c r="CB26">
+        <v>300</v>
+      </c>
+      <c r="CC26">
+        <v>129</v>
+      </c>
+      <c r="CD26" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>193</v>
       </c>
@@ -2516,16 +2743,70 @@
         <v>176</v>
       </c>
       <c r="AO27" s="4"/>
+      <c r="BV27">
+        <v>40</v>
+      </c>
+      <c r="BW27">
+        <v>27</v>
+      </c>
+      <c r="BX27">
+        <v>55</v>
+      </c>
+      <c r="BY27">
+        <v>48</v>
+      </c>
+      <c r="BZ27">
+        <v>100</v>
+      </c>
+      <c r="CA27">
+        <v>278</v>
+      </c>
+      <c r="CB27">
+        <v>300</v>
+      </c>
+      <c r="CC27">
+        <v>129</v>
+      </c>
+      <c r="CD27" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>205</v>
       </c>
       <c r="BU28" t="s">
         <v>207</v>
       </c>
+      <c r="BV28">
+        <v>40</v>
+      </c>
+      <c r="BW28">
+        <v>27</v>
+      </c>
+      <c r="BX28">
+        <v>55</v>
+      </c>
+      <c r="BY28">
+        <v>48</v>
+      </c>
+      <c r="BZ28">
+        <v>100</v>
+      </c>
+      <c r="CA28">
+        <v>278</v>
+      </c>
+      <c r="CB28">
+        <v>300</v>
+      </c>
+      <c r="CC28">
+        <v>129</v>
+      </c>
+      <c r="CD28" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="33" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:39" x14ac:dyDescent="0.35">
       <c r="C33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>

</xml_diff>

<commit_message>
AdminValue prop bannert testcase No. - 77  commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDD0029-6737-4F5C-89E9-ADCD3FA5ADB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0211866-37E2-49F9-918A-718855525778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="220">
   <si>
     <t>DataSet</t>
   </si>
@@ -382,9 +382,6 @@
     <t>W32075</t>
   </si>
   <si>
-    <t>qaFlask</t>
-  </si>
-  <si>
     <t>EditContentSection</t>
   </si>
   <si>
@@ -631,12 +628,6 @@
     <t>QAHYDRO</t>
   </si>
   <si>
-    <t>skatipelli@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Aoypzjceqraq1!</t>
-  </si>
-  <si>
     <t>Categorydetails</t>
   </si>
   <si>
@@ -671,6 +662,24 @@
   </si>
   <si>
     <t>CSSclasses</t>
+  </si>
+  <si>
+    <t>Valuepropbanner</t>
+  </si>
+  <si>
+    <t>Cat_1.png</t>
+  </si>
+  <si>
+    <t>valuepropcard2</t>
+  </si>
+  <si>
+    <t>valuepropcard3</t>
+  </si>
+  <si>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>testing2</t>
   </si>
 </sst>
 </file>
@@ -680,7 +689,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,6 +723,12 @@
       <color rgb="FF242424"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1081,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CE6" sqref="CE6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,70 +1254,70 @@
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AJ1" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="AK1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL1" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="AM1" s="3" t="s">
         <v>16</v>
@@ -1401,40 +1416,40 @@
         <v>116</v>
       </c>
       <c r="BS1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="BT1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="BT1" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="BU1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV1" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="BW1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="BV1" s="16" t="s">
+      <c r="BX1" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="BY1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="BW1" s="16" t="s">
+      <c r="BZ1" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="BX1" s="16" t="s">
+      <c r="CA1" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="BY1" s="16" t="s">
+      <c r="CB1" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="BZ1" s="16" t="s">
+      <c r="CC1" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="CA1" s="16" t="s">
+      <c r="CD1" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="CB1" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="CC1" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="CD1" s="17" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:82" x14ac:dyDescent="0.35">
@@ -1442,10 +1457,10 @@
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1498,10 +1513,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -2074,6 +2089,9 @@
       <c r="BG17" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="BL17" s="4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="18" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -2084,6 +2102,9 @@
         <v>98</v>
       </c>
       <c r="BI18" s="8"/>
+      <c r="BL18" s="4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="19" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -2099,14 +2120,14 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="Y19" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z19" s="4"/>
       <c r="AA19" s="15"/>
@@ -2121,7 +2142,7 @@
       <c r="AJ19" s="4"/>
       <c r="AM19" s="4"/>
       <c r="AN19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO19" s="4"/>
       <c r="BH19" s="1"/>
@@ -2134,44 +2155,44 @@
       <c r="BK19" t="s">
         <v>102</v>
       </c>
-      <c r="BL19" t="s">
-        <v>120</v>
+      <c r="BL19" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="BM19" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BN19" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="BO19" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="BO19" s="5" t="s">
+      <c r="BP19" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="BP19" s="5" t="s">
-        <v>198</v>
-      </c>
       <c r="BV19">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="BW19">
         <v>27</v>
       </c>
       <c r="BX19">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="BY19">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="BZ19">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="CA19">
-        <v>278</v>
+        <v>35</v>
       </c>
       <c r="CB19">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="CC19">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="CD19" t="s">
         <v>77</v>
@@ -2204,25 +2225,52 @@
       <c r="BG20" s="9" t="s">
         <v>119</v>
       </c>
+      <c r="BL20" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="BM20" s="14" t="s">
         <v>118</v>
       </c>
       <c r="BN20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BO20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BQ20" t="s">
         <v>115</v>
       </c>
       <c r="BR20" t="s">
         <v>39</v>
+      </c>
+      <c r="BV20">
+        <v>25</v>
+      </c>
+      <c r="BW20">
+        <v>27</v>
+      </c>
+      <c r="BX20">
+        <v>15</v>
+      </c>
+      <c r="BY20">
+        <v>10</v>
+      </c>
+      <c r="BZ20">
+        <v>30</v>
+      </c>
+      <c r="CA20">
+        <v>35</v>
+      </c>
+      <c r="CB20">
+        <v>32</v>
+      </c>
+      <c r="CC20">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2231,7 +2279,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2258,12 +2306,39 @@
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
       <c r="AN21" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="BL21" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BV21">
+        <v>25</v>
+      </c>
+      <c r="BW21">
+        <v>27</v>
+      </c>
+      <c r="BX21">
+        <v>15</v>
+      </c>
+      <c r="BY21">
+        <v>10</v>
+      </c>
+      <c r="BZ21">
+        <v>30</v>
+      </c>
+      <c r="CA21">
+        <v>35</v>
+      </c>
+      <c r="CB21">
+        <v>32</v>
+      </c>
+      <c r="CC21">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2300,129 +2375,153 @@
       <c r="AM22" s="4"/>
       <c r="BD22" s="9"/>
       <c r="BE22" s="9"/>
-      <c r="BL22" t="s">
-        <v>120</v>
+      <c r="BL22" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="BM22" s="14" t="s">
         <v>103</v>
       </c>
       <c r="BS22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BT22" s="14" t="s">
         <v>118</v>
+      </c>
+      <c r="BV22">
+        <v>25</v>
+      </c>
+      <c r="BW22">
+        <v>27</v>
+      </c>
+      <c r="BX22">
+        <v>15</v>
+      </c>
+      <c r="BY22">
+        <v>10</v>
+      </c>
+      <c r="BZ22">
+        <v>30</v>
+      </c>
+      <c r="CA22">
+        <v>35</v>
+      </c>
+      <c r="CB22">
+        <v>32</v>
+      </c>
+      <c r="CC22">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:82" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q23" t="s">
+        <v>145</v>
+      </c>
+      <c r="R23" t="s">
         <v>146</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>147</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="U23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="U23" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="V23" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="W23" t="s">
         <v>152</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>153</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Y23" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="Z23" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA23" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB23" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="AB23" s="15" t="s">
-        <v>160</v>
       </c>
       <c r="AC23" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AD23" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE23" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="AE23" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="AF23" s="4">
         <v>3</v>
       </c>
       <c r="AG23" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH23" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AH23" s="4" t="s">
+      <c r="AI23" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="AI23" s="4" t="s">
+      <c r="AJ23" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="AJ23" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="AO23" s="4"/>
       <c r="AR23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BG23" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BI23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BK23" s="6"/>
       <c r="BL23" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BM23" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BV23">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="BW23">
         <v>27</v>
       </c>
       <c r="BX23">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="BY23">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="BZ23">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="CA23">
-        <v>278</v>
+        <v>35</v>
       </c>
       <c r="CB23">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="CC23">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="CD23" t="s">
         <v>77</v>
@@ -2430,103 +2529,103 @@
     </row>
     <row r="24" spans="1:82" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L24" s="4"/>
       <c r="Q24" t="s">
+        <v>145</v>
+      </c>
+      <c r="R24" t="s">
         <v>146</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>147</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="U24" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="U24" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="V24" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W24" t="s">
+        <v>152</v>
+      </c>
+      <c r="X24" t="s">
         <v>153</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Y24" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="Z24" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA24" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB24" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="AB24" s="15" t="s">
-        <v>160</v>
       </c>
       <c r="AC24" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AD24" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE24" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="AE24" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="AF24" s="4">
         <v>3</v>
       </c>
       <c r="AG24" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH24" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AH24" s="4" t="s">
+      <c r="AI24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="AI24" s="4" t="s">
+      <c r="AJ24" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="AJ24" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="AO24" s="4"/>
       <c r="BI24" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BK24" s="6"/>
       <c r="BL24" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BM24" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="BV24">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="BW24">
         <v>27</v>
       </c>
       <c r="BX24">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="BY24">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="BZ24">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="CA24">
-        <v>278</v>
+        <v>35</v>
       </c>
       <c r="CB24">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="CC24">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="CD24" t="s">
         <v>77</v>
@@ -2534,34 +2633,34 @@
     </row>
     <row r="25" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" t="s">
+        <v>145</v>
+      </c>
+      <c r="R25" t="s">
         <v>146</v>
       </c>
-      <c r="R25" t="s">
-        <v>147</v>
-      </c>
       <c r="S25" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="T25" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="T25" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z25" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
@@ -2570,13 +2669,13 @@
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
       <c r="AH25" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AI25" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="AI25" s="4" t="s">
+      <c r="AJ25" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="AJ25" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
@@ -2591,40 +2690,40 @@
       <c r="AU25" s="4"/>
       <c r="AV25" s="4"/>
       <c r="BL25" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BM25" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BN25" t="s">
+        <v>189</v>
+      </c>
+      <c r="BO25" t="s">
         <v>190</v>
       </c>
-      <c r="BO25" t="s">
-        <v>191</v>
-      </c>
       <c r="BV25">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="BW25">
         <v>27</v>
       </c>
       <c r="BX25">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="BY25">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="BZ25">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="CA25">
-        <v>278</v>
+        <v>35</v>
       </c>
       <c r="CB25">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="CC25">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="CD25" t="s">
         <v>77</v>
@@ -2632,21 +2731,21 @@
     </row>
     <row r="26" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R26" s="4"/>
       <c r="S26" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
@@ -2654,10 +2753,10 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
@@ -2666,22 +2765,22 @@
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="AI26" s="4" t="s">
-        <v>179</v>
-      </c>
       <c r="AJ26" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AN26" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="AL26" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AN26" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="AO26" s="4"/>
       <c r="AP26" s="4"/>
@@ -2693,34 +2792,34 @@
       <c r="AV26" s="4"/>
       <c r="BK26" s="9"/>
       <c r="BL26" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BM26" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BV26">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="BW26">
         <v>27</v>
       </c>
       <c r="BX26">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="BY26">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="BZ26">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="CA26">
-        <v>278</v>
+        <v>35</v>
       </c>
       <c r="CB26">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="CC26">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="CD26" t="s">
         <v>77</v>
@@ -2728,44 +2827,50 @@
     </row>
     <row r="27" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO27" s="4"/>
+      <c r="BL27" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM27" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="BV27">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="BW27">
         <v>27</v>
       </c>
       <c r="BX27">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="BY27">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="BZ27">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="CA27">
-        <v>278</v>
+        <v>35</v>
       </c>
       <c r="CB27">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="CC27">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="CD27" t="s">
         <v>77</v>
@@ -2773,37 +2878,160 @@
     </row>
     <row r="28" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>205</v>
+        <v>202</v>
+      </c>
+      <c r="BL28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM28" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="BU28" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="BV28">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="BW28">
         <v>27</v>
       </c>
       <c r="BX28">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="BY28">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="BZ28">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="CA28">
-        <v>278</v>
+        <v>35</v>
       </c>
       <c r="CB28">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="CC28">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="CD28" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>215</v>
+      </c>
+      <c r="BL29" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BV29">
+        <v>25</v>
+      </c>
+      <c r="BW29">
+        <v>27</v>
+      </c>
+      <c r="BX29">
+        <v>15</v>
+      </c>
+      <c r="BY29">
+        <v>10</v>
+      </c>
+      <c r="BZ29">
+        <v>30</v>
+      </c>
+      <c r="CA29">
+        <v>35</v>
+      </c>
+      <c r="CB29">
+        <v>32</v>
+      </c>
+      <c r="CC29">
+        <v>23</v>
+      </c>
+      <c r="CD29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>216</v>
+      </c>
+      <c r="BL30" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM30" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="BV30">
+        <v>12</v>
+      </c>
+      <c r="BW30">
+        <v>32</v>
+      </c>
+      <c r="BX30">
+        <v>22</v>
+      </c>
+      <c r="BY30">
+        <v>12</v>
+      </c>
+      <c r="BZ30">
+        <v>23</v>
+      </c>
+      <c r="CA30">
+        <v>20</v>
+      </c>
+      <c r="CB30">
+        <v>32</v>
+      </c>
+      <c r="CC30">
+        <v>21</v>
+      </c>
+      <c r="CD30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>217</v>
+      </c>
+      <c r="BL31" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM31" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BV31">
+        <v>32</v>
+      </c>
+      <c r="BW31">
+        <v>34</v>
+      </c>
+      <c r="BX31">
+        <v>54</v>
+      </c>
+      <c r="BY31">
+        <v>21</v>
+      </c>
+      <c r="BZ31">
+        <v>13</v>
+      </c>
+      <c r="CA31">
+        <v>5</v>
+      </c>
+      <c r="CB31">
+        <v>2</v>
+      </c>
+      <c r="CC31">
+        <v>12</v>
+      </c>
+      <c r="CD31" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="3:39" x14ac:dyDescent="0.35">
@@ -2844,6 +3072,7 @@
       <c r="AM33" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="F6" r:id="rId2" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
@@ -2865,8 +3094,12 @@
     <hyperlink ref="BM24" r:id="rId18" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
     <hyperlink ref="Y19" r:id="rId19" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
     <hyperlink ref="BT22" r:id="rId20" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="BM27:BM29" r:id="rId21" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="BM28:BM31" r:id="rId22" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="BM30" r:id="rId23" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="B2" r:id="rId24" xr:uid="{8FDC4EB0-4941-4FED-A3AE-F3040B45FB19}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
testimonials product car components and promo block components title
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0211866-37E2-49F9-918A-718855525778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DCB42C-627C-45A6-B742-6AF308818951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="238">
   <si>
     <t>DataSet</t>
   </si>
@@ -680,6 +680,60 @@
   </si>
   <si>
     <t>testing2</t>
+  </si>
+  <si>
+    <t>Author one</t>
+  </si>
+  <si>
+    <t>Author Two</t>
+  </si>
+  <si>
+    <t>Author Three</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>4 Stars</t>
+  </si>
+  <si>
+    <t>The product quality is too good</t>
+  </si>
+  <si>
+    <t>Lotusqa</t>
+  </si>
+  <si>
+    <t>5 Stars</t>
+  </si>
+  <si>
+    <t>Very reasonable Product</t>
+  </si>
+  <si>
+    <t>Lotuswave</t>
+  </si>
+  <si>
+    <t>1 Star</t>
+  </si>
+  <si>
+    <t>Product price is too High</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>qaFlask</t>
   </si>
 </sst>
 </file>
@@ -1094,117 +1148,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD33"/>
+  <dimension ref="A1:CG34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7265625" customWidth="1"/>
-    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.453125" customWidth="1"/>
-    <col min="12" max="12" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="30.7265625" customWidth="1"/>
-    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7265625" customWidth="1"/>
-    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.42578125" customWidth="1"/>
+    <col min="12" max="12" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="17.54296875" customWidth="1"/>
-    <col min="29" max="29" width="14.7265625" customWidth="1"/>
-    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7265625" customWidth="1"/>
-    <col min="34" max="34" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.7265625" customWidth="1"/>
-    <col min="36" max="36" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="45.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="68.54296875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="38" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="11.26953125" customWidth="1"/>
-    <col min="52" max="52" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.1796875" customWidth="1"/>
-    <col min="58" max="58" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="49.54296875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="14.54296875" customWidth="1"/>
-    <col min="74" max="74" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="146.81640625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="15" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="12" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="17" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="8" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="14" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="5" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="17.5703125" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.7109375" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.7109375" customWidth="1"/>
+    <col min="39" max="39" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="38" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="11.28515625" customWidth="1"/>
+    <col min="55" max="55" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.140625" customWidth="1"/>
+    <col min="61" max="61" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.5703125" customWidth="1"/>
+    <col min="77" max="77" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="146.85546875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="15" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="12" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="17" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="8" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="14" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="5" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:85" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1284,175 +1341,184 @@
         <v>134</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="BV1" s="16" t="s">
+      <c r="BY1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="BW1" s="16" t="s">
+      <c r="BZ1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="BX1" s="16" t="s">
+      <c r="CA1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="BY1" s="16" t="s">
+      <c r="CB1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="BZ1" s="16" t="s">
+      <c r="CC1" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="CA1" s="16" t="s">
+      <c r="CD1" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="CB1" s="16" t="s">
+      <c r="CE1" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="CC1" s="16" t="s">
+      <c r="CF1" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="CD1" s="17" t="s">
+      <c r="CG1" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1496,19 +1562,22 @@
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
       <c r="AM2" s="4"/>
-      <c r="AN2" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="AN2" s="4"/>
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
+      <c r="AQ2" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="AR2" s="4"/>
       <c r="AS2" s="4"/>
       <c r="AT2" s="4"/>
       <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
-    </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
+    </row>
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1552,24 +1621,27 @@
       <c r="AK3" s="4"/>
       <c r="AL3" s="4"/>
       <c r="AM3" s="4"/>
-      <c r="AN3" s="5" t="s">
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AO3" s="5" t="s">
+      <c r="AR3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="4"/>
-      <c r="AR3" s="4"/>
       <c r="AS3" s="4"/>
       <c r="AT3" s="4"/>
       <c r="AU3" s="4"/>
       <c r="AV3" s="4"/>
-      <c r="BD3" s="6"/>
-      <c r="BE3" s="6"/>
-      <c r="BF3" s="7"/>
-    </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="AW3" s="4"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="BG3" s="6"/>
+      <c r="BH3" s="6"/>
+      <c r="BI3" s="7"/>
+    </row>
+    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1614,20 +1686,23 @@
       <c r="AH4" s="4"/>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="4"/>
-      <c r="AN4" s="5"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AQ4" s="5"/>
       <c r="AR4" s="4"/>
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4"/>
       <c r="AV4" s="4"/>
-      <c r="BD4" s="6"/>
-      <c r="BE4" s="6"/>
-      <c r="BF4" s="7"/>
-    </row>
-    <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AW4" s="4"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
+      <c r="BG4" s="6"/>
+      <c r="BH4" s="6"/>
+      <c r="BI4" s="7"/>
+    </row>
+    <row r="5" spans="1:85" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1672,10 +1747,13 @@
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="4"/>
-      <c r="BH5" s="1"/>
-      <c r="BI5" s="8"/>
-    </row>
-    <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="8"/>
+    </row>
+    <row r="6" spans="1:85" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1715,17 +1793,20 @@
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
-      <c r="AP6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
       <c r="AQ6" s="4"/>
       <c r="AR6" s="4"/>
       <c r="AS6" s="4"/>
       <c r="AT6" s="4"/>
       <c r="AU6" s="4"/>
       <c r="AV6" s="4"/>
-    </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="AW6" s="4"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+    </row>
+    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1764,15 +1845,18 @@
       <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
       <c r="AM7" s="4"/>
-      <c r="AN7" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
-      <c r="AQ7" s="4"/>
+      <c r="AQ7" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="AR7" s="4"/>
-    </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="AS7" s="4"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+    </row>
+    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1811,15 +1895,18 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="5"/>
-      <c r="AM8" s="5" t="s">
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AN8" s="5"/>
-      <c r="AO8" s="4"/>
-    </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="4"/>
+    </row>
+    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1854,13 +1941,16 @@
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
       <c r="AJ9" s="4"/>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="5"/>
-      <c r="AM9" s="5"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
       <c r="AN9" s="5"/>
-      <c r="AO9" s="4"/>
-    </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="5"/>
+      <c r="AR9" s="4"/>
+    </row>
+    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1876,16 +1966,16 @@
       <c r="O10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="5" t="s">
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AQ10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1898,16 +1988,16 @@
       <c r="O11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AK11" s="5"/>
-      <c r="AL11" s="5"/>
-      <c r="AM11" s="5" t="s">
+      <c r="AN11" s="5"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AN11" s="2" t="s">
+      <c r="AQ11" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1946,15 +2036,18 @@
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
       <c r="AJ12" s="4"/>
-      <c r="AK12" s="5"/>
-      <c r="AL12" s="5"/>
-      <c r="AM12" s="5" t="s">
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AN12" s="4"/>
-      <c r="AO12" s="4"/>
-    </row>
-    <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="4"/>
+    </row>
+    <row r="13" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1974,10 +2067,10 @@
       <c r="L13" t="s">
         <v>75</v>
       </c>
-      <c r="BH13" s="1"/>
-      <c r="BI13" s="8"/>
-    </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="BK13" s="1"/>
+      <c r="BL13" s="8"/>
+    </row>
+    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2009,104 +2102,107 @@
       <c r="AH14" s="4"/>
       <c r="AI14" s="4"/>
       <c r="AJ14" s="4"/>
-      <c r="AP14" s="5" t="s">
+      <c r="AK14" s="4"/>
+      <c r="AL14" s="4"/>
+      <c r="AM14" s="4"/>
+      <c r="AS14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AQ14" s="5" t="s">
+      <c r="AT14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AR14" s="11" t="s">
+      <c r="AU14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="AS14" s="12" t="s">
+      <c r="AV14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="AT14" s="12" t="s">
+      <c r="AW14" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AU14" s="12" t="s">
+      <c r="AX14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AV14" s="12" t="s">
+      <c r="AY14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AW14" s="11" t="s">
+      <c r="AZ14" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AX14" s="11"/>
-      <c r="AY14" s="11"/>
-    </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="BA14" s="11"/>
+      <c r="BB14" s="11"/>
+    </row>
+    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
       <c r="I15" t="s">
         <v>72</v>
       </c>
-      <c r="AS15" s="12" t="s">
+      <c r="AV15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AX15" t="s">
+      <c r="BA15" t="s">
         <v>109</v>
       </c>
-      <c r="AY15" t="s">
+      <c r="BB15" t="s">
         <v>110</v>
       </c>
-      <c r="AZ15" s="5" t="s">
+      <c r="BC15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="BA15" s="5" t="s">
+      <c r="BD15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="BB15" s="9" t="s">
+      <c r="BE15" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BC15" s="13" t="s">
+      <c r="BF15" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="BD15" s="12" t="s">
+      <c r="BG15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="BE15" s="12" t="s">
+      <c r="BH15" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="BM15" s="4" t="s">
+      <c r="BP15" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="BF16" s="9" t="s">
+      <c r="BI16" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="BG17" s="9" t="s">
+      <c r="BJ17" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="BL17" s="4" t="s">
+      <c r="BO17" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="BH18" t="s">
+      <c r="BK18" t="s">
         <v>98</v>
       </c>
-      <c r="BI18" s="8"/>
-      <c r="BL18" s="4" t="s">
+      <c r="BL18" s="8"/>
+      <c r="BO18" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2130,75 +2226,78 @@
         <v>154</v>
       </c>
       <c r="Z19" s="4"/>
-      <c r="AA19" s="15"/>
-      <c r="AB19" s="15"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
-      <c r="AE19" s="4"/>
+      <c r="AE19" s="15"/>
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
       <c r="AH19" s="4"/>
       <c r="AI19" s="4"/>
       <c r="AJ19" s="4"/>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="4"/>
       <c r="AM19" s="4"/>
-      <c r="AN19" t="s">
+      <c r="AP19" s="4"/>
+      <c r="AQ19" t="s">
         <v>199</v>
       </c>
-      <c r="AO19" s="4"/>
-      <c r="BH19" s="1"/>
-      <c r="BI19" t="s">
+      <c r="AR19" s="4"/>
+      <c r="BK19" s="1"/>
+      <c r="BL19" t="s">
         <v>100</v>
       </c>
-      <c r="BJ19" t="s">
+      <c r="BM19" t="s">
         <v>101</v>
       </c>
-      <c r="BK19" t="s">
+      <c r="BN19" t="s">
         <v>102</v>
       </c>
-      <c r="BL19" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BM19" s="4" t="s">
+      <c r="BO19" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BP19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BN19" s="5" t="s">
+      <c r="BQ19" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="BO19" s="5" t="s">
+      <c r="BR19" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="BP19" s="5" t="s">
+      <c r="BS19" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="BV19">
+      <c r="BY19">
         <v>25</v>
       </c>
-      <c r="BW19">
+      <c r="BZ19">
         <v>27</v>
       </c>
-      <c r="BX19">
+      <c r="CA19">
         <v>15</v>
       </c>
-      <c r="BY19">
+      <c r="CB19">
         <v>10</v>
       </c>
-      <c r="BZ19">
+      <c r="CC19">
         <v>30</v>
       </c>
-      <c r="CA19">
+      <c r="CD19">
         <v>35</v>
       </c>
-      <c r="CB19">
+      <c r="CE19">
         <v>32</v>
       </c>
-      <c r="CC19">
+      <c r="CF19">
         <v>23</v>
       </c>
-      <c r="CD19" t="s">
+      <c r="CG19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -2209,66 +2308,69 @@
         <v>39</v>
       </c>
       <c r="Z20" s="4"/>
-      <c r="AA20" s="15"/>
-      <c r="AB20" s="15"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
-      <c r="AD20" s="4"/>
-      <c r="AE20" s="4"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="15"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
       <c r="AH20" s="4"/>
       <c r="AI20" s="4"/>
       <c r="AJ20" s="4"/>
-      <c r="BD20" s="6"/>
-      <c r="BE20" s="6"/>
-      <c r="BF20" s="7"/>
-      <c r="BG20" s="9" t="s">
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4"/>
+      <c r="BG20" s="6"/>
+      <c r="BH20" s="6"/>
+      <c r="BI20" s="7"/>
+      <c r="BJ20" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="BL20" s="4" t="s">
+      <c r="BO20" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM20" s="14" t="s">
+      <c r="BP20" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="BN20" t="s">
+      <c r="BQ20" t="s">
         <v>195</v>
       </c>
-      <c r="BO20" t="s">
+      <c r="BR20" t="s">
         <v>198</v>
       </c>
-      <c r="BQ20" t="s">
+      <c r="BT20" t="s">
         <v>115</v>
       </c>
-      <c r="BR20" t="s">
+      <c r="BU20" t="s">
         <v>39</v>
       </c>
-      <c r="BV20">
+      <c r="BY20">
         <v>25</v>
       </c>
-      <c r="BW20">
+      <c r="BZ20">
         <v>27</v>
       </c>
-      <c r="BX20">
+      <c r="CA20">
         <v>15</v>
       </c>
-      <c r="BY20">
+      <c r="CB20">
         <v>10</v>
       </c>
-      <c r="BZ20">
+      <c r="CC20">
         <v>30</v>
       </c>
-      <c r="CA20">
+      <c r="CD20">
         <v>35</v>
       </c>
-      <c r="CB20">
+      <c r="CE20">
         <v>32</v>
       </c>
-      <c r="CC20">
+      <c r="CF20">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -2293,9 +2395,9 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
@@ -2305,38 +2407,41 @@
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
-      <c r="AN21" t="s">
+      <c r="AN21" s="4"/>
+      <c r="AO21" s="4"/>
+      <c r="AP21" s="4"/>
+      <c r="AQ21" t="s">
         <v>200</v>
       </c>
-      <c r="BL21" s="4" t="s">
+      <c r="BO21" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BV21">
+      <c r="BY21">
         <v>25</v>
       </c>
-      <c r="BW21">
+      <c r="BZ21">
         <v>27</v>
       </c>
-      <c r="BX21">
+      <c r="CA21">
         <v>15</v>
       </c>
-      <c r="BY21">
+      <c r="CB21">
         <v>10</v>
       </c>
-      <c r="BZ21">
+      <c r="CC21">
         <v>30</v>
       </c>
-      <c r="CA21">
+      <c r="CD21">
         <v>35</v>
       </c>
-      <c r="CB21">
+      <c r="CE21">
         <v>32</v>
       </c>
-      <c r="CC21">
+      <c r="CF21">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -2373,46 +2478,49 @@
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
       <c r="AM22" s="4"/>
-      <c r="BD22" s="9"/>
-      <c r="BE22" s="9"/>
-      <c r="BL22" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BM22" s="14" t="s">
+      <c r="AN22" s="4"/>
+      <c r="AO22" s="4"/>
+      <c r="AP22" s="4"/>
+      <c r="BG22" s="9"/>
+      <c r="BH22" s="9"/>
+      <c r="BO22" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BP22" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="BS22" t="s">
+      <c r="BV22" t="s">
         <v>201</v>
       </c>
-      <c r="BT22" s="14" t="s">
+      <c r="BW22" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="BV22">
+      <c r="BY22">
         <v>25</v>
       </c>
-      <c r="BW22">
+      <c r="BZ22">
         <v>27</v>
       </c>
-      <c r="BX22">
+      <c r="CA22">
         <v>15</v>
       </c>
-      <c r="BY22">
+      <c r="CB22">
         <v>10</v>
       </c>
-      <c r="BZ22">
+      <c r="CC22">
         <v>30</v>
       </c>
-      <c r="CA22">
+      <c r="CD22">
         <v>35</v>
       </c>
-      <c r="CB22">
+      <c r="CE22">
         <v>32</v>
       </c>
-      <c r="CC22">
+      <c r="CF22">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:82" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:85" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>186</v>
       </c>
@@ -2452,82 +2560,85 @@
       <c r="Z23" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AA23" s="15" t="s">
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="AB23" s="15" t="s">
+      <c r="AE23" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AC23" s="4" t="s">
+      <c r="AF23" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AD23" s="4" t="s">
+      <c r="AG23" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AE23" s="4" t="s">
+      <c r="AH23" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AF23" s="4">
+      <c r="AI23" s="4">
         <v>3</v>
       </c>
-      <c r="AG23" s="4" t="s">
+      <c r="AJ23" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AH23" s="4" t="s">
+      <c r="AK23" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AI23" s="4" t="s">
+      <c r="AL23" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="AJ23" s="4" t="s">
+      <c r="AM23" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="AO23" s="4"/>
-      <c r="AR23" t="s">
+      <c r="AR23" s="4"/>
+      <c r="AU23" t="s">
         <v>181</v>
       </c>
-      <c r="BG23" s="4" t="s">
+      <c r="BJ23" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="BI23" s="4" t="s">
+      <c r="BL23" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="BK23" s="6"/>
-      <c r="BL23" s="4" t="s">
+      <c r="BN23" s="6"/>
+      <c r="BO23" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM23" s="4" t="s">
+      <c r="BP23" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BV23">
+      <c r="BY23">
         <v>25</v>
       </c>
-      <c r="BW23">
+      <c r="BZ23">
         <v>27</v>
       </c>
-      <c r="BX23">
+      <c r="CA23">
         <v>15</v>
       </c>
-      <c r="BY23">
+      <c r="CB23">
         <v>10</v>
       </c>
-      <c r="BZ23">
+      <c r="CC23">
         <v>30</v>
       </c>
-      <c r="CA23">
+      <c r="CD23">
         <v>35</v>
       </c>
-      <c r="CB23">
+      <c r="CE23">
         <v>32</v>
       </c>
-      <c r="CC23">
+      <c r="CF23">
         <v>23</v>
       </c>
-      <c r="CD23" t="s">
+      <c r="CG23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:82" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:85" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>187</v>
       </c>
@@ -2562,76 +2673,79 @@
       <c r="Z24" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AA24" s="15" t="s">
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="AB24" s="15" t="s">
+      <c r="AE24" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AC24" s="4" t="s">
+      <c r="AF24" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AD24" s="4" t="s">
+      <c r="AG24" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AE24" s="4" t="s">
+      <c r="AH24" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AF24" s="4">
+      <c r="AI24" s="4">
         <v>3</v>
       </c>
-      <c r="AG24" s="4" t="s">
+      <c r="AJ24" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AH24" s="4" t="s">
+      <c r="AK24" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AI24" s="4" t="s">
+      <c r="AL24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="AJ24" s="4" t="s">
+      <c r="AM24" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="AO24" s="4"/>
-      <c r="BI24" s="4" t="s">
+      <c r="AR24" s="4"/>
+      <c r="BL24" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="BK24" s="6"/>
-      <c r="BL24" s="4" t="s">
+      <c r="BN24" s="6"/>
+      <c r="BO24" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM24" s="4" t="s">
+      <c r="BP24" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="BV24">
+      <c r="BY24">
         <v>25</v>
       </c>
-      <c r="BW24">
+      <c r="BZ24">
         <v>27</v>
       </c>
-      <c r="BX24">
+      <c r="CA24">
         <v>15</v>
       </c>
-      <c r="BY24">
+      <c r="CB24">
         <v>10</v>
       </c>
-      <c r="BZ24">
+      <c r="CC24">
         <v>30</v>
       </c>
-      <c r="CA24">
+      <c r="CD24">
         <v>35</v>
       </c>
-      <c r="CB24">
+      <c r="CE24">
         <v>32</v>
       </c>
-      <c r="CC24">
+      <c r="CF24">
         <v>23</v>
       </c>
-      <c r="CD24" t="s">
+      <c r="CG24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>188</v>
       </c>
@@ -2659,27 +2773,27 @@
       <c r="Z25" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AA25" t="s">
-        <v>171</v>
-      </c>
+      <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
-      <c r="AD25" s="4"/>
+      <c r="AD25" t="s">
+        <v>171</v>
+      </c>
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
-      <c r="AH25" s="4" t="s">
+      <c r="AH25" s="4"/>
+      <c r="AI25" s="4"/>
+      <c r="AJ25" s="4"/>
+      <c r="AK25" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AI25" s="4" t="s">
+      <c r="AL25" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="AJ25" s="4" t="s">
+      <c r="AM25" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="AK25" s="4"/>
-      <c r="AL25" s="4"/>
-      <c r="AM25" s="4"/>
       <c r="AN25" s="4"/>
       <c r="AO25" s="4"/>
       <c r="AP25" s="4"/>
@@ -2689,47 +2803,50 @@
       <c r="AT25" s="4"/>
       <c r="AU25" s="4"/>
       <c r="AV25" s="4"/>
-      <c r="BL25" s="4" t="s">
+      <c r="AW25" s="4"/>
+      <c r="AX25" s="4"/>
+      <c r="AY25" s="4"/>
+      <c r="BO25" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM25" s="4" t="s">
+      <c r="BP25" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BN25" t="s">
+      <c r="BQ25" t="s">
         <v>189</v>
       </c>
-      <c r="BO25" t="s">
+      <c r="BR25" t="s">
         <v>190</v>
       </c>
-      <c r="BV25">
+      <c r="BY25">
         <v>25</v>
       </c>
-      <c r="BW25">
+      <c r="BZ25">
         <v>27</v>
       </c>
-      <c r="BX25">
+      <c r="CA25">
         <v>15</v>
       </c>
-      <c r="BY25">
+      <c r="CB25">
         <v>10</v>
       </c>
-      <c r="BZ25">
+      <c r="CC25">
         <v>30</v>
       </c>
-      <c r="CA25">
+      <c r="CD25">
         <v>35</v>
       </c>
-      <c r="CB25">
+      <c r="CE25">
         <v>32</v>
       </c>
-      <c r="CC25">
+      <c r="CF25">
         <v>23</v>
       </c>
-      <c r="CD25" t="s">
+      <c r="CG25" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>191</v>
       </c>
@@ -2755,77 +2872,80 @@
       <c r="Z26" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AA26" s="4" t="s">
-        <v>176</v>
-      </c>
+      <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-      <c r="AD26" s="4"/>
+      <c r="AD26" s="4" t="s">
+        <v>176</v>
+      </c>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
-      <c r="AH26" s="4" t="s">
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4"/>
+      <c r="AK26" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="AI26" s="4" t="s">
+      <c r="AL26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="AJ26" s="4" t="s">
+      <c r="AM26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="AK26" s="4" t="s">
+      <c r="AN26" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="AL26" s="4" t="s">
+      <c r="AO26" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="AN26" s="4" t="s">
+      <c r="AQ26" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="AO26" s="4"/>
-      <c r="AP26" s="4"/>
-      <c r="AQ26" s="4"/>
       <c r="AR26" s="4"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="4"/>
       <c r="AU26" s="4"/>
       <c r="AV26" s="4"/>
-      <c r="BK26" s="9"/>
-      <c r="BL26" s="4" t="s">
+      <c r="AW26" s="4"/>
+      <c r="AX26" s="4"/>
+      <c r="AY26" s="4"/>
+      <c r="BN26" s="9"/>
+      <c r="BO26" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM26" s="4" t="s">
+      <c r="BP26" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BV26">
+      <c r="BY26">
         <v>25</v>
       </c>
-      <c r="BW26">
+      <c r="BZ26">
         <v>27</v>
       </c>
-      <c r="BX26">
+      <c r="CA26">
         <v>15</v>
       </c>
-      <c r="BY26">
+      <c r="CB26">
         <v>10</v>
       </c>
-      <c r="BZ26">
+      <c r="CC26">
         <v>30</v>
       </c>
-      <c r="CA26">
+      <c r="CD26">
         <v>35</v>
       </c>
-      <c r="CB26">
+      <c r="CE26">
         <v>32</v>
       </c>
-      <c r="CC26">
+      <c r="CF26">
         <v>23</v>
       </c>
-      <c r="CD26" t="s">
+      <c r="CG26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>192</v>
       </c>
@@ -2841,200 +2961,220 @@
       <c r="T27" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="AO27" s="4"/>
-      <c r="BL27" s="4" t="s">
+      <c r="AR27" s="4"/>
+      <c r="BO27" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM27" s="4" t="s">
+      <c r="BP27" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BV27">
+      <c r="BY27">
         <v>25</v>
       </c>
-      <c r="BW27">
+      <c r="BZ27">
         <v>27</v>
       </c>
-      <c r="BX27">
+      <c r="CA27">
         <v>15</v>
       </c>
-      <c r="BY27">
+      <c r="CB27">
         <v>10</v>
       </c>
-      <c r="BZ27">
+      <c r="CC27">
         <v>30</v>
       </c>
-      <c r="CA27">
+      <c r="CD27">
         <v>35</v>
       </c>
-      <c r="CB27">
+      <c r="CE27">
         <v>32</v>
       </c>
-      <c r="CC27">
+      <c r="CF27">
         <v>23</v>
       </c>
-      <c r="CD27" t="s">
+      <c r="CG27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>202</v>
       </c>
-      <c r="BL28" s="4" t="s">
+      <c r="BO28" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM28" s="4" t="s">
+      <c r="BP28" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BU28" t="s">
+      <c r="BX28" t="s">
         <v>204</v>
       </c>
-      <c r="BV28">
+      <c r="BY28">
         <v>25</v>
       </c>
-      <c r="BW28">
+      <c r="BZ28">
         <v>27</v>
       </c>
-      <c r="BX28">
+      <c r="CA28">
         <v>15</v>
       </c>
-      <c r="BY28">
+      <c r="CB28">
         <v>10</v>
       </c>
-      <c r="BZ28">
+      <c r="CC28">
         <v>30</v>
       </c>
-      <c r="CA28">
+      <c r="CD28">
         <v>35</v>
       </c>
-      <c r="CB28">
+      <c r="CE28">
         <v>32</v>
       </c>
-      <c r="CC28">
+      <c r="CF28">
         <v>23</v>
       </c>
-      <c r="CD28" t="s">
+      <c r="CG28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>214</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AD29" t="s">
         <v>215</v>
       </c>
-      <c r="BL29" s="4" t="s">
+      <c r="BO29" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM29" s="4" t="s">
+      <c r="BP29" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BV29">
+      <c r="BY29">
         <v>25</v>
       </c>
-      <c r="BW29">
+      <c r="BZ29">
         <v>27</v>
       </c>
-      <c r="BX29">
+      <c r="CA29">
         <v>15</v>
       </c>
-      <c r="BY29">
+      <c r="CB29">
         <v>10</v>
       </c>
-      <c r="BZ29">
+      <c r="CC29">
         <v>30</v>
       </c>
-      <c r="CA29">
+      <c r="CD29">
         <v>35</v>
       </c>
-      <c r="CB29">
+      <c r="CE29">
         <v>32</v>
       </c>
-      <c r="CC29">
+      <c r="CF29">
         <v>23</v>
       </c>
-      <c r="CD29" t="s">
+      <c r="CG29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>216</v>
       </c>
-      <c r="BL30" s="4" t="s">
+      <c r="BO30" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM30" s="4" t="s">
+      <c r="BP30" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="BV30">
-        <v>12</v>
-      </c>
-      <c r="BW30">
-        <v>32</v>
-      </c>
-      <c r="BX30">
-        <v>22</v>
       </c>
       <c r="BY30">
         <v>12</v>
       </c>
       <c r="BZ30">
+        <v>32</v>
+      </c>
+      <c r="CA30">
+        <v>22</v>
+      </c>
+      <c r="CB30">
+        <v>12</v>
+      </c>
+      <c r="CC30">
         <v>23</v>
       </c>
-      <c r="CA30">
+      <c r="CD30">
         <v>20</v>
       </c>
-      <c r="CB30">
+      <c r="CE30">
         <v>32</v>
       </c>
-      <c r="CC30">
+      <c r="CF30">
         <v>21</v>
       </c>
-      <c r="CD30" t="s">
+      <c r="CG30" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>217</v>
       </c>
-      <c r="BL31" s="4" t="s">
+      <c r="BO31" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BM31" s="4" t="s">
+      <c r="BP31" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BV31">
+      <c r="BY31">
         <v>32</v>
       </c>
-      <c r="BW31">
+      <c r="BZ31">
         <v>34</v>
       </c>
-      <c r="BX31">
+      <c r="CA31">
         <v>54</v>
       </c>
-      <c r="BY31">
+      <c r="CB31">
         <v>21</v>
       </c>
-      <c r="BZ31">
+      <c r="CC31">
         <v>13</v>
       </c>
-      <c r="CA31">
+      <c r="CD31">
         <v>5</v>
       </c>
-      <c r="CB31">
+      <c r="CE31">
         <v>2</v>
       </c>
-      <c r="CC31">
+      <c r="CF31">
         <v>12</v>
       </c>
-      <c r="CD31" t="s">
+      <c r="CG31" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>228</v>
+      </c>
+      <c r="BL32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>221</v>
+      </c>
       <c r="C33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -3057,9 +3197,15 @@
       <c r="X33" s="4"/>
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="4"/>
+      <c r="AA33" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>231</v>
+      </c>
       <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
@@ -3070,6 +3216,29 @@
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
       <c r="AM33" s="4"/>
+      <c r="AN33" s="4"/>
+      <c r="AO33" s="4"/>
+      <c r="AP33" s="4"/>
+      <c r="BL33" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>234</v>
+      </c>
+      <c r="BL34" t="s">
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -3080,24 +3249,24 @@
     <hyperlink ref="C4" r:id="rId4" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
     <hyperlink ref="F14" r:id="rId6" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
-    <hyperlink ref="BM19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="BM15" r:id="rId8" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="BM20" r:id="rId9" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
-    <hyperlink ref="BM22" r:id="rId10" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="BP19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="BP15" r:id="rId8" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="BP20" r:id="rId9" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="BP22" r:id="rId10" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
     <hyperlink ref="Y23" r:id="rId11" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
     <hyperlink ref="Y25" r:id="rId12" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
     <hyperlink ref="Y24" r:id="rId13" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
     <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="BM23" r:id="rId15" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
-    <hyperlink ref="BM25" r:id="rId16" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BM26" r:id="rId17" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BM24" r:id="rId18" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BP23" r:id="rId15" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="BP25" r:id="rId16" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BP26" r:id="rId17" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BP24" r:id="rId18" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
     <hyperlink ref="Y19" r:id="rId19" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BT22" r:id="rId20" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
-    <hyperlink ref="BM27:BM29" r:id="rId21" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
-    <hyperlink ref="BM28:BM31" r:id="rId22" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
-    <hyperlink ref="BM30" r:id="rId23" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="B2" r:id="rId24" xr:uid="{8FDC4EB0-4941-4FED-A3AE-F3040B45FB19}"/>
+    <hyperlink ref="BW22" r:id="rId20" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="BP27:BP29" r:id="rId21" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="BP28:BP31" r:id="rId22" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="BP30" r:id="rId23" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="B2" r:id="rId24" xr:uid="{CEF5097F-CBD2-4E5B-AE29-526DB25B999E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId25"/>

</xml_diff>

<commit_message>
Admin 4 new Hero banner Testcase, Adminhelper, Testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DCB42C-627C-45A6-B742-6AF308818951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215F0D2B-6568-4CDA-9C52-B124AA090E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19220" windowHeight="9670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="248">
   <si>
     <t>DataSet</t>
   </si>
@@ -734,6 +734,36 @@
   </si>
   <si>
     <t>qaFlask</t>
+  </si>
+  <si>
+    <t>Herobanner</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>Right Alignment</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>QA Testing Hero Banner</t>
+  </si>
+  <si>
+    <t>HydroFlask</t>
+  </si>
+  <si>
+    <t>QA test Hero Banner</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>Test Banner</t>
   </si>
 </sst>
 </file>
@@ -838,7 +868,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -867,6 +897,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1148,120 +1185,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CG34"/>
+  <dimension ref="A1:CJ35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.42578125" customWidth="1"/>
-    <col min="12" max="12" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7265625" customWidth="1"/>
+    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.453125" customWidth="1"/>
+    <col min="12" max="12" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7265625" customWidth="1"/>
+    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7265625" customWidth="1"/>
+    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="17.5703125" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="17.54296875" customWidth="1"/>
+    <col min="32" max="32" width="14.7265625" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="21" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.7109375" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.7109375" customWidth="1"/>
-    <col min="39" max="39" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="68.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="38" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="11.28515625" customWidth="1"/>
-    <col min="55" max="55" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.140625" customWidth="1"/>
-    <col min="61" max="61" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="14.5703125" customWidth="1"/>
-    <col min="77" max="77" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="146.85546875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="15" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="12" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="17" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="8" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="14" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="5" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.7265625" customWidth="1"/>
+    <col min="37" max="37" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.7265625" customWidth="1"/>
+    <col min="39" max="39" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="60.6328125" customWidth="1"/>
+    <col min="44" max="44" width="26.26953125" style="18" customWidth="1"/>
+    <col min="45" max="45" width="38" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="11.26953125" customWidth="1"/>
+    <col min="56" max="56" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.1796875" customWidth="1"/>
+    <col min="62" max="62" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="13.1796875" customWidth="1"/>
+    <col min="67" max="67" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="14.54296875" customWidth="1"/>
+    <col min="80" max="80" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="146.81640625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="15" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="12" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="17" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="8" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="14" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="5" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:88" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1391,141 +1430,150 @@
       <c r="AQ1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="BO1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="BY1" s="16" t="s">
+      <c r="CB1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="BZ1" s="16" t="s">
+      <c r="CC1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="CA1" s="16" t="s">
+      <c r="CD1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="CB1" s="16" t="s">
+      <c r="CE1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="CC1" s="16" t="s">
+      <c r="CF1" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="CD1" s="16" t="s">
+      <c r="CG1" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="CE1" s="16" t="s">
+      <c r="CH1" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="CF1" s="16" t="s">
+      <c r="CI1" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="CG1" s="17" t="s">
+      <c r="CJ1" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="21" t="s">
         <v>194</v>
       </c>
       <c r="F2" s="4"/>
@@ -1568,7 +1616,7 @@
       <c r="AQ2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="4"/>
+      <c r="AR2" s="22"/>
       <c r="AS2" s="4"/>
       <c r="AT2" s="4"/>
       <c r="AU2" s="4"/>
@@ -1576,8 +1624,9 @@
       <c r="AW2" s="4"/>
       <c r="AX2" s="4"/>
       <c r="AY2" s="4"/>
+      <c r="AZ2" s="4"/>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1627,21 +1676,22 @@
       <c r="AQ3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AR3" s="5" t="s">
+      <c r="AR3" s="22"/>
+      <c r="AS3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AS3" s="4"/>
       <c r="AT3" s="4"/>
       <c r="AU3" s="4"/>
       <c r="AV3" s="4"/>
       <c r="AW3" s="4"/>
       <c r="AX3" s="4"/>
       <c r="AY3" s="4"/>
-      <c r="BG3" s="6"/>
+      <c r="AZ3" s="4"/>
       <c r="BH3" s="6"/>
-      <c r="BI3" s="7"/>
+      <c r="BI3" s="6"/>
+      <c r="BJ3" s="7"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1690,7 +1740,7 @@
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
       <c r="AQ4" s="5"/>
-      <c r="AR4" s="4"/>
+      <c r="AR4" s="22"/>
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4"/>
@@ -1698,11 +1748,12 @@
       <c r="AW4" s="4"/>
       <c r="AX4" s="4"/>
       <c r="AY4" s="4"/>
-      <c r="BG4" s="6"/>
+      <c r="AZ4" s="4"/>
       <c r="BH4" s="6"/>
-      <c r="BI4" s="7"/>
+      <c r="BI4" s="6"/>
+      <c r="BJ4" s="7"/>
     </row>
-    <row r="5" spans="1:85" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:88" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1750,10 +1801,12 @@
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
-      <c r="BK5" s="1"/>
-      <c r="BL5" s="8"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="8"/>
     </row>
-    <row r="6" spans="1:85" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:88" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1797,7 +1850,7 @@
       <c r="AL6" s="4"/>
       <c r="AM6" s="4"/>
       <c r="AQ6" s="4"/>
-      <c r="AR6" s="4"/>
+      <c r="AR6" s="21"/>
       <c r="AS6" s="4"/>
       <c r="AT6" s="4"/>
       <c r="AU6" s="4"/>
@@ -1805,8 +1858,9 @@
       <c r="AW6" s="4"/>
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1851,12 +1905,13 @@
       <c r="AQ7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR7" s="4"/>
+      <c r="AR7" s="22"/>
       <c r="AS7" s="4"/>
       <c r="AT7" s="4"/>
       <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1904,9 +1959,10 @@
         <v>59</v>
       </c>
       <c r="AQ8" s="5"/>
-      <c r="AR8" s="4"/>
+      <c r="AR8" s="22"/>
+      <c r="AS8" s="4"/>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1948,9 +2004,10 @@
       <c r="AO9" s="5"/>
       <c r="AP9" s="5"/>
       <c r="AQ9" s="5"/>
-      <c r="AR9" s="4"/>
+      <c r="AR9" s="22"/>
+      <c r="AS9" s="4"/>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1975,7 +2032,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:88" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1996,8 +2053,9 @@
       <c r="AQ11" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="AR11" s="19"/>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2045,9 +2103,10 @@
         <v>59</v>
       </c>
       <c r="AQ12" s="4"/>
-      <c r="AR12" s="4"/>
+      <c r="AR12" s="21"/>
+      <c r="AS12" s="4"/>
     </row>
-    <row r="13" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2067,10 +2126,12 @@
       <c r="L13" t="s">
         <v>75</v>
       </c>
-      <c r="BK13" s="1"/>
-      <c r="BL13" s="8"/>
+      <c r="BL13" s="1"/>
+      <c r="BM13" s="1"/>
+      <c r="BN13" s="1"/>
+      <c r="BO13" s="8"/>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2105,104 +2166,104 @@
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
-      <c r="AS14" s="5" t="s">
+      <c r="AT14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AT14" s="5" t="s">
+      <c r="AU14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AU14" s="11" t="s">
+      <c r="AV14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="AV14" s="12" t="s">
+      <c r="AW14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="AW14" s="12" t="s">
+      <c r="AX14" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AX14" s="12" t="s">
+      <c r="AY14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AY14" s="12" t="s">
+      <c r="AZ14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AZ14" s="11" t="s">
+      <c r="BA14" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="BA14" s="11"/>
       <c r="BB14" s="11"/>
+      <c r="BC14" s="11"/>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
       <c r="I15" t="s">
         <v>72</v>
       </c>
-      <c r="AV15" s="12" t="s">
+      <c r="AW15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="BA15" t="s">
+      <c r="BB15" t="s">
         <v>109</v>
       </c>
-      <c r="BB15" t="s">
+      <c r="BC15" t="s">
         <v>110</v>
       </c>
-      <c r="BC15" s="5" t="s">
+      <c r="BD15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="BD15" s="5" t="s">
+      <c r="BE15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="BE15" s="9" t="s">
+      <c r="BF15" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BF15" s="13" t="s">
+      <c r="BG15" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="BG15" s="12" t="s">
+      <c r="BH15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="BH15" s="12" t="s">
+      <c r="BI15" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="BP15" s="4" t="s">
+      <c r="BS15" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="BI16" s="9" t="s">
+      <c r="BJ16" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="BJ17" s="9" t="s">
+      <c r="BK17" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="BO17" s="4" t="s">
+      <c r="BR17" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="BK18" t="s">
+      <c r="BL18" t="s">
         <v>98</v>
       </c>
-      <c r="BL18" s="8"/>
-      <c r="BO18" s="4" t="s">
+      <c r="BO18" s="8"/>
+      <c r="BR18" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2243,75 +2304,92 @@
       <c r="AQ19" t="s">
         <v>199</v>
       </c>
-      <c r="AR19" s="4"/>
-      <c r="BK19" s="1"/>
-      <c r="BL19" t="s">
+      <c r="AS19" s="4"/>
+      <c r="BL19" s="1"/>
+      <c r="BM19" s="1"/>
+      <c r="BN19" s="1"/>
+      <c r="BO19" t="s">
         <v>100</v>
       </c>
-      <c r="BM19" t="s">
+      <c r="BP19" t="s">
         <v>101</v>
       </c>
-      <c r="BN19" t="s">
+      <c r="BQ19" t="s">
         <v>102</v>
       </c>
-      <c r="BO19" s="5" t="s">
+      <c r="BR19" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="BP19" s="4" t="s">
+      <c r="BS19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BQ19" s="5" t="s">
+      <c r="BT19" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="BR19" s="5" t="s">
+      <c r="BU19" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="BS19" s="5" t="s">
+      <c r="BV19" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="BY19">
+      <c r="CB19">
         <v>25</v>
       </c>
-      <c r="BZ19">
+      <c r="CC19">
         <v>27</v>
       </c>
-      <c r="CA19">
+      <c r="CD19">
         <v>15</v>
       </c>
-      <c r="CB19">
+      <c r="CE19">
         <v>10</v>
       </c>
-      <c r="CC19">
+      <c r="CF19">
         <v>30</v>
       </c>
-      <c r="CD19">
+      <c r="CG19">
         <v>35</v>
       </c>
-      <c r="CE19">
+      <c r="CH19">
         <v>32</v>
       </c>
-      <c r="CF19">
+      <c r="CI19">
         <v>23</v>
       </c>
-      <c r="CG19" t="s">
+      <c r="CJ19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>117</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" t="s">
+        <v>181</v>
+      </c>
+      <c r="P20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="Y20" s="5" t="s">
-        <v>39</v>
+      <c r="Y20" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
-      <c r="AD20" s="15"/>
+      <c r="AD20" s="4"/>
       <c r="AE20" s="15"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
@@ -2321,84 +2399,92 @@
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
       <c r="AM20" s="4"/>
-      <c r="BG20" s="6"/>
-      <c r="BH20" s="6"/>
-      <c r="BI20" s="7"/>
-      <c r="BJ20" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="BO20" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BP20" s="14" t="s">
-        <v>118</v>
+      <c r="AN20" t="s">
+        <v>242</v>
+      </c>
+      <c r="AP20" s="4"/>
+      <c r="AQ20" t="s">
+        <v>245</v>
+      </c>
+      <c r="AR20" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="AS20" s="4"/>
+      <c r="BL20" s="1"/>
+      <c r="BM20" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="BN20" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="BO20" t="s">
+        <v>100</v>
+      </c>
+      <c r="BP20" t="s">
+        <v>101</v>
       </c>
       <c r="BQ20" t="s">
+        <v>102</v>
+      </c>
+      <c r="BR20" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BS20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BT20" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="BR20" t="s">
-        <v>198</v>
-      </c>
-      <c r="BT20" t="s">
-        <v>115</v>
-      </c>
-      <c r="BU20" t="s">
-        <v>39</v>
-      </c>
-      <c r="BY20">
+      <c r="BU20" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="BV20" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="CB20">
         <v>25</v>
       </c>
-      <c r="BZ20">
+      <c r="CC20">
         <v>27</v>
       </c>
-      <c r="CA20">
+      <c r="CD20">
         <v>15</v>
       </c>
-      <c r="CB20">
+      <c r="CE20">
         <v>10</v>
       </c>
-      <c r="CC20">
+      <c r="CF20">
         <v>30</v>
       </c>
-      <c r="CD20">
+      <c r="CG20">
         <v>35</v>
       </c>
-      <c r="CE20">
+      <c r="CH20">
         <v>32</v>
       </c>
-      <c r="CF20">
+      <c r="CI20">
         <v>23</v>
       </c>
+      <c r="CJ20" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="21" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="S21" s="4"/>
+        <v>117</v>
+      </c>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
+      <c r="Y21" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
-      <c r="AE21" s="4"/>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="15"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="4"/>
@@ -2407,43 +2493,58 @@
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
-      <c r="AO21" s="4"/>
-      <c r="AP21" s="4"/>
-      <c r="AQ21" t="s">
-        <v>200</v>
-      </c>
-      <c r="BO21" s="4" t="s">
+      <c r="BH21" s="6"/>
+      <c r="BI21" s="6"/>
+      <c r="BJ21" s="7"/>
+      <c r="BK21" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="BR21" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BY21">
+      <c r="BS21" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="BT21" t="s">
+        <v>195</v>
+      </c>
+      <c r="BU21" t="s">
+        <v>198</v>
+      </c>
+      <c r="BW21" t="s">
+        <v>115</v>
+      </c>
+      <c r="BX21" t="s">
+        <v>39</v>
+      </c>
+      <c r="CB21">
         <v>25</v>
       </c>
-      <c r="BZ21">
+      <c r="CC21">
         <v>27</v>
       </c>
-      <c r="CA21">
+      <c r="CD21">
         <v>15</v>
       </c>
-      <c r="CB21">
+      <c r="CE21">
         <v>10</v>
       </c>
-      <c r="CC21">
+      <c r="CF21">
         <v>30</v>
       </c>
-      <c r="CD21">
+      <c r="CG21">
         <v>35</v>
       </c>
-      <c r="CE21">
+      <c r="CH21">
         <v>32</v>
       </c>
-      <c r="CF21">
+      <c r="CI21">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2451,12 +2552,13 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="L22" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
@@ -2468,7 +2570,6 @@
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
-      <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
@@ -2481,168 +2582,126 @@
       <c r="AN22" s="4"/>
       <c r="AO22" s="4"/>
       <c r="AP22" s="4"/>
-      <c r="BG22" s="9"/>
-      <c r="BH22" s="9"/>
-      <c r="BO22" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="BP22" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="BV22" t="s">
-        <v>201</v>
-      </c>
-      <c r="BW22" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="BY22">
+      <c r="AQ22" t="s">
+        <v>200</v>
+      </c>
+      <c r="BR22" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="CB22">
         <v>25</v>
       </c>
-      <c r="BZ22">
+      <c r="CC22">
         <v>27</v>
       </c>
-      <c r="CA22">
+      <c r="CD22">
         <v>15</v>
       </c>
-      <c r="CB22">
+      <c r="CE22">
         <v>10</v>
       </c>
-      <c r="CC22">
+      <c r="CF22">
         <v>30</v>
       </c>
-      <c r="CD22">
+      <c r="CG22">
         <v>35</v>
       </c>
-      <c r="CE22">
+      <c r="CH22">
         <v>32</v>
       </c>
-      <c r="CF22">
+      <c r="CI22">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:85" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>186</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="O23" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>145</v>
-      </c>
-      <c r="R23" t="s">
-        <v>146</v>
-      </c>
-      <c r="S23" t="s">
-        <v>147</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="U23" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="V23" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="W23" t="s">
-        <v>152</v>
-      </c>
-      <c r="X23" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y23" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z23" s="4" t="s">
-        <v>156</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
-      <c r="AD23" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE23" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="AF23" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG23" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AH23" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AI23" s="4">
-        <v>3</v>
-      </c>
-      <c r="AJ23" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK23" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AL23" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM23" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="AR23" s="4"/>
-      <c r="AU23" t="s">
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
+      <c r="AL23" s="4"/>
+      <c r="AM23" s="4"/>
+      <c r="AN23" s="4"/>
+      <c r="AO23" s="4"/>
+      <c r="AP23" s="4"/>
+      <c r="BH23" s="9"/>
+      <c r="BI23" s="9"/>
+      <c r="BR23" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BS23" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="BY23" t="s">
+        <v>201</v>
+      </c>
+      <c r="BZ23" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="CB23">
+        <v>25</v>
+      </c>
+      <c r="CC23">
+        <v>27</v>
+      </c>
+      <c r="CD23">
+        <v>15</v>
+      </c>
+      <c r="CE23">
+        <v>10</v>
+      </c>
+      <c r="CF23">
+        <v>30</v>
+      </c>
+      <c r="CG23">
+        <v>35</v>
+      </c>
+      <c r="CH23">
+        <v>32</v>
+      </c>
+      <c r="CI23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:88" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="O24" t="s">
         <v>181</v>
       </c>
-      <c r="BJ23" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="BL23" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="BN23" s="6"/>
-      <c r="BO23" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BP23" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BY23">
-        <v>25</v>
-      </c>
-      <c r="BZ23">
-        <v>27</v>
-      </c>
-      <c r="CA23">
-        <v>15</v>
-      </c>
-      <c r="CB23">
-        <v>10</v>
-      </c>
-      <c r="CC23">
-        <v>30</v>
-      </c>
-      <c r="CD23">
-        <v>35</v>
-      </c>
-      <c r="CE23">
-        <v>32</v>
-      </c>
-      <c r="CF23">
-        <v>23</v>
-      </c>
-      <c r="CG23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:85" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>187</v>
-      </c>
-      <c r="L24" s="4"/>
       <c r="Q24" t="s">
         <v>145</v>
       </c>
@@ -2659,7 +2718,7 @@
         <v>149</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="W24" t="s">
         <v>152</v>
@@ -2706,67 +2765,80 @@
       <c r="AM24" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="AR24" s="4"/>
-      <c r="BL24" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="BN24" s="6"/>
+      <c r="AS24" s="4"/>
+      <c r="AV24" t="s">
+        <v>181</v>
+      </c>
+      <c r="BK24" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="BO24" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="BQ24" s="6"/>
+      <c r="BR24" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP24" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="BY24">
+      <c r="BS24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="CB24">
         <v>25</v>
       </c>
-      <c r="BZ24">
+      <c r="CC24">
         <v>27</v>
       </c>
-      <c r="CA24">
+      <c r="CD24">
         <v>15</v>
       </c>
-      <c r="CB24">
+      <c r="CE24">
         <v>10</v>
       </c>
-      <c r="CC24">
+      <c r="CF24">
         <v>30</v>
       </c>
-      <c r="CD24">
+      <c r="CG24">
         <v>35</v>
       </c>
-      <c r="CE24">
+      <c r="CH24">
         <v>32</v>
       </c>
-      <c r="CF24">
+      <c r="CI24">
         <v>23</v>
       </c>
-      <c r="CG24" t="s">
+      <c r="CJ24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:88" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L25" s="4"/>
-      <c r="P25" s="4"/>
       <c r="Q25" t="s">
         <v>145</v>
       </c>
       <c r="R25" t="s">
         <v>146</v>
       </c>
-      <c r="S25" s="4" t="s">
-        <v>169</v>
+      <c r="S25" t="s">
+        <v>147</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="W25" t="s">
+        <v>152</v>
+      </c>
+      <c r="X25" t="s">
+        <v>153</v>
+      </c>
       <c r="Y25" s="4" t="s">
         <v>154</v>
       </c>
@@ -2776,107 +2848,108 @@
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
-      <c r="AD25" t="s">
-        <v>171</v>
-      </c>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
-      <c r="AG25" s="4"/>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AJ25" s="4"/>
+      <c r="AD25" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE25" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI25" s="4">
+        <v>3</v>
+      </c>
+      <c r="AJ25" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="AK25" s="4" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="AL25" s="4" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="AM25" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN25" s="4"/>
-      <c r="AO25" s="4"/>
-      <c r="AP25" s="4"/>
-      <c r="AQ25" s="4"/>
-      <c r="AR25" s="4"/>
+        <v>165</v>
+      </c>
       <c r="AS25" s="4"/>
-      <c r="AT25" s="4"/>
-      <c r="AU25" s="4"/>
-      <c r="AV25" s="4"/>
-      <c r="AW25" s="4"/>
-      <c r="AX25" s="4"/>
-      <c r="AY25" s="4"/>
       <c r="BO25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="BQ25" s="6"/>
+      <c r="BR25" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BQ25" t="s">
-        <v>189</v>
-      </c>
-      <c r="BR25" t="s">
-        <v>190</v>
-      </c>
-      <c r="BY25">
+      <c r="BS25" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="CB25">
         <v>25</v>
       </c>
-      <c r="BZ25">
+      <c r="CC25">
         <v>27</v>
       </c>
-      <c r="CA25">
+      <c r="CD25">
         <v>15</v>
       </c>
-      <c r="CB25">
+      <c r="CE25">
         <v>10</v>
       </c>
-      <c r="CC25">
+      <c r="CF25">
         <v>30</v>
       </c>
-      <c r="CD25">
+      <c r="CG25">
         <v>35</v>
       </c>
-      <c r="CE25">
+      <c r="CH25">
         <v>32</v>
       </c>
-      <c r="CF25">
+      <c r="CI25">
         <v>23</v>
       </c>
-      <c r="CG25" t="s">
+      <c r="CJ25" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>191</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="L26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" t="s">
         <v>145</v>
       </c>
-      <c r="R26" s="4"/>
+      <c r="R26" t="s">
+        <v>146</v>
+      </c>
       <c r="S26" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
+      <c r="Y26" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="Z26" s="4" t="s">
         <v>156</v>
       </c>
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-      <c r="AD26" s="4" t="s">
-        <v>176</v>
+      <c r="AD26" t="s">
+        <v>171</v>
       </c>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
@@ -2885,24 +2958,19 @@
       <c r="AI26" s="4"/>
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="AL26" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AM26" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN26" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AO26" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AQ26" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AR26" s="4"/>
+        <v>174</v>
+      </c>
+      <c r="AN26" s="4"/>
+      <c r="AO26" s="4"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="4"/>
+      <c r="AR26" s="21"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="4"/>
       <c r="AU26" s="4"/>
@@ -2910,333 +2978,439 @@
       <c r="AW26" s="4"/>
       <c r="AX26" s="4"/>
       <c r="AY26" s="4"/>
-      <c r="BN26" s="9"/>
-      <c r="BO26" s="4" t="s">
+      <c r="AZ26" s="4"/>
+      <c r="BR26" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP26" s="4" t="s">
+      <c r="BS26" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BY26">
+      <c r="BT26" t="s">
+        <v>189</v>
+      </c>
+      <c r="BU26" t="s">
+        <v>190</v>
+      </c>
+      <c r="CB26">
         <v>25</v>
       </c>
-      <c r="BZ26">
+      <c r="CC26">
         <v>27</v>
       </c>
-      <c r="CA26">
+      <c r="CD26">
         <v>15</v>
       </c>
-      <c r="CB26">
+      <c r="CE26">
         <v>10</v>
       </c>
-      <c r="CC26">
+      <c r="CF26">
         <v>30</v>
       </c>
-      <c r="CD26">
+      <c r="CG26">
         <v>35</v>
       </c>
-      <c r="CE26">
+      <c r="CH26">
         <v>32</v>
       </c>
-      <c r="CF26">
+      <c r="CI26">
         <v>23</v>
       </c>
-      <c r="CG26" t="s">
+      <c r="CJ26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>180</v>
       </c>
+      <c r="P27" s="4"/>
       <c r="Q27" t="s">
         <v>145</v>
       </c>
+      <c r="R27" s="4"/>
       <c r="S27" s="4" t="s">
         <v>175</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="AR27" s="4"/>
-      <c r="BO27" s="4" t="s">
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL27" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AM27" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN27" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO27" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AQ27" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR27" s="21"/>
+      <c r="AS27" s="4"/>
+      <c r="AT27" s="4"/>
+      <c r="AU27" s="4"/>
+      <c r="AV27" s="4"/>
+      <c r="AW27" s="4"/>
+      <c r="AX27" s="4"/>
+      <c r="AY27" s="4"/>
+      <c r="AZ27" s="4"/>
+      <c r="BQ27" s="9"/>
+      <c r="BR27" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP27" s="4" t="s">
+      <c r="BS27" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BY27">
+      <c r="CB27">
         <v>25</v>
       </c>
-      <c r="BZ27">
+      <c r="CC27">
         <v>27</v>
       </c>
-      <c r="CA27">
+      <c r="CD27">
         <v>15</v>
       </c>
-      <c r="CB27">
+      <c r="CE27">
         <v>10</v>
       </c>
-      <c r="CC27">
+      <c r="CF27">
         <v>30</v>
       </c>
-      <c r="CD27">
+      <c r="CG27">
         <v>35</v>
       </c>
-      <c r="CE27">
+      <c r="CH27">
         <v>32</v>
       </c>
-      <c r="CF27">
+      <c r="CI27">
         <v>23</v>
       </c>
-      <c r="CG27" t="s">
+      <c r="CJ27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:88" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>192</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>145</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AS28" s="4"/>
+      <c r="BR28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BS28" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="CB28">
+        <v>25</v>
+      </c>
+      <c r="CC28">
+        <v>27</v>
+      </c>
+      <c r="CD28">
+        <v>15</v>
+      </c>
+      <c r="CE28">
+        <v>10</v>
+      </c>
+      <c r="CF28">
+        <v>30</v>
+      </c>
+      <c r="CG28">
+        <v>35</v>
+      </c>
+      <c r="CH28">
+        <v>32</v>
+      </c>
+      <c r="CI28">
+        <v>23</v>
+      </c>
+      <c r="CJ28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:88" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>202</v>
       </c>
-      <c r="BO28" s="4" t="s">
+      <c r="BR29" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP28" s="4" t="s">
+      <c r="BS29" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BX28" t="s">
+      <c r="CA29" t="s">
         <v>204</v>
       </c>
-      <c r="BY28">
+      <c r="CB29">
         <v>25</v>
       </c>
-      <c r="BZ28">
+      <c r="CC29">
         <v>27</v>
       </c>
-      <c r="CA28">
+      <c r="CD29">
         <v>15</v>
       </c>
-      <c r="CB28">
+      <c r="CE29">
         <v>10</v>
       </c>
-      <c r="CC28">
+      <c r="CF29">
         <v>30</v>
       </c>
-      <c r="CD28">
+      <c r="CG29">
         <v>35</v>
       </c>
-      <c r="CE28">
+      <c r="CH29">
         <v>32</v>
       </c>
-      <c r="CF28">
+      <c r="CI29">
         <v>23</v>
       </c>
-      <c r="CG28" t="s">
+      <c r="CJ29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:88" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>214</v>
       </c>
-      <c r="AD29" t="s">
+      <c r="AD30" t="s">
         <v>215</v>
       </c>
-      <c r="BO29" s="4" t="s">
+      <c r="BR30" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP29" s="4" t="s">
+      <c r="BS30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BY29">
+      <c r="CB30">
         <v>25</v>
       </c>
-      <c r="BZ29">
+      <c r="CC30">
         <v>27</v>
       </c>
-      <c r="CA29">
+      <c r="CD30">
         <v>15</v>
       </c>
-      <c r="CB29">
+      <c r="CE30">
         <v>10</v>
       </c>
-      <c r="CC29">
+      <c r="CF30">
         <v>30</v>
       </c>
-      <c r="CD29">
+      <c r="CG30">
         <v>35</v>
       </c>
-      <c r="CE29">
+      <c r="CH30">
         <v>32</v>
       </c>
-      <c r="CF29">
+      <c r="CI30">
         <v>23</v>
       </c>
-      <c r="CG29" t="s">
+      <c r="CJ30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:88" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>216</v>
       </c>
-      <c r="BO30" s="4" t="s">
+      <c r="BR31" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP30" s="4" t="s">
+      <c r="BS31" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="BY30">
+      <c r="CB31">
         <v>12</v>
       </c>
-      <c r="BZ30">
+      <c r="CC31">
         <v>32</v>
       </c>
-      <c r="CA30">
+      <c r="CD31">
         <v>22</v>
       </c>
-      <c r="CB30">
+      <c r="CE31">
         <v>12</v>
       </c>
-      <c r="CC30">
+      <c r="CF31">
         <v>23</v>
       </c>
-      <c r="CD30">
+      <c r="CG31">
         <v>20</v>
       </c>
-      <c r="CE30">
+      <c r="CH31">
         <v>32</v>
       </c>
-      <c r="CF30">
+      <c r="CI31">
         <v>21</v>
       </c>
-      <c r="CG30" t="s">
+      <c r="CJ31" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:88" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>217</v>
       </c>
-      <c r="BO31" s="4" t="s">
+      <c r="BR32" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="BP31" s="4" t="s">
+      <c r="BS32" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BY31">
+      <c r="CB32">
         <v>32</v>
       </c>
-      <c r="BZ31">
+      <c r="CC32">
         <v>34</v>
       </c>
-      <c r="CA31">
+      <c r="CD32">
         <v>54</v>
       </c>
-      <c r="CB31">
+      <c r="CE32">
         <v>21</v>
       </c>
-      <c r="CC31">
+      <c r="CF32">
         <v>13</v>
       </c>
-      <c r="CD31">
+      <c r="CG32">
         <v>5</v>
       </c>
-      <c r="CE31">
+      <c r="CH32">
         <v>2</v>
       </c>
-      <c r="CF31">
+      <c r="CI32">
         <v>12</v>
       </c>
-      <c r="CG31" t="s">
+      <c r="CJ32" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>220</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AA33" t="s">
         <v>226</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AB33" t="s">
         <v>227</v>
       </c>
-      <c r="AC32" t="s">
+      <c r="AC33" t="s">
         <v>228</v>
       </c>
-      <c r="BL32" t="s">
+      <c r="BO33" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>221</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-      <c r="AA33" t="s">
+      <c r="C34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" t="s">
         <v>229</v>
       </c>
-      <c r="AB33" t="s">
+      <c r="AB34" t="s">
         <v>230</v>
       </c>
-      <c r="AC33" t="s">
+      <c r="AC34" t="s">
         <v>231</v>
       </c>
-      <c r="AD33" s="4"/>
-      <c r="AE33" s="4"/>
-      <c r="AF33" s="4"/>
-      <c r="AG33" s="4"/>
-      <c r="AH33" s="4"/>
-      <c r="AI33" s="4"/>
-      <c r="AJ33" s="4"/>
-      <c r="AK33" s="4"/>
-      <c r="AL33" s="4"/>
-      <c r="AM33" s="4"/>
-      <c r="AN33" s="4"/>
-      <c r="AO33" s="4"/>
-      <c r="AP33" s="4"/>
-      <c r="BL33" t="s">
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="4"/>
+      <c r="AJ34" s="4"/>
+      <c r="AK34" s="4"/>
+      <c r="AL34" s="4"/>
+      <c r="AM34" s="4"/>
+      <c r="AN34" s="4"/>
+      <c r="AO34" s="4"/>
+      <c r="AP34" s="4"/>
+      <c r="BO34" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>222</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AA35" t="s">
         <v>232</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AB35" t="s">
         <v>233</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AC35" t="s">
         <v>234</v>
       </c>
-      <c r="BL34" t="s">
+      <c r="BO35" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3249,26 +3423,28 @@
     <hyperlink ref="C4" r:id="rId4" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
     <hyperlink ref="F14" r:id="rId6" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
-    <hyperlink ref="BP19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="BP15" r:id="rId8" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="BP20" r:id="rId9" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
-    <hyperlink ref="BP22" r:id="rId10" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="Y23" r:id="rId11" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
-    <hyperlink ref="Y25" r:id="rId12" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
-    <hyperlink ref="Y24" r:id="rId13" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="BS19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="BS15" r:id="rId8" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="BS21" r:id="rId9" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="BS23" r:id="rId10" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="Y24" r:id="rId11" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="Y26" r:id="rId12" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y25" r:id="rId13" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
     <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="BP23" r:id="rId15" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
-    <hyperlink ref="BP25" r:id="rId16" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BP26" r:id="rId17" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BP24" r:id="rId18" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BS24" r:id="rId15" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="BS26" r:id="rId16" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BS27" r:id="rId17" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BS25" r:id="rId18" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
     <hyperlink ref="Y19" r:id="rId19" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BW22" r:id="rId20" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
-    <hyperlink ref="BP27:BP29" r:id="rId21" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
-    <hyperlink ref="BP28:BP31" r:id="rId22" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
-    <hyperlink ref="BP30" r:id="rId23" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="B2" r:id="rId24" xr:uid="{CEF5097F-CBD2-4E5B-AE29-526DB25B999E}"/>
+    <hyperlink ref="BZ23" r:id="rId20" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="BS28:BS30" r:id="rId21" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="BS29:BS32" r:id="rId22" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="BS31" r:id="rId23" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="BS20" r:id="rId24" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
+    <hyperlink ref="Y20" r:id="rId25" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
+    <hyperlink ref="B2" r:id="rId26" xr:uid="{C530F640-5A3A-45E7-800F-3A1EC68A3189}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Product card configuration- Helper,testdata,Tetscase Code commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215F0D2B-6568-4CDA-9C52-B124AA090E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BDD5EA-16A1-425E-848C-4147AE63B031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19220" windowHeight="9670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="270">
   <si>
     <t>DataSet</t>
   </si>
@@ -475,9 +475,6 @@
     <t>W32075,W32410,W32520,1115580,1165700,1071499B</t>
   </si>
   <si>
-    <t>32 oz Wide Mouth - Copper Brown,32 oz Wide Mouth - Everest Blue,32 oz Wide Mouth - Acai Purple</t>
-  </si>
-  <si>
     <t>Price: high to low</t>
   </si>
   <si>
@@ -496,9 +493,6 @@
     <t>#a8d098</t>
   </si>
   <si>
-    <t>demo-desktop_3.png</t>
-  </si>
-  <si>
     <t>QATEST</t>
   </si>
   <si>
@@ -520,9 +514,6 @@
     <t>hot-card-tiles</t>
   </si>
   <si>
-    <t>OXO 10-Piece POP Container Set,3-Piece Mixing Bowl Set,Cherry &amp; Olive Pitter</t>
-  </si>
-  <si>
     <t>https://mcloud-na-stage.oxo.com/</t>
   </si>
   <si>
@@ -764,6 +755,81 @@
   </si>
   <si>
     <t>Test Banner</t>
+  </si>
+  <si>
+    <t>skatipelli@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Avtuvzwzjogm1!</t>
+  </si>
+  <si>
+    <t>ButtonlinkURL</t>
+  </si>
+  <si>
+    <t>Buttonlinkcategory</t>
+  </si>
+  <si>
+    <t>Buttonlinkproduct</t>
+  </si>
+  <si>
+    <t>Buttonlinkpage</t>
+  </si>
+  <si>
+    <t>alterantivetext</t>
+  </si>
+  <si>
+    <t>titleaatribute</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com/shop/bottles-drinkware/bottles.html</t>
+  </si>
+  <si>
+    <t>Outdoor Kitchen</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Copper Brown</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.oxo.com/shop/kitchenware/pop-containers.html</t>
+  </si>
+  <si>
+    <t>POP Containers</t>
+  </si>
+  <si>
+    <t>OXO 10-Piece POP Container Set</t>
+  </si>
+  <si>
+    <t>qatestalt</t>
+  </si>
+  <si>
+    <t>qatesttitle</t>
+  </si>
+  <si>
+    <t>32-oz-wide-mouth-copper-brown,32-oz-wide-mouth-everest-blue,32-oz-wide-mouth-acai-purple</t>
+  </si>
+  <si>
+    <t>oxo-10-piece-pop-container-set,3-piece-mixing-bowl-set-colored-handles,cherry-olive-pitter</t>
+  </si>
+  <si>
+    <t>preprodURL</t>
+  </si>
+  <si>
+    <t>stageURL</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-preprod.hydroflask.com/</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-preprod.oxo.com/</t>
+  </si>
+  <si>
+    <t>cms-corporate-</t>
+  </si>
+  <si>
+    <t>cms-corporate-pur</t>
+  </si>
+  <si>
+    <t>Test Page</t>
   </si>
 </sst>
 </file>
@@ -773,7 +839,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,6 +879,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -868,7 +940,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -904,6 +976,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1185,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ35"/>
+  <dimension ref="A1:CQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="AG10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK27" sqref="AK27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,95 +1285,99 @@
     <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="17.54296875" customWidth="1"/>
+    <col min="30" max="30" width="29.6328125" customWidth="1"/>
+    <col min="31" max="31" width="17.54296875" customWidth="1"/>
     <col min="32" max="32" width="14.7265625" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.7265625" customWidth="1"/>
-    <col min="37" max="37" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.7265625" customWidth="1"/>
-    <col min="39" max="39" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="45.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="60.6328125" customWidth="1"/>
-    <col min="44" max="44" width="26.26953125" style="18" customWidth="1"/>
-    <col min="45" max="45" width="38" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="11.26953125" customWidth="1"/>
-    <col min="56" max="56" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.1796875" customWidth="1"/>
-    <col min="62" max="62" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="49.54296875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="13.1796875" customWidth="1"/>
-    <col min="67" max="67" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="14.54296875" customWidth="1"/>
-    <col min="80" max="80" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="146.81640625" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="15" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="12" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="17" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="8" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="14" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="5" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="21" style="18" customWidth="1"/>
+    <col min="38" max="38" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.7265625" customWidth="1"/>
+    <col min="41" max="41" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.7265625" customWidth="1"/>
+    <col min="43" max="43" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="17.1796875" style="18" customWidth="1"/>
+    <col min="48" max="48" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.6328125" customWidth="1"/>
+    <col min="50" max="50" width="26.26953125" style="18" customWidth="1"/>
+    <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.26953125" customWidth="1"/>
+    <col min="62" max="62" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.1796875" customWidth="1"/>
+    <col min="68" max="68" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="13.1796875" customWidth="1"/>
+    <col min="73" max="73" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.7265625" style="18" customWidth="1"/>
+    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.54296875" customWidth="1"/>
+    <col min="87" max="87" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="146.81640625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="15" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="17" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="8" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="14" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="5" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:95" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1380,13 +1457,13 @@
         <v>134</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>135</v>
@@ -1400,181 +1477,202 @@
       <c r="AG1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI1" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="AJ1" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="AK1" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="AL1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AN1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AT1" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="AU1" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="AV1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AX1" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="AY1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="BM1" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="BN1" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="BU1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="BS1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="BZ1" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="CA1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="CI1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="CJ1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="CB1" s="16" t="s">
+      <c r="CK1" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="CL1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="CC1" s="16" t="s">
+      <c r="CM1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="CD1" s="16" t="s">
+      <c r="CN1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="CE1" s="16" t="s">
+      <c r="CO1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="CF1" s="16" t="s">
+      <c r="CP1" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="CG1" s="16" t="s">
+      <c r="CQ1" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="CH1" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="CI1" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="CJ1" s="17" t="s">
-        <v>213</v>
-      </c>
     </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>193</v>
+        <v>245</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>194</v>
+        <v>246</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1604,37 +1702,43 @@
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="21"/>
       <c r="AL2" s="4"/>
       <c r="AM2" s="4"/>
       <c r="AN2" s="4"/>
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
-      <c r="AQ2" s="5" t="s">
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="21"/>
+      <c r="AU2" s="21"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="4"/>
-      <c r="AT2" s="4"/>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="4"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4"/>
+      <c r="AX2" s="22"/>
       <c r="AY2" s="4"/>
       <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4"/>
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="4"/>
+      <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1664,34 +1768,40 @@
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="21"/>
       <c r="AL3" s="4"/>
       <c r="AM3" s="4"/>
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
-      <c r="AQ3" s="5" t="s">
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="21"/>
+      <c r="AU3" s="21"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AR3" s="22"/>
-      <c r="AS3" s="5" t="s">
+      <c r="AX3" s="22"/>
+      <c r="AY3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AT3" s="4"/>
-      <c r="AU3" s="4"/>
-      <c r="AV3" s="4"/>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4"/>
-      <c r="AY3" s="4"/>
       <c r="AZ3" s="4"/>
-      <c r="BH3" s="6"/>
-      <c r="BI3" s="6"/>
-      <c r="BJ3" s="7"/>
+      <c r="BA3" s="4"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4"/>
+      <c r="BD3" s="4"/>
+      <c r="BE3" s="4"/>
+      <c r="BF3" s="4"/>
+      <c r="BN3" s="6"/>
+      <c r="BO3" s="6"/>
+      <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1733,27 +1843,31 @@
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="21"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
-      <c r="AQ4" s="5"/>
-      <c r="AR4" s="22"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="22"/>
       <c r="AY4" s="4"/>
       <c r="AZ4" s="4"/>
-      <c r="BH4" s="6"/>
-      <c r="BI4" s="6"/>
-      <c r="BJ4" s="7"/>
+      <c r="BA4" s="4"/>
+      <c r="BB4" s="4"/>
+      <c r="BC4" s="4"/>
+      <c r="BD4" s="4"/>
+      <c r="BE4" s="4"/>
+      <c r="BF4" s="4"/>
+      <c r="BN4" s="6"/>
+      <c r="BO4" s="6"/>
+      <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:88" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1795,18 +1909,22 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="21"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="21"/>
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
-      <c r="BL5" s="1"/>
-      <c r="BM5" s="1"/>
-      <c r="BN5" s="1"/>
-      <c r="BO5" s="8"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="BR5" s="1"/>
+      <c r="BS5" s="1"/>
+      <c r="BT5" s="1"/>
+      <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:88" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1843,24 +1961,28 @@
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
+      <c r="AH6" s="21"/>
+      <c r="AI6" s="21"/>
+      <c r="AJ6" s="21"/>
+      <c r="AK6" s="21"/>
       <c r="AL6" s="4"/>
       <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="4"/>
+      <c r="AP6" s="4"/>
       <c r="AQ6" s="4"/>
-      <c r="AR6" s="21"/>
-      <c r="AS6" s="4"/>
-      <c r="AT6" s="4"/>
-      <c r="AU6" s="4"/>
-      <c r="AV6" s="4"/>
       <c r="AW6" s="4"/>
-      <c r="AX6" s="4"/>
+      <c r="AX6" s="21"/>
       <c r="AY6" s="4"/>
       <c r="AZ6" s="4"/>
+      <c r="BA6" s="4"/>
+      <c r="BB6" s="4"/>
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="4"/>
+      <c r="BE6" s="4"/>
+      <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1893,25 +2015,31 @@
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="4"/>
-      <c r="AJ7" s="4"/>
-      <c r="AK7" s="4"/>
+      <c r="AH7" s="21"/>
+      <c r="AI7" s="21"/>
+      <c r="AJ7" s="21"/>
+      <c r="AK7" s="21"/>
       <c r="AL7" s="4"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
-      <c r="AQ7" s="5" t="s">
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="4"/>
+      <c r="AT7" s="21"/>
+      <c r="AU7" s="21"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR7" s="22"/>
-      <c r="AS7" s="4"/>
-      <c r="AT7" s="4"/>
-      <c r="AU7" s="4"/>
-      <c r="AV7" s="4"/>
+      <c r="AX7" s="22"/>
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="4"/>
+      <c r="BA7" s="4"/>
+      <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1947,22 +2075,28 @@
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="4"/>
-      <c r="AJ8" s="4"/>
-      <c r="AK8" s="4"/>
+      <c r="AH8" s="21"/>
+      <c r="AI8" s="21"/>
+      <c r="AJ8" s="21"/>
+      <c r="AK8" s="21"/>
       <c r="AL8" s="4"/>
       <c r="AM8" s="4"/>
-      <c r="AN8" s="5"/>
-      <c r="AO8" s="5"/>
-      <c r="AP8" s="5" t="s">
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="4"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="22"/>
+      <c r="AU8" s="22"/>
+      <c r="AV8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="22"/>
-      <c r="AS8" s="4"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="22"/>
+      <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1994,20 +2128,26 @@
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="4"/>
-      <c r="AK9" s="4"/>
+      <c r="AH9" s="21"/>
+      <c r="AI9" s="21"/>
+      <c r="AJ9" s="21"/>
+      <c r="AK9" s="21"/>
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
-      <c r="AN9" s="5"/>
-      <c r="AO9" s="5"/>
-      <c r="AP9" s="5"/>
-      <c r="AQ9" s="5"/>
-      <c r="AR9" s="22"/>
-      <c r="AS9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="4"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="22"/>
+      <c r="AU9" s="22"/>
+      <c r="AV9" s="5"/>
+      <c r="AW9" s="5"/>
+      <c r="AX9" s="22"/>
+      <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2023,16 +2163,18 @@
       <c r="O10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AN10" s="5"/>
-      <c r="AO10" s="5"/>
-      <c r="AP10" s="5" t="s">
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="22"/>
+      <c r="AU10" s="22"/>
+      <c r="AV10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AQ10" t="s">
+      <c r="AW10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:88" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2045,17 +2187,24 @@
       <c r="O11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AN11" s="5"/>
-      <c r="AO11" s="5"/>
-      <c r="AP11" s="5" t="s">
+      <c r="AH11" s="19"/>
+      <c r="AI11" s="19"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="22"/>
+      <c r="AU11" s="22"/>
+      <c r="AV11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AQ11" s="2" t="s">
+      <c r="AW11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AR11" s="19"/>
+      <c r="AX11" s="19"/>
+      <c r="BZ11" s="19"/>
     </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2091,22 +2240,28 @@
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="4"/>
-      <c r="AJ12" s="4"/>
-      <c r="AK12" s="4"/>
+      <c r="AH12" s="21"/>
+      <c r="AI12" s="21"/>
+      <c r="AJ12" s="21"/>
+      <c r="AK12" s="21"/>
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
-      <c r="AN12" s="5"/>
-      <c r="AO12" s="5"/>
-      <c r="AP12" s="5" t="s">
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="4"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="22"/>
+      <c r="AU12" s="22"/>
+      <c r="AV12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AQ12" s="4"/>
-      <c r="AR12" s="21"/>
-      <c r="AS12" s="4"/>
+      <c r="AW12" s="4"/>
+      <c r="AX12" s="21"/>
+      <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2126,12 +2281,12 @@
       <c r="L13" t="s">
         <v>75</v>
       </c>
-      <c r="BL13" s="1"/>
-      <c r="BM13" s="1"/>
-      <c r="BN13" s="1"/>
-      <c r="BO13" s="8"/>
+      <c r="BR13" s="1"/>
+      <c r="BS13" s="1"/>
+      <c r="BT13" s="1"/>
+      <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2160,110 +2315,115 @@
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="4"/>
-      <c r="AJ14" s="4"/>
-      <c r="AK14" s="4"/>
+      <c r="AH14" s="21"/>
+      <c r="AI14" s="21"/>
+      <c r="AJ14" s="21"/>
+      <c r="AK14" s="21"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
-      <c r="AT14" s="5" t="s">
+      <c r="AN14" s="4"/>
+      <c r="AO14" s="4"/>
+      <c r="AP14" s="4"/>
+      <c r="AQ14" s="4"/>
+      <c r="AZ14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AU14" s="5" t="s">
+      <c r="BA14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AV14" s="11" t="s">
+      <c r="BB14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="AW14" s="12" t="s">
+      <c r="BC14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="AX14" s="12" t="s">
+      <c r="BD14" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="AY14" s="12" t="s">
+      <c r="BE14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AZ14" s="12" t="s">
+      <c r="BF14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="BA14" s="11" t="s">
+      <c r="BG14" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="BB14" s="11"/>
-      <c r="BC14" s="11"/>
+      <c r="BH14" s="11"/>
+      <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
       <c r="I15" t="s">
         <v>72</v>
       </c>
-      <c r="AW15" s="12" t="s">
+      <c r="BC15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="BB15" t="s">
+      <c r="BH15" t="s">
         <v>109</v>
       </c>
-      <c r="BC15" t="s">
+      <c r="BI15" t="s">
         <v>110</v>
       </c>
-      <c r="BD15" s="5" t="s">
+      <c r="BJ15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="BE15" s="5" t="s">
+      <c r="BK15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="BF15" s="9" t="s">
+      <c r="BL15" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BG15" s="13" t="s">
+      <c r="BM15" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="BH15" s="12" t="s">
+      <c r="BN15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="BI15" s="12" t="s">
+      <c r="BO15" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="BS15" s="4" t="s">
+      <c r="BY15" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="BZ15" s="21"/>
     </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="BJ16" s="9" t="s">
+      <c r="BP16" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="BK17" s="9" t="s">
+      <c r="BQ17" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="BR17" s="4" t="s">
-        <v>155</v>
+      <c r="BX17" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="BL18" t="s">
+      <c r="BR18" t="s">
         <v>98</v>
       </c>
-      <c r="BO18" s="8"/>
-      <c r="BR18" s="4" t="s">
-        <v>155</v>
+      <c r="BU18" s="8"/>
+      <c r="BX18" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2277,14 +2437,14 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="P19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="Y19" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
@@ -2294,75 +2454,76 @@
       <c r="AE19" s="15"/>
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
-      <c r="AH19" s="4"/>
-      <c r="AI19" s="4"/>
-      <c r="AJ19" s="4"/>
-      <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
       <c r="AM19" s="4"/>
+      <c r="AN19" s="4"/>
+      <c r="AO19" s="4"/>
       <c r="AP19" s="4"/>
-      <c r="AQ19" t="s">
-        <v>199</v>
-      </c>
-      <c r="AS19" s="4"/>
-      <c r="BL19" s="1"/>
-      <c r="BM19" s="1"/>
-      <c r="BN19" s="1"/>
-      <c r="BO19" t="s">
+      <c r="AQ19" s="4"/>
+      <c r="AV19" s="4"/>
+      <c r="AW19" t="s">
+        <v>196</v>
+      </c>
+      <c r="AY19" s="4"/>
+      <c r="BR19" s="1"/>
+      <c r="BS19" s="1"/>
+      <c r="BT19" s="1"/>
+      <c r="BU19" t="s">
         <v>100</v>
       </c>
-      <c r="BP19" t="s">
+      <c r="BV19" t="s">
         <v>101</v>
       </c>
-      <c r="BQ19" t="s">
+      <c r="BW19" t="s">
         <v>102</v>
       </c>
-      <c r="BR19" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="BS19" s="4" t="s">
+      <c r="BX19" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="BY19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BT19" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="BU19" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="BV19" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="CB19">
+      <c r="BZ19" s="21"/>
+      <c r="CA19" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="CB19" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="CC19" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="CI19">
         <v>25</v>
       </c>
-      <c r="CC19">
+      <c r="CJ19">
         <v>27</v>
       </c>
-      <c r="CD19">
+      <c r="CK19">
         <v>15</v>
       </c>
-      <c r="CE19">
+      <c r="CL19">
         <v>10</v>
       </c>
-      <c r="CF19">
+      <c r="CM19">
         <v>30</v>
       </c>
-      <c r="CG19">
+      <c r="CN19">
         <v>35</v>
       </c>
-      <c r="CH19">
+      <c r="CO19">
         <v>32</v>
       </c>
-      <c r="CI19">
+      <c r="CP19">
         <v>23</v>
       </c>
-      <c r="CJ19" t="s">
+      <c r="CQ19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2371,19 +2532,19 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="P20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
       <c r="Y20" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
@@ -2393,83 +2554,88 @@
       <c r="AE20" s="15"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
-      <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
-      <c r="AJ20" s="4"/>
-      <c r="AK20" s="4"/>
+      <c r="AH20" s="21"/>
+      <c r="AI20" s="21"/>
+      <c r="AJ20" s="21"/>
+      <c r="AK20" s="21"/>
       <c r="AL20" s="4"/>
       <c r="AM20" s="4"/>
-      <c r="AN20" t="s">
+      <c r="AN20" s="4"/>
+      <c r="AO20" s="4"/>
+      <c r="AP20" s="4"/>
+      <c r="AQ20" s="4"/>
+      <c r="AR20" t="s">
+        <v>239</v>
+      </c>
+      <c r="AV20" s="4"/>
+      <c r="AW20" t="s">
         <v>242</v>
       </c>
-      <c r="AP20" s="4"/>
-      <c r="AQ20" t="s">
-        <v>245</v>
-      </c>
-      <c r="AR20" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="AS20" s="4"/>
-      <c r="BL20" s="1"/>
-      <c r="BM20" s="1" t="s">
+      <c r="AX20" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="BN20" s="1" t="s">
+      <c r="AY20" s="4"/>
+      <c r="BR20" s="1"/>
+      <c r="BS20" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="BO20" t="s">
+      <c r="BT20" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BU20" t="s">
         <v>100</v>
       </c>
-      <c r="BP20" t="s">
+      <c r="BV20" t="s">
         <v>101</v>
       </c>
-      <c r="BQ20" t="s">
+      <c r="BW20" t="s">
         <v>102</v>
       </c>
-      <c r="BR20" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="BS20" s="4" t="s">
+      <c r="BX20" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="BY20" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BT20" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="BU20" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="BV20" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="CB20">
+      <c r="BZ20" s="21"/>
+      <c r="CA20" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="CB20" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="CC20" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="CI20">
         <v>25</v>
       </c>
-      <c r="CC20">
+      <c r="CJ20">
         <v>27</v>
       </c>
-      <c r="CD20">
+      <c r="CK20">
         <v>15</v>
       </c>
-      <c r="CE20">
+      <c r="CL20">
         <v>10</v>
       </c>
-      <c r="CF20">
+      <c r="CM20">
         <v>30</v>
       </c>
-      <c r="CG20">
+      <c r="CN20">
         <v>35</v>
       </c>
-      <c r="CH20">
+      <c r="CO20">
         <v>32</v>
       </c>
-      <c r="CI20">
+      <c r="CP20">
         <v>23</v>
       </c>
-      <c r="CJ20" t="s">
+      <c r="CQ20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -2487,62 +2653,67 @@
       <c r="AE21" s="15"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
-      <c r="AJ21" s="4"/>
-      <c r="AK21" s="4"/>
+      <c r="AH21" s="21"/>
+      <c r="AI21" s="21"/>
+      <c r="AJ21" s="21"/>
+      <c r="AK21" s="21"/>
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
-      <c r="BH21" s="6"/>
-      <c r="BI21" s="6"/>
-      <c r="BJ21" s="7"/>
-      <c r="BK21" s="9" t="s">
+      <c r="AN21" s="4"/>
+      <c r="AO21" s="4"/>
+      <c r="AP21" s="4"/>
+      <c r="AQ21" s="4"/>
+      <c r="BN21" s="6"/>
+      <c r="BO21" s="6"/>
+      <c r="BP21" s="7"/>
+      <c r="BQ21" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="BR21" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS21" s="14" t="s">
+      <c r="BX21" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY21" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="BT21" t="s">
+      <c r="BZ21" s="14"/>
+      <c r="CA21" t="s">
+        <v>192</v>
+      </c>
+      <c r="CB21" t="s">
         <v>195</v>
       </c>
-      <c r="BU21" t="s">
-        <v>198</v>
-      </c>
-      <c r="BW21" t="s">
+      <c r="CD21" t="s">
         <v>115</v>
       </c>
-      <c r="BX21" t="s">
+      <c r="CE21" t="s">
         <v>39</v>
       </c>
-      <c r="CB21">
+      <c r="CI21">
         <v>25</v>
       </c>
-      <c r="CC21">
+      <c r="CJ21">
         <v>27</v>
       </c>
-      <c r="CD21">
+      <c r="CK21">
         <v>15</v>
       </c>
-      <c r="CE21">
+      <c r="CL21">
         <v>10</v>
       </c>
-      <c r="CF21">
+      <c r="CM21">
         <v>30</v>
       </c>
-      <c r="CG21">
+      <c r="CN21">
         <v>35</v>
       </c>
-      <c r="CH21">
+      <c r="CO21">
         <v>32</v>
       </c>
-      <c r="CI21">
+      <c r="CP21">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -2573,47 +2744,53 @@
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
-      <c r="AH22" s="4"/>
-      <c r="AI22" s="4"/>
-      <c r="AJ22" s="4"/>
-      <c r="AK22" s="4"/>
+      <c r="AH22" s="21"/>
+      <c r="AI22" s="21"/>
+      <c r="AJ22" s="21"/>
+      <c r="AK22" s="21"/>
       <c r="AL22" s="4"/>
       <c r="AM22" s="4"/>
       <c r="AN22" s="4"/>
       <c r="AO22" s="4"/>
       <c r="AP22" s="4"/>
-      <c r="AQ22" t="s">
-        <v>200</v>
-      </c>
-      <c r="BR22" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="CB22">
+      <c r="AQ22" s="4"/>
+      <c r="AR22" s="4"/>
+      <c r="AS22" s="4"/>
+      <c r="AT22" s="21"/>
+      <c r="AU22" s="21"/>
+      <c r="AV22" s="4"/>
+      <c r="AW22" t="s">
+        <v>197</v>
+      </c>
+      <c r="BX22" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="CI22">
         <v>25</v>
       </c>
-      <c r="CC22">
+      <c r="CJ22">
         <v>27</v>
       </c>
-      <c r="CD22">
+      <c r="CK22">
         <v>15</v>
       </c>
-      <c r="CE22">
+      <c r="CL22">
         <v>10</v>
       </c>
-      <c r="CF22">
+      <c r="CM22">
         <v>30</v>
       </c>
-      <c r="CG22">
+      <c r="CN22">
         <v>35</v>
       </c>
-      <c r="CH22">
+      <c r="CO22">
         <v>32</v>
       </c>
-      <c r="CI22">
+      <c r="CP22">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -2644,63 +2821,70 @@
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
-      <c r="AH23" s="4"/>
-      <c r="AI23" s="4"/>
-      <c r="AJ23" s="4"/>
-      <c r="AK23" s="4"/>
+      <c r="AH23" s="21"/>
+      <c r="AI23" s="21"/>
+      <c r="AJ23" s="21"/>
+      <c r="AK23" s="21"/>
       <c r="AL23" s="4"/>
       <c r="AM23" s="4"/>
       <c r="AN23" s="4"/>
       <c r="AO23" s="4"/>
       <c r="AP23" s="4"/>
-      <c r="BH23" s="9"/>
-      <c r="BI23" s="9"/>
-      <c r="BR23" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="BS23" s="14" t="s">
+      <c r="AQ23" s="4"/>
+      <c r="AR23" s="4"/>
+      <c r="AS23" s="4"/>
+      <c r="AT23" s="21"/>
+      <c r="AU23" s="21"/>
+      <c r="AV23" s="4"/>
+      <c r="BN23" s="9"/>
+      <c r="BO23" s="9"/>
+      <c r="BX23" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="BY23" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="BY23" t="s">
-        <v>201</v>
-      </c>
-      <c r="BZ23" s="14" t="s">
+      <c r="BZ23" s="14"/>
+      <c r="CF23" t="s">
+        <v>198</v>
+      </c>
+      <c r="CG23" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="CB23">
+      <c r="CI23">
         <v>25</v>
       </c>
-      <c r="CC23">
+      <c r="CJ23">
         <v>27</v>
       </c>
-      <c r="CD23">
+      <c r="CK23">
         <v>15</v>
       </c>
-      <c r="CE23">
+      <c r="CL23">
         <v>10</v>
       </c>
-      <c r="CF23">
+      <c r="CM23">
         <v>30</v>
       </c>
-      <c r="CG23">
+      <c r="CN23">
         <v>35</v>
       </c>
-      <c r="CH23">
+      <c r="CO23">
         <v>32</v>
       </c>
-      <c r="CI23">
+      <c r="CP23">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:88" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="O24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q24" t="s">
         <v>145</v>
@@ -2718,101 +2902,122 @@
         <v>149</v>
       </c>
       <c r="V24" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="W24" t="s">
         <v>151</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>152</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="Y24" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="Z24" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="15" t="s">
-        <v>158</v>
+        <v>267</v>
       </c>
       <c r="AE24" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AF24" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AG24" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH24" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="AI24" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ24" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK24" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AL24" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AM24" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN24" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AH24" s="4" t="s">
+      <c r="AO24" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AI24" s="4">
-        <v>3</v>
-      </c>
-      <c r="AJ24" s="4" t="s">
+      <c r="AP24" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AK24" s="4" t="s">
+      <c r="AQ24" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AL24" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM24" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="AS24" s="4"/>
-      <c r="AV24" t="s">
-        <v>181</v>
-      </c>
-      <c r="BK24" s="4" t="s">
+      <c r="AT24" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="AU24" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="AY24" s="4"/>
+      <c r="BB24" t="s">
+        <v>178</v>
+      </c>
+      <c r="BQ24" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="BO24" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="BQ24" s="6"/>
-      <c r="BR24" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS24" s="4" t="s">
+      <c r="BU24" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="BW24" s="6"/>
+      <c r="BX24" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY24" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CB24">
+      <c r="BZ24" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="CI24">
         <v>25</v>
       </c>
-      <c r="CC24">
+      <c r="CJ24">
         <v>27</v>
       </c>
-      <c r="CD24">
+      <c r="CK24">
         <v>15</v>
       </c>
-      <c r="CE24">
+      <c r="CL24">
         <v>10</v>
       </c>
-      <c r="CF24">
+      <c r="CM24">
         <v>30</v>
       </c>
-      <c r="CG24">
+      <c r="CN24">
         <v>35</v>
       </c>
-      <c r="CH24">
+      <c r="CO24">
         <v>32</v>
       </c>
-      <c r="CI24">
+      <c r="CP24">
         <v>23</v>
       </c>
-      <c r="CJ24" t="s">
+      <c r="CQ24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:88" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="L25" s="4"/>
       <c r="Q25" t="s">
@@ -2831,95 +3036,116 @@
         <v>149</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>166</v>
+        <v>262</v>
       </c>
       <c r="W25" t="s">
+        <v>151</v>
+      </c>
+      <c r="X25" t="s">
         <v>152</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="Y25" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="Z25" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="15" t="s">
-        <v>158</v>
+        <v>268</v>
       </c>
       <c r="AE25" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AF25" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AG25" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH25" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="AI25" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="AJ25" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="AK25" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AL25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AM25" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN25" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AH25" s="4" t="s">
+      <c r="AO25" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AI25" s="4">
-        <v>3</v>
-      </c>
-      <c r="AJ25" s="4" t="s">
+      <c r="AP25" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AK25" s="4" t="s">
+      <c r="AQ25" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AL25" s="4" t="s">
+      <c r="AT25" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="AU25" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="AY25" s="4"/>
+      <c r="BU25" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="BW25" s="6"/>
+      <c r="BX25" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY25" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="AM25" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="AS25" s="4"/>
-      <c r="BO25" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="BQ25" s="6"/>
-      <c r="BR25" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS25" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="CB25">
+      <c r="BZ25" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="CI25">
         <v>25</v>
       </c>
-      <c r="CC25">
+      <c r="CJ25">
         <v>27</v>
       </c>
-      <c r="CD25">
+      <c r="CK25">
         <v>15</v>
       </c>
-      <c r="CE25">
+      <c r="CL25">
         <v>10</v>
       </c>
-      <c r="CF25">
+      <c r="CM25">
         <v>30</v>
       </c>
-      <c r="CG25">
+      <c r="CN25">
         <v>35</v>
       </c>
-      <c r="CH25">
+      <c r="CO25">
         <v>32</v>
       </c>
-      <c r="CI25">
+      <c r="CP25">
         <v>23</v>
       </c>
-      <c r="CJ25" t="s">
+      <c r="CQ25" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L26" s="4"/>
       <c r="P26" s="4"/>
@@ -2930,101 +3156,112 @@
         <v>146</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z26" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
       <c r="AD26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
-      <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
-      <c r="AJ26" s="4"/>
-      <c r="AK26" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL26" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM26" s="4" t="s">
-        <v>174</v>
-      </c>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="21"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="4"/>
       <c r="AN26" s="4"/>
-      <c r="AO26" s="4"/>
-      <c r="AP26" s="4"/>
-      <c r="AQ26" s="4"/>
-      <c r="AR26" s="21"/>
+      <c r="AO26" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AP26" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AQ26" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AR26" s="4"/>
       <c r="AS26" s="4"/>
-      <c r="AT26" s="4"/>
-      <c r="AU26" s="4"/>
+      <c r="AT26" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="AU26" s="21" t="s">
+        <v>260</v>
+      </c>
       <c r="AV26" s="4"/>
       <c r="AW26" s="4"/>
-      <c r="AX26" s="4"/>
+      <c r="AX26" s="21"/>
       <c r="AY26" s="4"/>
       <c r="AZ26" s="4"/>
-      <c r="BR26" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS26" s="4" t="s">
+      <c r="BA26" s="4"/>
+      <c r="BB26" s="4"/>
+      <c r="BC26" s="4"/>
+      <c r="BD26" s="4"/>
+      <c r="BE26" s="4"/>
+      <c r="BF26" s="4"/>
+      <c r="BX26" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY26" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BT26" t="s">
-        <v>189</v>
-      </c>
-      <c r="BU26" t="s">
-        <v>190</v>
-      </c>
-      <c r="CB26">
+      <c r="BZ26" s="21"/>
+      <c r="CA26" t="s">
+        <v>186</v>
+      </c>
+      <c r="CB26" t="s">
+        <v>187</v>
+      </c>
+      <c r="CI26">
         <v>25</v>
       </c>
-      <c r="CC26">
+      <c r="CJ26">
         <v>27</v>
       </c>
-      <c r="CD26">
+      <c r="CK26">
         <v>15</v>
       </c>
-      <c r="CE26">
+      <c r="CL26">
         <v>10</v>
       </c>
-      <c r="CF26">
+      <c r="CM26">
         <v>30</v>
       </c>
-      <c r="CG26">
+      <c r="CN26">
         <v>35</v>
       </c>
-      <c r="CH26">
+      <c r="CO26">
         <v>32</v>
       </c>
-      <c r="CI26">
+      <c r="CP26">
         <v>23</v>
       </c>
-      <c r="CJ26" t="s">
+      <c r="CQ26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" t="s">
@@ -3032,10 +3269,10 @@
       </c>
       <c r="R27" s="4"/>
       <c r="S27" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
@@ -3043,311 +3280,323 @@
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
       <c r="AD27" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
-      <c r="AH27" s="4"/>
-      <c r="AI27" s="4"/>
-      <c r="AJ27" s="4"/>
-      <c r="AK27" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="AL27" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AM27" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN27" s="4" t="s">
-        <v>184</v>
-      </c>
+      <c r="AH27" s="21"/>
+      <c r="AI27" s="21"/>
+      <c r="AJ27" s="21"/>
+      <c r="AK27" s="21"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
       <c r="AO27" s="4" t="s">
-        <v>184</v>
+        <v>174</v>
+      </c>
+      <c r="AP27" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="AQ27" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AR27" s="21"/>
-      <c r="AS27" s="4"/>
-      <c r="AT27" s="4"/>
-      <c r="AU27" s="4"/>
-      <c r="AV27" s="4"/>
-      <c r="AW27" s="4"/>
-      <c r="AX27" s="4"/>
+        <v>175</v>
+      </c>
+      <c r="AR27" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AS27" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AT27" s="21"/>
+      <c r="AU27" s="21"/>
+      <c r="AW27" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AX27" s="21"/>
       <c r="AY27" s="4"/>
       <c r="AZ27" s="4"/>
-      <c r="BQ27" s="9"/>
-      <c r="BR27" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS27" s="4" t="s">
+      <c r="BA27" s="4"/>
+      <c r="BB27" s="4"/>
+      <c r="BC27" s="4"/>
+      <c r="BD27" s="4"/>
+      <c r="BE27" s="4"/>
+      <c r="BF27" s="4"/>
+      <c r="BW27" s="9"/>
+      <c r="BX27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY27" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CB27">
+      <c r="BZ27" s="21"/>
+      <c r="CI27">
         <v>25</v>
       </c>
-      <c r="CC27">
+      <c r="CJ27">
         <v>27</v>
       </c>
-      <c r="CD27">
+      <c r="CK27">
         <v>15</v>
       </c>
-      <c r="CE27">
+      <c r="CL27">
         <v>10</v>
       </c>
-      <c r="CF27">
+      <c r="CM27">
         <v>30</v>
       </c>
-      <c r="CG27">
+      <c r="CN27">
         <v>35</v>
       </c>
-      <c r="CH27">
+      <c r="CO27">
         <v>32</v>
       </c>
-      <c r="CI27">
+      <c r="CP27">
         <v>23</v>
       </c>
-      <c r="CJ27" t="s">
+      <c r="CQ27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Q28" t="s">
         <v>145</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AS28" s="4"/>
-      <c r="BR28" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS28" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AY28" s="4"/>
+      <c r="BX28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY28" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CB28">
+      <c r="BZ28" s="21"/>
+      <c r="CI28">
         <v>25</v>
       </c>
-      <c r="CC28">
+      <c r="CJ28">
         <v>27</v>
       </c>
-      <c r="CD28">
+      <c r="CK28">
         <v>15</v>
       </c>
-      <c r="CE28">
+      <c r="CL28">
         <v>10</v>
       </c>
-      <c r="CF28">
+      <c r="CM28">
         <v>30</v>
       </c>
-      <c r="CG28">
+      <c r="CN28">
         <v>35</v>
       </c>
-      <c r="CH28">
+      <c r="CO28">
         <v>32</v>
       </c>
-      <c r="CI28">
+      <c r="CP28">
         <v>23</v>
       </c>
-      <c r="CJ28" t="s">
+      <c r="CQ28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>202</v>
-      </c>
-      <c r="BR29" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS29" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="BX29" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY29" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CA29" t="s">
-        <v>204</v>
-      </c>
-      <c r="CB29">
+      <c r="BZ29" s="21"/>
+      <c r="CH29" t="s">
+        <v>201</v>
+      </c>
+      <c r="CI29">
         <v>25</v>
       </c>
-      <c r="CC29">
+      <c r="CJ29">
         <v>27</v>
       </c>
-      <c r="CD29">
+      <c r="CK29">
         <v>15</v>
       </c>
-      <c r="CE29">
+      <c r="CL29">
         <v>10</v>
       </c>
-      <c r="CF29">
+      <c r="CM29">
         <v>30</v>
       </c>
-      <c r="CG29">
+      <c r="CN29">
         <v>35</v>
       </c>
-      <c r="CH29">
+      <c r="CO29">
         <v>32</v>
       </c>
-      <c r="CI29">
+      <c r="CP29">
         <v>23</v>
       </c>
-      <c r="CJ29" t="s">
+      <c r="CQ29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:88" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>212</v>
+      </c>
+      <c r="BX30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY30" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BZ30" s="21"/>
+      <c r="CI30">
+        <v>25</v>
+      </c>
+      <c r="CJ30">
+        <v>27</v>
+      </c>
+      <c r="CK30">
+        <v>15</v>
+      </c>
+      <c r="CL30">
+        <v>10</v>
+      </c>
+      <c r="CM30">
+        <v>30</v>
+      </c>
+      <c r="CN30">
+        <v>35</v>
+      </c>
+      <c r="CO30">
+        <v>32</v>
+      </c>
+      <c r="CP30">
+        <v>23</v>
+      </c>
+      <c r="CQ30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>213</v>
+      </c>
+      <c r="BX31" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY31" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="BZ31" s="21"/>
+      <c r="CI31">
+        <v>12</v>
+      </c>
+      <c r="CJ31">
+        <v>32</v>
+      </c>
+      <c r="CK31">
+        <v>22</v>
+      </c>
+      <c r="CL31">
+        <v>12</v>
+      </c>
+      <c r="CM31">
+        <v>23</v>
+      </c>
+      <c r="CN31">
+        <v>20</v>
+      </c>
+      <c r="CO31">
+        <v>32</v>
+      </c>
+      <c r="CP31">
+        <v>21</v>
+      </c>
+      <c r="CQ31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>214</v>
       </c>
-      <c r="AD30" t="s">
-        <v>215</v>
-      </c>
-      <c r="BR30" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS30" s="4" t="s">
+      <c r="BX32" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY32" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CB30">
-        <v>25</v>
-      </c>
-      <c r="CC30">
-        <v>27</v>
-      </c>
-      <c r="CD30">
-        <v>15</v>
-      </c>
-      <c r="CE30">
-        <v>10</v>
-      </c>
-      <c r="CF30">
-        <v>30</v>
-      </c>
-      <c r="CG30">
-        <v>35</v>
-      </c>
-      <c r="CH30">
+      <c r="BZ32" s="21"/>
+      <c r="CI32">
         <v>32</v>
       </c>
-      <c r="CI30">
-        <v>23</v>
-      </c>
-      <c r="CJ30" t="s">
-        <v>77</v>
+      <c r="CJ32">
+        <v>34</v>
+      </c>
+      <c r="CK32">
+        <v>54</v>
+      </c>
+      <c r="CL32">
+        <v>21</v>
+      </c>
+      <c r="CM32">
+        <v>13</v>
+      </c>
+      <c r="CN32">
+        <v>5</v>
+      </c>
+      <c r="CO32">
+        <v>2</v>
+      </c>
+      <c r="CP32">
+        <v>12</v>
+      </c>
+      <c r="CQ32" t="s">
+        <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:88" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>216</v>
-      </c>
-      <c r="BR31" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS31" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="CB31">
-        <v>12</v>
-      </c>
-      <c r="CC31">
-        <v>32</v>
-      </c>
-      <c r="CD31">
-        <v>22</v>
-      </c>
-      <c r="CE31">
-        <v>12</v>
-      </c>
-      <c r="CF31">
-        <v>23</v>
-      </c>
-      <c r="CG31">
-        <v>20</v>
-      </c>
-      <c r="CH31">
-        <v>32</v>
-      </c>
-      <c r="CI31">
-        <v>21</v>
-      </c>
-      <c r="CJ31" t="s">
+    <row r="33" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>225</v>
+      </c>
+      <c r="BU33" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:88" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>217</v>
-      </c>
-      <c r="BR32" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BS32" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="CB32">
-        <v>32</v>
-      </c>
-      <c r="CC32">
-        <v>34</v>
-      </c>
-      <c r="CD32">
-        <v>54</v>
-      </c>
-      <c r="CE32">
-        <v>21</v>
-      </c>
-      <c r="CF32">
-        <v>13</v>
-      </c>
-      <c r="CG32">
-        <v>5</v>
-      </c>
-      <c r="CH32">
-        <v>2</v>
-      </c>
-      <c r="CI32">
-        <v>12</v>
-      </c>
-      <c r="CJ32" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="33" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>220</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>226</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>227</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>228</v>
-      </c>
-      <c r="BO33" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>221</v>
       </c>
       <c r="C34" s="4"/>
       <c r="F34" s="4"/>
@@ -3372,79 +3621,89 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
       <c r="AA34" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="AB34" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AC34" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
-      <c r="AH34" s="4"/>
-      <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="4"/>
+      <c r="AH34" s="21"/>
+      <c r="AI34" s="21"/>
+      <c r="AJ34" s="21"/>
+      <c r="AK34" s="21"/>
       <c r="AL34" s="4"/>
       <c r="AM34" s="4"/>
       <c r="AN34" s="4"/>
       <c r="AO34" s="4"/>
       <c r="AP34" s="4"/>
-      <c r="BO34" t="s">
-        <v>236</v>
+      <c r="AQ34" s="4"/>
+      <c r="AR34" s="4"/>
+      <c r="AS34" s="4"/>
+      <c r="AT34" s="21"/>
+      <c r="AU34" s="21"/>
+      <c r="AV34" s="4"/>
+      <c r="BU34" t="s">
+        <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA35" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>231</v>
+      </c>
+      <c r="BU35" t="s">
         <v>232</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>233</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>234</v>
-      </c>
-      <c r="BO35" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="F14" r:id="rId6" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
-    <hyperlink ref="BS19" r:id="rId7" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="BS15" r:id="rId8" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="BS21" r:id="rId9" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
-    <hyperlink ref="BS23" r:id="rId10" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="Y24" r:id="rId11" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
-    <hyperlink ref="Y26" r:id="rId12" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
-    <hyperlink ref="Y25" r:id="rId13" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
-    <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="BS24" r:id="rId15" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
-    <hyperlink ref="BS26" r:id="rId16" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BS27" r:id="rId17" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BS25" r:id="rId18" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
-    <hyperlink ref="Y19" r:id="rId19" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BZ23" r:id="rId20" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
-    <hyperlink ref="BS28:BS30" r:id="rId21" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
-    <hyperlink ref="BS29:BS32" r:id="rId22" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
-    <hyperlink ref="BS31" r:id="rId23" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="BS20" r:id="rId24" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
-    <hyperlink ref="Y20" r:id="rId25" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
-    <hyperlink ref="B2" r:id="rId26" xr:uid="{C530F640-5A3A-45E7-800F-3A1EC68A3189}"/>
+    <hyperlink ref="BY29:BY32" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="AH25" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
+    <hyperlink ref="AH24" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{C530F640-5A3A-45E7-800F-3A1EC68A3189}"/>
+    <hyperlink ref="Y20" r:id="rId5" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
+    <hyperlink ref="BY20" r:id="rId6" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
+    <hyperlink ref="BY31" r:id="rId7" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="BY28:BY30" r:id="rId8" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="CG23" r:id="rId9" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="Y19" r:id="rId10" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
+    <hyperlink ref="BY25" r:id="rId11" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BY27" r:id="rId12" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BY26" r:id="rId13" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BY24" r:id="rId14" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="B3" r:id="rId15" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
+    <hyperlink ref="Y25" r:id="rId16" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="Y26" r:id="rId17" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y24" r:id="rId18" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="BY23" r:id="rId19" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="BY21" r:id="rId20" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="BY15" r:id="rId21" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="BY19" r:id="rId22" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="F14" r:id="rId23" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
+    <hyperlink ref="B4" r:id="rId24" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
+    <hyperlink ref="C4" r:id="rId25" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="F5" r:id="rId26" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="F6" r:id="rId27" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="B5" r:id="rId28" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
+    <hyperlink ref="BZ25" r:id="rId29" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
+    <hyperlink ref="BZ24" r:id="rId30" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Magento admin testcase commit, testdata, Helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BDD5EA-16A1-425E-848C-4147AE63B031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32165AA6-A0ED-474F-B7A9-7251907B8DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:CQ35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AG10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK27" sqref="AK27"/>
+      <selection activeCell="AK25" sqref="AK24:AK25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changes for Admin Testdata & Config
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32165AA6-A0ED-474F-B7A9-7251907B8DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFEFB7F-2C56-4740-92AC-1C90D55A0A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="11078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="269">
   <si>
     <t>DataSet</t>
   </si>
@@ -812,9 +812,6 @@
   </si>
   <si>
     <t>preprodURL</t>
-  </si>
-  <si>
-    <t>stageURL</t>
   </si>
   <si>
     <t>https://mcloud-na-preprod.hydroflask.com/</t>
@@ -940,7 +937,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -969,13 +966,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1260,11 +1250,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK25" sqref="AK24:AK25"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BY7" sqref="BY7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
@@ -1291,7 +1281,7 @@
     <col min="31" max="31" width="17.54296875" customWidth="1"/>
     <col min="32" max="32" width="14.7265625" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="21" style="18" customWidth="1"/>
+    <col min="34" max="37" width="21" customWidth="1"/>
     <col min="38" max="38" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="15.7265625" customWidth="1"/>
@@ -1300,10 +1290,10 @@
     <col min="43" max="43" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="17.1796875" style="18" customWidth="1"/>
+    <col min="46" max="47" width="17.1796875" customWidth="1"/>
     <col min="48" max="48" width="45.81640625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="60.6328125" customWidth="1"/>
-    <col min="50" max="50" width="26.26953125" style="18" customWidth="1"/>
+    <col min="50" max="50" width="26.26953125" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="10.54296875" bestFit="1" customWidth="1"/>
@@ -1329,7 +1319,7 @@
     <col min="75" max="75" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7265625" style="18" customWidth="1"/>
+    <col min="78" max="78" width="54.7265625" customWidth="1"/>
     <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="9.1796875" bestFit="1" customWidth="1"/>
@@ -1377,7 +1367,7 @@
     <col min="123" max="123" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:95" ht="23.55" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1477,16 +1467,16 @@
       <c r="AG1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" s="20" t="s">
+      <c r="AH1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="AI1" s="20" t="s">
+      <c r="AI1" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="AJ1" s="20" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="AK1" s="20" t="s">
+      <c r="AK1" s="3" t="s">
         <v>250</v>
       </c>
       <c r="AL1" s="3" t="s">
@@ -1513,10 +1503,10 @@
       <c r="AS1" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="AT1" s="20" t="s">
+      <c r="AT1" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="AU1" s="20" t="s">
+      <c r="AU1" s="3" t="s">
         <v>252</v>
       </c>
       <c r="AV1" s="3" t="s">
@@ -1525,7 +1515,7 @@
       <c r="AW1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AX1" s="20" t="s">
+      <c r="AX1" s="3" t="s">
         <v>243</v>
       </c>
       <c r="AY1" s="3" t="s">
@@ -1607,9 +1597,9 @@
         <v>38</v>
       </c>
       <c r="BY1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="BZ1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
         <v>263</v>
       </c>
       <c r="CA1" s="3" t="s">
@@ -1664,14 +1654,14 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="4" t="s">
         <v>246</v>
       </c>
       <c r="F2" s="4"/>
@@ -1702,10 +1692,10 @@
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
       <c r="AM2" s="4"/>
       <c r="AN2" s="4"/>
@@ -1714,13 +1704,13 @@
       <c r="AQ2" s="4"/>
       <c r="AR2" s="4"/>
       <c r="AS2" s="4"/>
-      <c r="AT2" s="21"/>
-      <c r="AU2" s="21"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
       <c r="AW2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AX2" s="22"/>
+      <c r="AX2" s="5"/>
       <c r="AY2" s="4"/>
       <c r="AZ2" s="4"/>
       <c r="BA2" s="4"/>
@@ -1730,7 +1720,7 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1768,10 +1758,10 @@
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21"/>
-      <c r="AK3" s="21"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
       <c r="AL3" s="4"/>
       <c r="AM3" s="4"/>
       <c r="AN3" s="4"/>
@@ -1780,13 +1770,13 @@
       <c r="AQ3" s="4"/>
       <c r="AR3" s="4"/>
       <c r="AS3" s="4"/>
-      <c r="AT3" s="21"/>
-      <c r="AU3" s="21"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
       <c r="AV3" s="4"/>
       <c r="AW3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AX3" s="22"/>
+      <c r="AX3" s="5"/>
       <c r="AY3" s="5" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1791,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1843,10 +1833,10 @@
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
-      <c r="AH4" s="21"/>
-      <c r="AI4" s="21"/>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="21"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
@@ -1854,7 +1844,7 @@
       <c r="AP4" s="4"/>
       <c r="AQ4" s="4"/>
       <c r="AW4" s="5"/>
-      <c r="AX4" s="22"/>
+      <c r="AX4" s="5"/>
       <c r="AY4" s="4"/>
       <c r="AZ4" s="4"/>
       <c r="BA4" s="4"/>
@@ -1867,7 +1857,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:95" ht="24.7" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1909,10 +1899,10 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="21"/>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="21"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
@@ -1924,7 +1914,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:95" ht="13.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1961,10 +1951,10 @@
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="21"/>
-      <c r="AI6" s="21"/>
-      <c r="AJ6" s="21"/>
-      <c r="AK6" s="21"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
@@ -1972,7 +1962,7 @@
       <c r="AP6" s="4"/>
       <c r="AQ6" s="4"/>
       <c r="AW6" s="4"/>
-      <c r="AX6" s="21"/>
+      <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
       <c r="AZ6" s="4"/>
       <c r="BA6" s="4"/>
@@ -1982,7 +1972,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2015,10 +2005,10 @@
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="21"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
@@ -2027,19 +2017,19 @@
       <c r="AQ7" s="4"/>
       <c r="AR7" s="4"/>
       <c r="AS7" s="4"/>
-      <c r="AT7" s="21"/>
-      <c r="AU7" s="21"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
       <c r="AV7" s="4"/>
       <c r="AW7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AX7" s="22"/>
+      <c r="AX7" s="5"/>
       <c r="AY7" s="4"/>
       <c r="AZ7" s="4"/>
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2075,10 +2065,10 @@
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
-      <c r="AH8" s="21"/>
-      <c r="AI8" s="21"/>
-      <c r="AJ8" s="21"/>
-      <c r="AK8" s="21"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
       <c r="AM8" s="4"/>
       <c r="AN8" s="4"/>
@@ -2087,16 +2077,16 @@
       <c r="AQ8" s="4"/>
       <c r="AR8" s="5"/>
       <c r="AS8" s="5"/>
-      <c r="AT8" s="22"/>
-      <c r="AU8" s="22"/>
+      <c r="AT8" s="5"/>
+      <c r="AU8" s="5"/>
       <c r="AV8" s="5" t="s">
         <v>59</v>
       </c>
       <c r="AW8" s="5"/>
-      <c r="AX8" s="22"/>
+      <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2128,10 +2118,10 @@
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
-      <c r="AH9" s="21"/>
-      <c r="AI9" s="21"/>
-      <c r="AJ9" s="21"/>
-      <c r="AK9" s="21"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
@@ -2140,14 +2130,14 @@
       <c r="AQ9" s="4"/>
       <c r="AR9" s="5"/>
       <c r="AS9" s="5"/>
-      <c r="AT9" s="22"/>
-      <c r="AU9" s="22"/>
+      <c r="AT9" s="5"/>
+      <c r="AU9" s="5"/>
       <c r="AV9" s="5"/>
       <c r="AW9" s="5"/>
-      <c r="AX9" s="22"/>
+      <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2165,8 +2155,8 @@
       </c>
       <c r="AR10" s="5"/>
       <c r="AS10" s="5"/>
-      <c r="AT10" s="22"/>
-      <c r="AU10" s="22"/>
+      <c r="AT10" s="5"/>
+      <c r="AU10" s="5"/>
       <c r="AV10" s="5" t="s">
         <v>59</v>
       </c>
@@ -2174,7 +2164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:95" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2187,24 +2177,18 @@
       <c r="O11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AH11" s="19"/>
-      <c r="AI11" s="19"/>
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
       <c r="AR11" s="5"/>
       <c r="AS11" s="5"/>
-      <c r="AT11" s="22"/>
-      <c r="AU11" s="22"/>
+      <c r="AT11" s="5"/>
+      <c r="AU11" s="5"/>
       <c r="AV11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="AW11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AX11" s="19"/>
-      <c r="BZ11" s="19"/>
     </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2240,10 +2224,10 @@
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="21"/>
-      <c r="AI12" s="21"/>
-      <c r="AJ12" s="21"/>
-      <c r="AK12" s="21"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
@@ -2252,16 +2236,16 @@
       <c r="AQ12" s="4"/>
       <c r="AR12" s="5"/>
       <c r="AS12" s="5"/>
-      <c r="AT12" s="22"/>
-      <c r="AU12" s="22"/>
+      <c r="AT12" s="5"/>
+      <c r="AU12" s="5"/>
       <c r="AV12" s="5" t="s">
         <v>59</v>
       </c>
       <c r="AW12" s="4"/>
-      <c r="AX12" s="21"/>
+      <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:95" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2286,7 +2270,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2315,10 +2299,10 @@
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
-      <c r="AH14" s="21"/>
-      <c r="AI14" s="21"/>
-      <c r="AJ14" s="21"/>
-      <c r="AK14" s="21"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -2352,7 +2336,7 @@
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2389,9 +2373,9 @@
       <c r="BY15" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="BZ15" s="21"/>
+      <c r="BZ15" s="4"/>
     </row>
-    <row r="16" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2399,7 +2383,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2410,7 +2394,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:95" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2423,7 +2407,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2483,7 +2467,7 @@
       <c r="BY19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ19" s="21"/>
+      <c r="BZ19" s="4"/>
       <c r="CA19" s="5" t="s">
         <v>192</v>
       </c>
@@ -2521,7 +2505,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>235</v>
       </c>
@@ -2554,10 +2538,10 @@
       <c r="AE20" s="15"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
-      <c r="AH20" s="21"/>
-      <c r="AI20" s="21"/>
-      <c r="AJ20" s="21"/>
-      <c r="AK20" s="21"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
       <c r="AM20" s="4"/>
       <c r="AN20" s="4"/>
@@ -2571,7 +2555,7 @@
       <c r="AW20" t="s">
         <v>242</v>
       </c>
-      <c r="AX20" s="18" t="s">
+      <c r="AX20" t="s">
         <v>244</v>
       </c>
       <c r="AY20" s="4"/>
@@ -2597,7 +2581,7 @@
       <c r="BY20" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ20" s="21"/>
+      <c r="BZ20" s="4"/>
       <c r="CA20" s="5" t="s">
         <v>192</v>
       </c>
@@ -2635,7 +2619,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -2653,10 +2637,10 @@
       <c r="AE21" s="15"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
-      <c r="AH21" s="21"/>
-      <c r="AI21" s="21"/>
-      <c r="AJ21" s="21"/>
-      <c r="AK21" s="21"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
@@ -2713,7 +2697,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -2744,10 +2728,10 @@
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
-      <c r="AH22" s="21"/>
-      <c r="AI22" s="21"/>
-      <c r="AJ22" s="21"/>
-      <c r="AK22" s="21"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
       <c r="AM22" s="4"/>
       <c r="AN22" s="4"/>
@@ -2756,8 +2740,8 @@
       <c r="AQ22" s="4"/>
       <c r="AR22" s="4"/>
       <c r="AS22" s="4"/>
-      <c r="AT22" s="21"/>
-      <c r="AU22" s="21"/>
+      <c r="AT22" s="4"/>
+      <c r="AU22" s="4"/>
       <c r="AV22" s="4"/>
       <c r="AW22" t="s">
         <v>197</v>
@@ -2790,7 +2774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -2821,10 +2805,10 @@
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
-      <c r="AH23" s="21"/>
-      <c r="AI23" s="21"/>
-      <c r="AJ23" s="21"/>
-      <c r="AK23" s="21"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
       <c r="AM23" s="4"/>
       <c r="AN23" s="4"/>
@@ -2833,8 +2817,8 @@
       <c r="AQ23" s="4"/>
       <c r="AR23" s="4"/>
       <c r="AS23" s="4"/>
-      <c r="AT23" s="21"/>
-      <c r="AU23" s="21"/>
+      <c r="AT23" s="4"/>
+      <c r="AU23" s="4"/>
       <c r="AV23" s="4"/>
       <c r="BN23" s="9"/>
       <c r="BO23" s="9"/>
@@ -2876,7 +2860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>183</v>
       </c>
@@ -2920,7 +2904,7 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AE24" s="15" t="s">
         <v>157</v>
@@ -2931,17 +2915,17 @@
       <c r="AG24" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AH24" s="21" t="s">
+      <c r="AH24" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="AI24" s="23" t="s">
+      <c r="AI24" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="AJ24" s="23" t="s">
+      <c r="AJ24" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="AK24" s="21" t="s">
-        <v>269</v>
+      <c r="AK24" s="4" t="s">
+        <v>268</v>
       </c>
       <c r="AL24" s="4" t="s">
         <v>159</v>
@@ -2961,10 +2945,10 @@
       <c r="AQ24" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AT24" s="21" t="s">
+      <c r="AT24" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="AU24" s="21" t="s">
+      <c r="AU24" s="4" t="s">
         <v>260</v>
       </c>
       <c r="AY24" s="4"/>
@@ -2984,8 +2968,8 @@
       <c r="BY24" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ24" s="21" t="s">
-        <v>265</v>
+      <c r="BZ24" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="CI24">
         <v>25</v>
@@ -3015,7 +2999,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>184</v>
       </c>
@@ -3054,7 +3038,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AE25" s="15" t="s">
         <v>157</v>
@@ -3065,17 +3049,17 @@
       <c r="AG25" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AH25" s="21" t="s">
+      <c r="AH25" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="AI25" s="23" t="s">
+      <c r="AI25" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="AJ25" s="21" t="s">
+      <c r="AJ25" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="AK25" s="21" t="s">
-        <v>269</v>
+      <c r="AK25" s="4" t="s">
+        <v>268</v>
       </c>
       <c r="AL25" s="4" t="s">
         <v>159</v>
@@ -3095,10 +3079,10 @@
       <c r="AQ25" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AT25" s="21" t="s">
+      <c r="AT25" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="AU25" s="21" t="s">
+      <c r="AU25" s="4" t="s">
         <v>260</v>
       </c>
       <c r="AY25" s="4"/>
@@ -3112,8 +3096,8 @@
       <c r="BY25" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="BZ25" s="21" t="s">
-        <v>266</v>
+      <c r="BZ25" s="4" t="s">
+        <v>265</v>
       </c>
       <c r="CI25">
         <v>25</v>
@@ -3143,7 +3127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>185</v>
       </c>
@@ -3180,10 +3164,10 @@
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
-      <c r="AH26" s="21"/>
-      <c r="AI26" s="21"/>
-      <c r="AJ26" s="21"/>
-      <c r="AK26" s="21"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4"/>
+      <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
       <c r="AM26" s="4"/>
       <c r="AN26" s="4"/>
@@ -3198,15 +3182,15 @@
       </c>
       <c r="AR26" s="4"/>
       <c r="AS26" s="4"/>
-      <c r="AT26" s="21" t="s">
+      <c r="AT26" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="AU26" s="21" t="s">
+      <c r="AU26" s="4" t="s">
         <v>260</v>
       </c>
       <c r="AV26" s="4"/>
       <c r="AW26" s="4"/>
-      <c r="AX26" s="21"/>
+      <c r="AX26" s="4"/>
       <c r="AY26" s="4"/>
       <c r="AZ26" s="4"/>
       <c r="BA26" s="4"/>
@@ -3221,7 +3205,7 @@
       <c r="BY26" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ26" s="21"/>
+      <c r="BZ26" s="4"/>
       <c r="CA26" t="s">
         <v>186</v>
       </c>
@@ -3256,7 +3240,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>188</v>
       </c>
@@ -3291,10 +3275,10 @@
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
-      <c r="AH27" s="21"/>
-      <c r="AI27" s="21"/>
-      <c r="AJ27" s="21"/>
-      <c r="AK27" s="21"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="4"/>
       <c r="AN27" s="4"/>
@@ -3313,12 +3297,12 @@
       <c r="AS27" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="AT27" s="21"/>
-      <c r="AU27" s="21"/>
+      <c r="AT27" s="4"/>
+      <c r="AU27" s="4"/>
       <c r="AW27" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="AX27" s="21"/>
+      <c r="AX27" s="4"/>
       <c r="AY27" s="4"/>
       <c r="AZ27" s="4"/>
       <c r="BA27" s="4"/>
@@ -3334,7 +3318,7 @@
       <c r="BY27" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ27" s="21"/>
+      <c r="BZ27" s="4"/>
       <c r="CI27">
         <v>25</v>
       </c>
@@ -3363,7 +3347,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>189</v>
       </c>
@@ -3386,7 +3370,7 @@
       <c r="BY28" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ28" s="21"/>
+      <c r="BZ28" s="4"/>
       <c r="CI28">
         <v>25</v>
       </c>
@@ -3415,7 +3399,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>199</v>
       </c>
@@ -3425,7 +3409,7 @@
       <c r="BY29" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ29" s="21"/>
+      <c r="BZ29" s="4"/>
       <c r="CH29" t="s">
         <v>201</v>
       </c>
@@ -3457,7 +3441,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>211</v>
       </c>
@@ -3470,7 +3454,7 @@
       <c r="BY30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ30" s="21"/>
+      <c r="BZ30" s="4"/>
       <c r="CI30">
         <v>25</v>
       </c>
@@ -3499,7 +3483,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>213</v>
       </c>
@@ -3509,7 +3493,7 @@
       <c r="BY31" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="BZ31" s="21"/>
+      <c r="BZ31" s="4"/>
       <c r="CI31">
         <v>12</v>
       </c>
@@ -3538,7 +3522,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>214</v>
       </c>
@@ -3548,7 +3532,7 @@
       <c r="BY32" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ32" s="21"/>
+      <c r="BZ32" s="4"/>
       <c r="CI32">
         <v>32</v>
       </c>
@@ -3577,7 +3561,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:73" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>217</v>
       </c>
@@ -3594,7 +3578,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:73" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>218</v>
       </c>
@@ -3633,10 +3617,10 @@
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
-      <c r="AH34" s="21"/>
-      <c r="AI34" s="21"/>
-      <c r="AJ34" s="21"/>
-      <c r="AK34" s="21"/>
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="4"/>
+      <c r="AJ34" s="4"/>
+      <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
       <c r="AM34" s="4"/>
       <c r="AN34" s="4"/>
@@ -3645,14 +3629,14 @@
       <c r="AQ34" s="4"/>
       <c r="AR34" s="4"/>
       <c r="AS34" s="4"/>
-      <c r="AT34" s="21"/>
-      <c r="AU34" s="21"/>
+      <c r="AT34" s="4"/>
+      <c r="AU34" s="4"/>
       <c r="AV34" s="4"/>
       <c r="BU34" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:73" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
Admin testcase commit - testcase, helper,testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFEFB7F-2C56-4740-92AC-1C90D55A0A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{CEFEFB7F-2C56-4740-92AC-1C90D55A0A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3ABA440-1CAA-41DE-8DA1-C45F71B1C10A}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="11078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="270">
   <si>
     <t>DataSet</t>
   </si>
@@ -499,9 +499,6 @@
     <t>Page</t>
   </si>
   <si>
-    <t>Shop,Bottles</t>
-  </si>
-  <si>
     <t>Bottles</t>
   </si>
   <si>
@@ -796,9 +793,6 @@
     <t>POP Containers</t>
   </si>
   <si>
-    <t>OXO 10-Piece POP Container Set</t>
-  </si>
-  <si>
     <t>qatestalt</t>
   </si>
   <si>
@@ -827,6 +821,15 @@
   </si>
   <si>
     <t>Test Page</t>
+  </si>
+  <si>
+    <t>Cups &amp; Tumblers,Food Jars</t>
+  </si>
+  <si>
+    <t>POP Containers,Cookware &amp; Bakeware Sets</t>
+  </si>
+  <si>
+    <t>POP Container Set</t>
   </si>
 </sst>
 </file>
@@ -1250,11 +1253,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BT1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BY7" sqref="BY7"/>
+    <sheetView tabSelected="1" topLeftCell="AE7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
@@ -1281,8 +1284,10 @@
     <col min="31" max="31" width="17.54296875" customWidth="1"/>
     <col min="32" max="32" width="14.7265625" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="21" customWidth="1"/>
+    <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21" customWidth="1"/>
+    <col min="38" max="38" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="15.7265625" customWidth="1"/>
     <col min="41" max="41" width="20.26953125" bestFit="1" customWidth="1"/>
@@ -1367,7 +1372,7 @@
     <col min="123" max="123" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" ht="23.55" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:95" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1447,13 +1452,13 @@
         <v>134</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>135</v>
@@ -1468,16 +1473,16 @@
         <v>138</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="AL1" s="3" t="s">
         <v>139</v>
@@ -1498,16 +1503,16 @@
         <v>144</v>
       </c>
       <c r="AR1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="AS1" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="AT1" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU1" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>16</v>
@@ -1516,7 +1521,7 @@
         <v>17</v>
       </c>
       <c r="AX1" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AY1" s="3" t="s">
         <v>18</v>
@@ -1579,10 +1584,10 @@
         <v>34</v>
       </c>
       <c r="BS1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="BT1" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="BU1" s="3" t="s">
         <v>35</v>
@@ -1600,7 +1605,7 @@
         <v>39</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="CA1" s="3" t="s">
         <v>104</v>
@@ -1624,45 +1629,45 @@
         <v>124</v>
       </c>
       <c r="CH1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="CI1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="CJ1" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="CJ1" s="16" t="s">
+      <c r="CK1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="CK1" s="16" t="s">
+      <c r="CL1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="CL1" s="16" t="s">
+      <c r="CM1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="CM1" s="16" t="s">
+      <c r="CN1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="CN1" s="16" t="s">
+      <c r="CO1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="CO1" s="16" t="s">
+      <c r="CP1" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="CP1" s="16" t="s">
+      <c r="CQ1" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="CQ1" s="17" t="s">
-        <v>210</v>
-      </c>
     </row>
-    <row r="2" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1720,15 +1725,15 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1791,7 +1796,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1857,7 +1862,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:95" ht="24.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1914,7 +1919,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:95" ht="13.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1972,7 +1977,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2029,7 +2034,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2086,7 +2091,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2137,7 +2142,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2164,7 +2169,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:95" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2188,7 +2193,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2245,7 +2250,7 @@
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:95" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2270,7 +2275,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2336,7 +2341,7 @@
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2375,7 +2380,7 @@
       </c>
       <c r="BZ15" s="4"/>
     </row>
-    <row r="16" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2383,7 +2388,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2394,7 +2399,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:95" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2407,7 +2412,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2421,7 +2426,7 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P19" s="4"/>
       <c r="T19" s="4"/>
@@ -2446,7 +2451,7 @@
       <c r="AQ19" s="4"/>
       <c r="AV19" s="4"/>
       <c r="AW19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AY19" s="4"/>
       <c r="BR19" s="1"/>
@@ -2462,20 +2467,20 @@
         <v>102</v>
       </c>
       <c r="BX19" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BY19" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BZ19" s="4"/>
       <c r="CA19" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="CB19" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="CB19" s="5" t="s">
+      <c r="CC19" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="CC19" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="CI19">
         <v>25</v>
@@ -2505,9 +2510,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2516,12 +2521,12 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P20" s="4"/>
       <c r="T20" s="4"/>
@@ -2549,22 +2554,22 @@
       <c r="AP20" s="4"/>
       <c r="AQ20" s="4"/>
       <c r="AR20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AV20" s="4"/>
       <c r="AW20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AX20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AY20" s="4"/>
       <c r="BR20" s="1"/>
       <c r="BS20" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="BT20" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="BU20" t="s">
         <v>100</v>
@@ -2576,20 +2581,20 @@
         <v>102</v>
       </c>
       <c r="BX20" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BY20" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BZ20" s="4"/>
       <c r="CA20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="CB20" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="CB20" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="CC20" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="CI20">
         <v>25</v>
@@ -2619,7 +2624,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -2661,10 +2666,10 @@
       </c>
       <c r="BZ21" s="14"/>
       <c r="CA21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="CB21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="CD21" t="s">
         <v>115</v>
@@ -2697,7 +2702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -2744,7 +2749,7 @@
       <c r="AU22" s="4"/>
       <c r="AV22" s="4"/>
       <c r="AW22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="BX22" s="4" t="s">
         <v>154</v>
@@ -2774,7 +2779,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -2823,14 +2828,14 @@
       <c r="BN23" s="9"/>
       <c r="BO23" s="9"/>
       <c r="BX23" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BY23" s="14" t="s">
         <v>103</v>
       </c>
       <c r="BZ23" s="14"/>
       <c r="CF23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="CG23" s="14" t="s">
         <v>118</v>
@@ -2860,15 +2865,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q24" t="s">
         <v>145</v>
@@ -2886,7 +2891,7 @@
         <v>149</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="W24" t="s">
         <v>151</v>
@@ -2904,7 +2909,7 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AE24" s="15" t="s">
         <v>157</v>
@@ -2916,44 +2921,44 @@
         <v>158</v>
       </c>
       <c r="AH24" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AI24" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="AI24" s="18" t="s">
+      <c r="AJ24" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="AJ24" s="18" t="s">
-        <v>255</v>
-      </c>
       <c r="AK24" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AL24" s="4" t="s">
-        <v>159</v>
+        <v>267</v>
       </c>
       <c r="AM24" s="4">
         <v>3</v>
       </c>
       <c r="AN24" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO24" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AO24" s="4" t="s">
+      <c r="AP24" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AP24" s="4" t="s">
+      <c r="AQ24" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AQ24" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="AT24" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AU24" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AY24" s="4"/>
       <c r="BB24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="BQ24" s="4" t="s">
         <v>150</v>
@@ -2969,7 +2974,7 @@
         <v>103</v>
       </c>
       <c r="BZ24" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="CI24">
         <v>25</v>
@@ -2999,9 +3004,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L25" s="4"/>
       <c r="Q25" t="s">
@@ -3020,7 +3025,7 @@
         <v>149</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W25" t="s">
         <v>151</v>
@@ -3038,7 +3043,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AE25" s="15" t="s">
         <v>157</v>
@@ -3047,57 +3052,57 @@
         <v>115</v>
       </c>
       <c r="AG25" s="4" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="AH25" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AI25" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="AI25" s="18" t="s">
-        <v>257</v>
-      </c>
       <c r="AJ25" s="4" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="AK25" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="AL25" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="AL25" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="AM25" s="4">
         <v>3</v>
       </c>
       <c r="AN25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO25" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AO25" s="4" t="s">
+      <c r="AP25" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AP25" s="4" t="s">
+      <c r="AQ25" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AQ25" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="AT25" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AU25" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AY25" s="4"/>
       <c r="BU25" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BW25" s="6"/>
       <c r="BX25" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY25" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BZ25" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="CI25">
         <v>25</v>
@@ -3127,9 +3132,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L26" s="4"/>
       <c r="P26" s="4"/>
@@ -3140,10 +3145,10 @@
         <v>146</v>
       </c>
       <c r="S26" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="T26" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="T26" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
@@ -3159,7 +3164,7 @@
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
       <c r="AD26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
@@ -3172,21 +3177,21 @@
       <c r="AM26" s="4"/>
       <c r="AN26" s="4"/>
       <c r="AO26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AP26" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="AP26" s="4" t="s">
+      <c r="AQ26" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="AQ26" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="AR26" s="4"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AU26" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AV26" s="4"/>
       <c r="AW26" s="4"/>
@@ -3207,10 +3212,10 @@
       </c>
       <c r="BZ26" s="4"/>
       <c r="CA26" t="s">
+        <v>185</v>
+      </c>
+      <c r="CB26" t="s">
         <v>186</v>
-      </c>
-      <c r="CB26" t="s">
-        <v>187</v>
       </c>
       <c r="CI26">
         <v>25</v>
@@ -3240,12 +3245,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" t="s">
@@ -3253,10 +3258,10 @@
       </c>
       <c r="R27" s="4"/>
       <c r="S27" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
@@ -3270,7 +3275,7 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
       <c r="AD27" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
@@ -3283,24 +3288,24 @@
       <c r="AM27" s="4"/>
       <c r="AN27" s="4"/>
       <c r="AO27" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP27" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="AP27" s="4" t="s">
-        <v>175</v>
-      </c>
       <c r="AQ27" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AR27" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AS27" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AT27" s="4"/>
       <c r="AU27" s="4"/>
       <c r="AW27" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AX27" s="4"/>
       <c r="AY27" s="4"/>
@@ -3347,21 +3352,21 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q28" t="s">
         <v>145</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AY28" s="4"/>
       <c r="BX28" s="4" t="s">
@@ -3399,9 +3404,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BX29" s="4" t="s">
         <v>154</v>
@@ -3411,7 +3416,7 @@
       </c>
       <c r="BZ29" s="4"/>
       <c r="CH29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="CI29">
         <v>25</v>
@@ -3441,12 +3446,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD30" t="s">
         <v>211</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>212</v>
       </c>
       <c r="BX30" s="4" t="s">
         <v>154</v>
@@ -3483,15 +3488,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BX31" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY31" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BZ31" s="4"/>
       <c r="CI31">
@@ -3519,12 +3524,12 @@
         <v>21</v>
       </c>
       <c r="CQ31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:95" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="BX32" s="4" t="s">
         <v>154</v>
@@ -3558,29 +3563,29 @@
         <v>12</v>
       </c>
       <c r="CQ32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>216</v>
       </c>
+      <c r="AA33" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>224</v>
+      </c>
+      <c r="BU33" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="33" spans="1:73" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="34" spans="1:73" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>217</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>224</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>225</v>
-      </c>
-      <c r="BU33" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="34" spans="1:73" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>218</v>
       </c>
       <c r="C34" s="4"/>
       <c r="F34" s="4"/>
@@ -3605,13 +3610,13 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
       <c r="AA34" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB34" t="s">
         <v>226</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AC34" t="s">
         <v>227</v>
-      </c>
-      <c r="AC34" t="s">
-        <v>228</v>
       </c>
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
@@ -3633,24 +3638,24 @@
       <c r="AU34" s="4"/>
       <c r="AV34" s="4"/>
       <c r="BU34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:73" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA35" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB35" t="s">
         <v>229</v>
       </c>
-      <c r="AB35" t="s">
+      <c r="AC35" t="s">
         <v>230</v>
       </c>
-      <c r="AC35" t="s">
+      <c r="BU35" t="s">
         <v>231</v>
-      </c>
-      <c r="BU35" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Category product Admin Test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{CEFEFB7F-2C56-4740-92AC-1C90D55A0A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3ABA440-1CAA-41DE-8DA1-C45F71B1C10A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F59C33C-6E9F-4988-AA2E-6CCACC5367EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="279">
   <si>
     <t>DataSet</t>
   </si>
@@ -754,12 +754,6 @@
     <t>Test Banner</t>
   </si>
   <si>
-    <t>skatipelli@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Avtuvzwzjogm1!</t>
-  </si>
-  <si>
     <t>ButtonlinkURL</t>
   </si>
   <si>
@@ -830,6 +824,39 @@
   </si>
   <si>
     <t>POP Container Set</t>
+  </si>
+  <si>
+    <t>spanem@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Aonqkziplddf1!</t>
+  </si>
+  <si>
+    <t>32 OZ WIDE MOUTH STAINLESS</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>QATESTING</t>
+  </si>
+  <si>
+    <t>CategoryProducts</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>HYDROFLASK QA TESTING</t>
+  </si>
+  <si>
+    <t>Qa Testing</t>
+  </si>
+  <si>
+    <t>SubTitle</t>
+  </si>
+  <si>
+    <t>TestingHydro</t>
   </si>
 </sst>
 </file>
@@ -1251,128 +1278,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CQ35"/>
+  <dimension ref="A1:CR37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ16" sqref="AJ16"/>
+    <sheetView tabSelected="1" topLeftCell="AU19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7265625" customWidth="1"/>
-    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.453125" customWidth="1"/>
-    <col min="12" max="12" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="30.7265625" customWidth="1"/>
-    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7265625" customWidth="1"/>
-    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.42578125" customWidth="1"/>
+    <col min="12" max="12" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.6328125" customWidth="1"/>
-    <col min="31" max="31" width="17.54296875" customWidth="1"/>
-    <col min="32" max="32" width="14.7265625" customWidth="1"/>
+    <col min="25" max="25" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.5703125" customWidth="1"/>
+    <col min="31" max="31" width="17.5703125" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="21" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.7265625" customWidth="1"/>
-    <col min="41" max="41" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.7265625" customWidth="1"/>
-    <col min="43" max="43" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="17.1796875" customWidth="1"/>
-    <col min="48" max="48" width="45.81640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="60.6328125" customWidth="1"/>
-    <col min="50" max="50" width="26.26953125" customWidth="1"/>
+    <col min="40" max="40" width="15.7109375" customWidth="1"/>
+    <col min="41" max="41" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.7109375" customWidth="1"/>
+    <col min="43" max="43" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="17.140625" customWidth="1"/>
+    <col min="48" max="48" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.5703125" customWidth="1"/>
+    <col min="50" max="50" width="26.28515625" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="11.26953125" customWidth="1"/>
-    <col min="62" max="62" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.28515625" customWidth="1"/>
+    <col min="62" max="62" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.1796875" customWidth="1"/>
-    <col min="68" max="68" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="49.54296875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="13.1796875" customWidth="1"/>
-    <col min="73" max="73" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7265625" customWidth="1"/>
-    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.54296875" customWidth="1"/>
-    <col min="87" max="87" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="146.81640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.140625" customWidth="1"/>
+    <col min="68" max="68" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="13.140625" customWidth="1"/>
+    <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.7109375" customWidth="1"/>
+    <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.5703125" customWidth="1"/>
+    <col min="87" max="87" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="146.85546875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="15" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="12" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="17" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="8" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="14" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="5" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:96" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1473,16 +1500,16 @@
         <v>138</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="AL1" s="3" t="s">
         <v>139</v>
@@ -1509,10 +1536,10 @@
         <v>179</v>
       </c>
       <c r="AT1" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AU1" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>16</v>
@@ -1605,7 +1632,7 @@
         <v>39</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="CA1" s="3" t="s">
         <v>104</v>
@@ -1658,16 +1685,19 @@
       <c r="CQ1" s="17" t="s">
         <v>209</v>
       </c>
+      <c r="CR1" s="17" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1725,7 +1755,7 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1796,7 +1826,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1862,7 +1892,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:96" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1919,7 +1949,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:96" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1977,7 +2007,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2034,7 +2064,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2091,7 +2121,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2142,7 +2172,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2169,7 +2199,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2193,7 +2223,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2250,7 +2280,7 @@
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2275,7 +2305,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2341,7 +2371,7 @@
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2380,7 +2410,7 @@
       </c>
       <c r="BZ15" s="4"/>
     </row>
-    <row r="16" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2388,7 +2418,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2399,7 +2429,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2412,7 +2442,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2510,7 +2540,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>234</v>
       </c>
@@ -2624,7 +2654,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -2702,7 +2732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -2779,7 +2809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -2865,7 +2895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
@@ -2891,7 +2921,7 @@
         <v>149</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="W24" t="s">
         <v>151</v>
@@ -2909,7 +2939,7 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AE24" s="15" t="s">
         <v>157</v>
@@ -2921,19 +2951,19 @@
         <v>158</v>
       </c>
       <c r="AH24" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI24" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ24" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="AI24" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="AJ24" s="18" t="s">
-        <v>254</v>
-      </c>
       <c r="AK24" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AL24" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AM24" s="4">
         <v>3</v>
@@ -2951,10 +2981,10 @@
         <v>162</v>
       </c>
       <c r="AT24" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AU24" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AY24" s="4"/>
       <c r="BB24" t="s">
@@ -2974,7 +3004,7 @@
         <v>103</v>
       </c>
       <c r="BZ24" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="CI24">
         <v>25</v>
@@ -3004,7 +3034,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>183</v>
       </c>
@@ -3025,7 +3055,7 @@
         <v>149</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="W25" t="s">
         <v>151</v>
@@ -3043,7 +3073,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AE25" s="15" t="s">
         <v>157</v>
@@ -3055,19 +3085,19 @@
         <v>194</v>
       </c>
       <c r="AH25" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AI25" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AJ25" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK25" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL25" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="AL25" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="AM25" s="4">
         <v>3</v>
@@ -3085,10 +3115,10 @@
         <v>162</v>
       </c>
       <c r="AT25" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AU25" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AY25" s="4"/>
       <c r="BU25" s="4" t="s">
@@ -3102,7 +3132,7 @@
         <v>163</v>
       </c>
       <c r="BZ25" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="CI25">
         <v>25</v>
@@ -3132,7 +3162,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>184</v>
       </c>
@@ -3188,10 +3218,10 @@
       <c r="AR26" s="4"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AU26" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AV26" s="4"/>
       <c r="AW26" s="4"/>
@@ -3245,7 +3275,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -3352,7 +3382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -3404,7 +3434,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>198</v>
       </c>
@@ -3446,7 +3476,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>210</v>
       </c>
@@ -3488,7 +3518,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>212</v>
       </c>
@@ -3527,7 +3557,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>213</v>
       </c>
@@ -3566,7 +3596,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>216</v>
       </c>
@@ -3583,7 +3613,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>217</v>
       </c>
@@ -3641,7 +3671,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>218</v>
       </c>
@@ -3656,6 +3686,61 @@
       </c>
       <c r="BU35" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>198</v>
+      </c>
+      <c r="U36" t="s">
+        <v>152</v>
+      </c>
+      <c r="V36" t="s">
+        <v>270</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>158</v>
+      </c>
+      <c r="AR36" t="s">
+        <v>271</v>
+      </c>
+      <c r="AW36" t="s">
+        <v>272</v>
+      </c>
+      <c r="AX36" t="s">
+        <v>278</v>
+      </c>
+      <c r="CB36" t="s">
+        <v>194</v>
+      </c>
+      <c r="CG36" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="CH36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>273</v>
+      </c>
+      <c r="U37" t="s">
+        <v>274</v>
+      </c>
+      <c r="AW37" t="s">
+        <v>275</v>
+      </c>
+      <c r="AX37" t="s">
+        <v>276</v>
+      </c>
+      <c r="BX37" t="s">
+        <v>233</v>
+      </c>
+      <c r="CR37" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3691,8 +3776,9 @@
     <hyperlink ref="B5" r:id="rId28" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="BZ25" r:id="rId29" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
     <hyperlink ref="BZ24" r:id="rId30" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
+    <hyperlink ref="CG36" r:id="rId31" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Category product slider admin test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F59C33C-6E9F-4988-AA2E-6CCACC5367EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12C9CC1-2247-4D0C-AAE9-185F74AA6A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView tabSelected="1" topLeftCell="BD19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AY32" sqref="AY32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Admin testcase commit - Promo Block (Color)- testcase, Testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12C9CC1-2247-4D0C-AAE9-185F74AA6A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94DF1F2-8C07-418A-B8C2-FA55AA97501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="281">
   <si>
     <t>DataSet</t>
   </si>
@@ -826,12 +826,6 @@
     <t>POP Container Set</t>
   </si>
   <si>
-    <t>spanem@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Aonqkziplddf1!</t>
-  </si>
-  <si>
     <t>32 OZ WIDE MOUTH STAINLESS</t>
   </si>
   <si>
@@ -857,6 +851,18 @@
   </si>
   <si>
     <t>TestingHydro</t>
+  </si>
+  <si>
+    <t>oxopromocontent</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVEpromocontent1</t>
+  </si>
+  <si>
+    <t>Avtuvzwzjogm1!</t>
+  </si>
+  <si>
+    <t>skatipelli@helenoftroy.com</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR37"/>
+  <dimension ref="A1:CR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AY32" sqref="AY32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1300,7 @@
     <col min="6" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="32.42578125" customWidth="1"/>
-    <col min="12" max="12" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52" customWidth="1"/>
     <col min="13" max="15" width="30.7109375" customWidth="1"/>
     <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="20" width="30.7109375" customWidth="1"/>
@@ -1349,7 +1355,7 @@
     <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="42.85546875" customWidth="1"/>
     <col min="77" max="77" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="54.7109375" customWidth="1"/>
     <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -1686,7 +1692,7 @@
         <v>209</v>
       </c>
       <c r="CR1" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:96" x14ac:dyDescent="0.25">
@@ -1694,10 +1700,10 @@
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -2434,6 +2440,9 @@
         <v>97</v>
       </c>
       <c r="C18" s="4"/>
+      <c r="L18" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="BR18" t="s">
         <v>98</v>
       </c>
@@ -2452,7 +2461,9 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+      <c r="L19" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" t="s">
@@ -2497,12 +2508,14 @@
         <v>102</v>
       </c>
       <c r="BX19" s="5" t="s">
-        <v>233</v>
+        <v>278</v>
       </c>
       <c r="BY19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="BZ19" s="4"/>
+      <c r="BZ19" s="4" t="s">
+        <v>260</v>
+      </c>
       <c r="CA19" s="5" t="s">
         <v>191</v>
       </c>
@@ -2542,7 +2555,7 @@
     </row>
     <row r="20" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>277</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2551,20 +2564,15 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4" t="s">
-        <v>239</v>
+        <v>121</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" t="s">
-        <v>177</v>
-      </c>
       <c r="P20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="Y20" s="4" t="s">
-        <v>153</v>
-      </c>
+      <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
@@ -2573,102 +2581,60 @@
       <c r="AE20" s="15"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
-      <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
-      <c r="AJ20" s="4"/>
-      <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
       <c r="AM20" s="4"/>
       <c r="AN20" s="4"/>
       <c r="AO20" s="4"/>
       <c r="AP20" s="4"/>
       <c r="AQ20" s="4"/>
-      <c r="AR20" t="s">
-        <v>238</v>
-      </c>
       <c r="AV20" s="4"/>
-      <c r="AW20" t="s">
-        <v>241</v>
-      </c>
-      <c r="AX20" t="s">
-        <v>243</v>
-      </c>
       <c r="AY20" s="4"/>
       <c r="BR20" s="1"/>
-      <c r="BS20" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="BT20" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="BU20" t="s">
-        <v>100</v>
-      </c>
-      <c r="BV20" t="s">
-        <v>101</v>
-      </c>
-      <c r="BW20" t="s">
-        <v>102</v>
-      </c>
+      <c r="BS20" s="1"/>
+      <c r="BT20" s="1"/>
       <c r="BX20" s="5" t="s">
-        <v>233</v>
+        <v>278</v>
       </c>
       <c r="BY20" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ20" s="4"/>
-      <c r="CA20" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="CB20" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="CC20" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="CI20">
-        <v>25</v>
-      </c>
-      <c r="CJ20">
-        <v>27</v>
-      </c>
-      <c r="CK20">
-        <v>15</v>
-      </c>
-      <c r="CL20">
-        <v>10</v>
-      </c>
-      <c r="CM20">
-        <v>30</v>
-      </c>
-      <c r="CN20">
-        <v>35</v>
-      </c>
-      <c r="CO20">
-        <v>32</v>
-      </c>
-      <c r="CP20">
-        <v>23</v>
-      </c>
-      <c r="CQ20" t="s">
-        <v>77</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="BZ20" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="CA20" s="5"/>
+      <c r="CB20" s="5"/>
+      <c r="CC20" s="5"/>
     </row>
     <row r="21" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" t="s">
+        <v>177</v>
+      </c>
+      <c r="P21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-      <c r="Y21" s="5" t="s">
-        <v>39</v>
+      <c r="Y21" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
-      <c r="AD21" s="15"/>
+      <c r="AD21" s="4"/>
       <c r="AE21" s="15"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
@@ -2682,30 +2648,48 @@
       <c r="AO21" s="4"/>
       <c r="AP21" s="4"/>
       <c r="AQ21" s="4"/>
-      <c r="BN21" s="6"/>
-      <c r="BO21" s="6"/>
-      <c r="BP21" s="7"/>
-      <c r="BQ21" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="BX21" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BY21" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="BZ21" s="14"/>
-      <c r="CA21" t="s">
+      <c r="AR21" t="s">
+        <v>238</v>
+      </c>
+      <c r="AV21" s="4"/>
+      <c r="AW21" t="s">
+        <v>241</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>243</v>
+      </c>
+      <c r="AY21" s="4"/>
+      <c r="BR21" s="1"/>
+      <c r="BS21" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="BT21" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="BU21" t="s">
+        <v>100</v>
+      </c>
+      <c r="BV21" t="s">
+        <v>101</v>
+      </c>
+      <c r="BW21" t="s">
+        <v>102</v>
+      </c>
+      <c r="BX21" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="BY21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BZ21" s="4"/>
+      <c r="CA21" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="CB21" t="s">
-        <v>194</v>
-      </c>
-      <c r="CD21" t="s">
-        <v>115</v>
-      </c>
-      <c r="CE21" t="s">
-        <v>39</v>
+      <c r="CB21" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="CC21" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="CI21">
         <v>25</v>
@@ -2730,37 +2714,27 @@
       </c>
       <c r="CP21">
         <v>23</v>
+      </c>
+      <c r="CQ21" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="S22" s="4"/>
+        <v>117</v>
+      </c>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
+      <c r="Y22" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
-      <c r="AE22" s="4"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
       <c r="AH22" s="4"/>
@@ -2773,16 +2747,30 @@
       <c r="AO22" s="4"/>
       <c r="AP22" s="4"/>
       <c r="AQ22" s="4"/>
-      <c r="AR22" s="4"/>
-      <c r="AS22" s="4"/>
-      <c r="AT22" s="4"/>
-      <c r="AU22" s="4"/>
-      <c r="AV22" s="4"/>
-      <c r="AW22" t="s">
-        <v>196</v>
+      <c r="BN22" s="6"/>
+      <c r="BO22" s="6"/>
+      <c r="BP22" s="7"/>
+      <c r="BQ22" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="BX22" s="4" t="s">
         <v>154</v>
+      </c>
+      <c r="BY22" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="BZ22" s="14"/>
+      <c r="CA22" t="s">
+        <v>191</v>
+      </c>
+      <c r="CB22" t="s">
+        <v>194</v>
+      </c>
+      <c r="CD22" t="s">
+        <v>115</v>
+      </c>
+      <c r="CE22" t="s">
+        <v>39</v>
       </c>
       <c r="CI22">
         <v>25</v>
@@ -2811,7 +2799,7 @@
     </row>
     <row r="23" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2819,12 +2807,13 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="L23" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
@@ -2836,7 +2825,6 @@
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
-      <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
@@ -2855,20 +2843,14 @@
       <c r="AT23" s="4"/>
       <c r="AU23" s="4"/>
       <c r="AV23" s="4"/>
-      <c r="BN23" s="9"/>
-      <c r="BO23" s="9"/>
-      <c r="BX23" s="5" t="s">
-        <v>233</v>
+      <c r="AW23" t="s">
+        <v>196</v>
+      </c>
+      <c r="BX23" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="BY23" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ23" s="14"/>
-      <c r="CF23" t="s">
-        <v>197</v>
-      </c>
-      <c r="CG23" s="14" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="CI23">
         <v>25</v>
@@ -2897,114 +2879,64 @@
     </row>
     <row r="24" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>182</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="O24" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>145</v>
-      </c>
-      <c r="R24" t="s">
-        <v>146</v>
-      </c>
-      <c r="S24" t="s">
-        <v>147</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="U24" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="V24" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W24" t="s">
-        <v>151</v>
-      </c>
-      <c r="X24" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y24" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z24" s="4" t="s">
-        <v>155</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
-      <c r="AD24" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE24" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF24" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG24" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH24" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="AI24" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="AJ24" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="AK24" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="AL24" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="AM24" s="4">
-        <v>3</v>
-      </c>
-      <c r="AN24" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO24" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AP24" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AQ24" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AT24" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AU24" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="AY24" s="4"/>
-      <c r="BB24" t="s">
-        <v>177</v>
-      </c>
-      <c r="BQ24" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="BU24" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="BW24" s="6"/>
-      <c r="BX24" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BY24" s="4" t="s">
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+      <c r="AG24" s="4"/>
+      <c r="AH24" s="4"/>
+      <c r="AI24" s="4"/>
+      <c r="AJ24" s="4"/>
+      <c r="AK24" s="4"/>
+      <c r="AL24" s="4"/>
+      <c r="AM24" s="4"/>
+      <c r="AN24" s="4"/>
+      <c r="AO24" s="4"/>
+      <c r="AP24" s="4"/>
+      <c r="AQ24" s="4"/>
+      <c r="AR24" s="4"/>
+      <c r="AS24" s="4"/>
+      <c r="AT24" s="4"/>
+      <c r="AU24" s="4"/>
+      <c r="AV24" s="4"/>
+      <c r="BN24" s="9"/>
+      <c r="BO24" s="9"/>
+      <c r="BX24" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="BY24" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="BZ24" s="4" t="s">
-        <v>260</v>
+      <c r="BZ24" s="14"/>
+      <c r="CF24" t="s">
+        <v>197</v>
+      </c>
+      <c r="CG24" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="CI24">
         <v>25</v>
@@ -3029,16 +2961,18 @@
       </c>
       <c r="CP24">
         <v>23</v>
-      </c>
-      <c r="CQ24" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>183</v>
-      </c>
-      <c r="L25" s="4"/>
+        <v>182</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="O25" t="s">
+        <v>177</v>
+      </c>
       <c r="Q25" t="s">
         <v>145</v>
       </c>
@@ -3055,7 +2989,7 @@
         <v>149</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W25" t="s">
         <v>151</v>
@@ -3073,7 +3007,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AE25" s="15" t="s">
         <v>157</v>
@@ -3082,22 +3016,22 @@
         <v>115</v>
       </c>
       <c r="AG25" s="4" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="AH25" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AI25" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="AJ25" s="4" t="s">
-        <v>267</v>
+        <v>251</v>
+      </c>
+      <c r="AJ25" s="18" t="s">
+        <v>252</v>
       </c>
       <c r="AK25" s="4" t="s">
         <v>264</v>
       </c>
       <c r="AL25" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AM25" s="4">
         <v>3</v>
@@ -3121,18 +3055,24 @@
         <v>256</v>
       </c>
       <c r="AY25" s="4"/>
+      <c r="BB25" t="s">
+        <v>177</v>
+      </c>
+      <c r="BQ25" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="BU25" s="4" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="BW25" s="6"/>
       <c r="BX25" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY25" s="4" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="BZ25" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CI25">
         <v>25</v>
@@ -3164,26 +3104,33 @@
     </row>
     <row r="26" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L26" s="4"/>
-      <c r="P26" s="4"/>
       <c r="Q26" t="s">
         <v>145</v>
       </c>
       <c r="R26" t="s">
         <v>146</v>
       </c>
-      <c r="S26" s="4" t="s">
-        <v>165</v>
+      <c r="S26" t="s">
+        <v>147</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="V26" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="W26" t="s">
+        <v>151</v>
+      </c>
+      <c r="X26" t="s">
+        <v>152</v>
+      </c>
       <c r="Y26" s="4" t="s">
         <v>153</v>
       </c>
@@ -3193,59 +3140,67 @@
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-      <c r="AD26" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE26" s="4"/>
-      <c r="AF26" s="4"/>
-      <c r="AG26" s="4"/>
-      <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
-      <c r="AJ26" s="4"/>
-      <c r="AK26" s="4"/>
-      <c r="AL26" s="4"/>
-      <c r="AM26" s="4"/>
-      <c r="AN26" s="4"/>
+      <c r="AD26" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE26" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF26" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG26" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="AH26" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AI26" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ26" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="AK26" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL26" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="AM26" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN26" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="AO26" s="4" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="AP26" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="AQ26" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AR26" s="4"/>
-      <c r="AS26" s="4"/>
+        <v>162</v>
+      </c>
       <c r="AT26" s="4" t="s">
         <v>255</v>
       </c>
       <c r="AU26" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="AV26" s="4"/>
-      <c r="AW26" s="4"/>
-      <c r="AX26" s="4"/>
       <c r="AY26" s="4"/>
-      <c r="AZ26" s="4"/>
-      <c r="BA26" s="4"/>
-      <c r="BB26" s="4"/>
-      <c r="BC26" s="4"/>
-      <c r="BD26" s="4"/>
-      <c r="BE26" s="4"/>
-      <c r="BF26" s="4"/>
+      <c r="BU26" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="BW26" s="6"/>
       <c r="BX26" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ26" s="4"/>
-      <c r="CA26" t="s">
-        <v>185</v>
-      </c>
-      <c r="CB26" t="s">
-        <v>186</v>
+        <v>163</v>
+      </c>
+      <c r="BZ26" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="CI26">
         <v>25</v>
@@ -3277,35 +3232,37 @@
     </row>
     <row r="27" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>187</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>176</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="L27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" t="s">
         <v>145</v>
       </c>
-      <c r="R27" s="4"/>
+      <c r="R27" t="s">
+        <v>146</v>
+      </c>
       <c r="S27" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
+      <c r="Y27" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="Z27" s="4" t="s">
         <v>155</v>
       </c>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
-      <c r="AD27" s="4" t="s">
-        <v>172</v>
+      <c r="AD27" t="s">
+        <v>167</v>
       </c>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
@@ -3318,25 +3275,24 @@
       <c r="AM27" s="4"/>
       <c r="AN27" s="4"/>
       <c r="AO27" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AP27" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="AQ27" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AR27" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AS27" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AT27" s="4"/>
-      <c r="AU27" s="4"/>
-      <c r="AW27" s="4" t="s">
-        <v>181</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="AR27" s="4"/>
+      <c r="AS27" s="4"/>
+      <c r="AT27" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AU27" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="AV27" s="4"/>
+      <c r="AW27" s="4"/>
       <c r="AX27" s="4"/>
       <c r="AY27" s="4"/>
       <c r="AZ27" s="4"/>
@@ -3346,7 +3302,6 @@
       <c r="BD27" s="4"/>
       <c r="BE27" s="4"/>
       <c r="BF27" s="4"/>
-      <c r="BW27" s="9"/>
       <c r="BX27" s="4" t="s">
         <v>154</v>
       </c>
@@ -3354,6 +3309,12 @@
         <v>103</v>
       </c>
       <c r="BZ27" s="4"/>
+      <c r="CA27" t="s">
+        <v>185</v>
+      </c>
+      <c r="CB27" t="s">
+        <v>186</v>
+      </c>
       <c r="CI27">
         <v>25</v>
       </c>
@@ -3384,21 +3345,76 @@
     </row>
     <row r="28" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>176</v>
       </c>
+      <c r="P28" s="4"/>
       <c r="Q28" t="s">
         <v>145</v>
       </c>
+      <c r="R28" s="4"/>
       <c r="S28" s="4" t="s">
         <v>171</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>171</v>
       </c>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="4"/>
+      <c r="AI28" s="4"/>
+      <c r="AJ28" s="4"/>
+      <c r="AK28" s="4"/>
+      <c r="AL28" s="4"/>
+      <c r="AM28" s="4"/>
+      <c r="AN28" s="4"/>
+      <c r="AO28" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP28" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AQ28" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AR28" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AS28" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AT28" s="4"/>
+      <c r="AU28" s="4"/>
+      <c r="AW28" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX28" s="4"/>
       <c r="AY28" s="4"/>
+      <c r="AZ28" s="4"/>
+      <c r="BA28" s="4"/>
+      <c r="BB28" s="4"/>
+      <c r="BC28" s="4"/>
+      <c r="BD28" s="4"/>
+      <c r="BE28" s="4"/>
+      <c r="BF28" s="4"/>
+      <c r="BW28" s="9"/>
       <c r="BX28" s="4" t="s">
         <v>154</v>
       </c>
@@ -3436,8 +3452,21 @@
     </row>
     <row r="29" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>198</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>145</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AY29" s="4"/>
       <c r="BX29" s="4" t="s">
         <v>154</v>
       </c>
@@ -3445,9 +3474,6 @@
         <v>103</v>
       </c>
       <c r="BZ29" s="4"/>
-      <c r="CH29" t="s">
-        <v>200</v>
-      </c>
       <c r="CI29">
         <v>25</v>
       </c>
@@ -3478,10 +3504,7 @@
     </row>
     <row r="30" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>210</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="BX30" s="4" t="s">
         <v>154</v>
@@ -3490,6 +3513,9 @@
         <v>103</v>
       </c>
       <c r="BZ30" s="4"/>
+      <c r="CH30" t="s">
+        <v>200</v>
+      </c>
       <c r="CI30">
         <v>25</v>
       </c>
@@ -3520,252 +3546,294 @@
     </row>
     <row r="31" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>212</v>
+        <v>210</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>211</v>
       </c>
       <c r="BX31" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY31" s="4" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="BZ31" s="4"/>
       <c r="CI31">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="CJ31">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="CK31">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="CL31">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="CM31">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="CN31">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="CO31">
         <v>32</v>
       </c>
       <c r="CP31">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="CQ31" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BX32" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY32" s="4" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="BZ32" s="4"/>
       <c r="CI32">
+        <v>12</v>
+      </c>
+      <c r="CJ32">
         <v>32</v>
       </c>
-      <c r="CJ32">
-        <v>34</v>
-      </c>
       <c r="CK32">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="CL32">
+        <v>12</v>
+      </c>
+      <c r="CM32">
+        <v>23</v>
+      </c>
+      <c r="CN32">
+        <v>20</v>
+      </c>
+      <c r="CO32">
+        <v>32</v>
+      </c>
+      <c r="CP32">
         <v>21</v>
       </c>
-      <c r="CM32">
-        <v>13</v>
-      </c>
-      <c r="CN32">
-        <v>5</v>
-      </c>
-      <c r="CO32">
-        <v>2</v>
-      </c>
-      <c r="CP32">
-        <v>12</v>
-      </c>
       <c r="CQ32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>216</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>222</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>223</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>224</v>
-      </c>
-      <c r="BU33" t="s">
-        <v>231</v>
+        <v>213</v>
+      </c>
+      <c r="BX33" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY33" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BZ33" s="4"/>
+      <c r="CI33">
+        <v>32</v>
+      </c>
+      <c r="CJ33">
+        <v>34</v>
+      </c>
+      <c r="CK33">
+        <v>54</v>
+      </c>
+      <c r="CL33">
+        <v>21</v>
+      </c>
+      <c r="CM33">
+        <v>13</v>
+      </c>
+      <c r="CN33">
+        <v>5</v>
+      </c>
+      <c r="CO33">
+        <v>2</v>
+      </c>
+      <c r="CP33">
+        <v>12</v>
+      </c>
+      <c r="CQ33" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
+        <v>216</v>
+      </c>
       <c r="AA34" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AB34" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AC34" t="s">
-        <v>227</v>
-      </c>
-      <c r="AD34" s="4"/>
-      <c r="AE34" s="4"/>
-      <c r="AF34" s="4"/>
-      <c r="AG34" s="4"/>
-      <c r="AH34" s="4"/>
-      <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="4"/>
-      <c r="AL34" s="4"/>
-      <c r="AM34" s="4"/>
-      <c r="AN34" s="4"/>
-      <c r="AO34" s="4"/>
-      <c r="AP34" s="4"/>
-      <c r="AQ34" s="4"/>
-      <c r="AR34" s="4"/>
-      <c r="AS34" s="4"/>
-      <c r="AT34" s="4"/>
-      <c r="AU34" s="4"/>
-      <c r="AV34" s="4"/>
+        <v>224</v>
+      </c>
       <c r="BU34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>218</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
       <c r="AA35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="AB35" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="AC35" t="s">
-        <v>230</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="4"/>
+      <c r="AI35" s="4"/>
+      <c r="AJ35" s="4"/>
+      <c r="AK35" s="4"/>
+      <c r="AL35" s="4"/>
+      <c r="AM35" s="4"/>
+      <c r="AN35" s="4"/>
+      <c r="AO35" s="4"/>
+      <c r="AP35" s="4"/>
+      <c r="AQ35" s="4"/>
+      <c r="AR35" s="4"/>
+      <c r="AS35" s="4"/>
+      <c r="AT35" s="4"/>
+      <c r="AU35" s="4"/>
+      <c r="AV35" s="4"/>
       <c r="BU35" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>198</v>
-      </c>
-      <c r="U36" t="s">
-        <v>152</v>
-      </c>
-      <c r="V36" t="s">
-        <v>270</v>
-      </c>
-      <c r="AE36" t="s">
-        <v>197</v>
-      </c>
-      <c r="AG36" t="s">
-        <v>158</v>
-      </c>
-      <c r="AR36" t="s">
-        <v>271</v>
-      </c>
-      <c r="AW36" t="s">
-        <v>272</v>
-      </c>
-      <c r="AX36" t="s">
-        <v>278</v>
-      </c>
-      <c r="CB36" t="s">
-        <v>194</v>
-      </c>
-      <c r="CG36" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="CH36" t="s">
-        <v>200</v>
+        <v>218</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>230</v>
+      </c>
+      <c r="BU36" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>273</v>
+        <v>198</v>
       </c>
       <c r="U37" t="s">
-        <v>274</v>
+        <v>152</v>
+      </c>
+      <c r="V37" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>158</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>269</v>
       </c>
       <c r="AW37" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AX37" t="s">
         <v>276</v>
       </c>
-      <c r="BX37" t="s">
+      <c r="CB37" t="s">
+        <v>194</v>
+      </c>
+      <c r="CG37" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="CH37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>271</v>
+      </c>
+      <c r="U38" t="s">
+        <v>272</v>
+      </c>
+      <c r="AW38" t="s">
+        <v>273</v>
+      </c>
+      <c r="AX38" t="s">
+        <v>274</v>
+      </c>
+      <c r="BX38" t="s">
         <v>233</v>
       </c>
-      <c r="CR37" t="s">
-        <v>276</v>
+      <c r="CR38" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="BY29:BY32" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
-    <hyperlink ref="AH25" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
-    <hyperlink ref="AH24" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
+    <hyperlink ref="BY30:BY33" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="AH26" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
+    <hyperlink ref="AH25" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
     <hyperlink ref="B2" r:id="rId4" xr:uid="{C530F640-5A3A-45E7-800F-3A1EC68A3189}"/>
-    <hyperlink ref="Y20" r:id="rId5" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
-    <hyperlink ref="BY20" r:id="rId6" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
-    <hyperlink ref="BY31" r:id="rId7" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="BY28:BY30" r:id="rId8" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
-    <hyperlink ref="CG23" r:id="rId9" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="Y21" r:id="rId5" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
+    <hyperlink ref="BY21" r:id="rId6" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
+    <hyperlink ref="BY32" r:id="rId7" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="BY29:BY31" r:id="rId8" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="CG24" r:id="rId9" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
     <hyperlink ref="Y19" r:id="rId10" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BY25" r:id="rId11" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
-    <hyperlink ref="BY27" r:id="rId12" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BY26" r:id="rId13" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BY24" r:id="rId14" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="BY26" r:id="rId11" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BY28" r:id="rId12" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BY27" r:id="rId13" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BY25" r:id="rId14" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
     <hyperlink ref="B3" r:id="rId15" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="Y25" r:id="rId16" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
-    <hyperlink ref="Y26" r:id="rId17" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
-    <hyperlink ref="Y24" r:id="rId18" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
-    <hyperlink ref="BY23" r:id="rId19" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="BY21" r:id="rId20" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="Y26" r:id="rId16" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="Y27" r:id="rId17" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y25" r:id="rId18" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="BY24" r:id="rId19" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="BY22" r:id="rId20" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
     <hyperlink ref="BY15" r:id="rId21" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
     <hyperlink ref="BY19" r:id="rId22" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
     <hyperlink ref="F14" r:id="rId23" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
@@ -3774,11 +3842,14 @@
     <hyperlink ref="F5" r:id="rId26" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
     <hyperlink ref="F6" r:id="rId27" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="B5" r:id="rId28" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="BZ25" r:id="rId29" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
-    <hyperlink ref="BZ24" r:id="rId30" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
-    <hyperlink ref="CG36" r:id="rId31" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
+    <hyperlink ref="BZ26" r:id="rId29" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
+    <hyperlink ref="BZ25" r:id="rId30" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
+    <hyperlink ref="CG37" r:id="rId31" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
+    <hyperlink ref="BY23" r:id="rId32" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
+    <hyperlink ref="BZ20" r:id="rId33" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
+    <hyperlink ref="BY20" r:id="rId34" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the code to ran in preprod
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94DF1F2-8C07-418A-B8C2-FA55AA97501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{B94DF1F2-8C07-418A-B8C2-FA55AA97501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FB74BA2-03DB-4C7E-A47B-4BAB3F25452D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="279">
   <si>
     <t>DataSet</t>
   </si>
@@ -857,12 +857,6 @@
   </si>
   <si>
     <t>QATESTINGLOTUSWAVEpromocontent1</t>
-  </si>
-  <si>
-    <t>Avtuvzwzjogm1!</t>
-  </si>
-  <si>
-    <t>skatipelli@helenoftroy.com</t>
   </si>
 </sst>
 </file>
@@ -1287,125 +1281,125 @@
   <dimension ref="A1:CR38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7265625" customWidth="1"/>
+    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.453125" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
-    <col min="13" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7265625" customWidth="1"/>
+    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7265625" customWidth="1"/>
+    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.5703125" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.54296875" customWidth="1"/>
+    <col min="31" max="31" width="17.54296875" customWidth="1"/>
+    <col min="32" max="32" width="14.7265625" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="21" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.7109375" customWidth="1"/>
-    <col min="41" max="41" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.7109375" customWidth="1"/>
-    <col min="43" max="43" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="17.140625" customWidth="1"/>
-    <col min="48" max="48" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="60.5703125" customWidth="1"/>
-    <col min="50" max="50" width="26.28515625" customWidth="1"/>
+    <col min="40" max="40" width="15.7265625" customWidth="1"/>
+    <col min="41" max="41" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.7265625" customWidth="1"/>
+    <col min="43" max="43" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="17.1796875" customWidth="1"/>
+    <col min="48" max="48" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.54296875" customWidth="1"/>
+    <col min="50" max="50" width="26.26953125" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="11.28515625" customWidth="1"/>
-    <col min="62" max="62" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.26953125" customWidth="1"/>
+    <col min="62" max="62" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.140625" customWidth="1"/>
-    <col min="68" max="68" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="13.140625" customWidth="1"/>
-    <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="42.85546875" customWidth="1"/>
-    <col min="77" max="77" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7109375" customWidth="1"/>
-    <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.5703125" customWidth="1"/>
-    <col min="87" max="87" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="146.85546875" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.1796875" customWidth="1"/>
+    <col min="68" max="68" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="13.1796875" customWidth="1"/>
+    <col min="73" max="73" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="42.81640625" customWidth="1"/>
+    <col min="77" max="77" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.7265625" customWidth="1"/>
+    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.54296875" customWidth="1"/>
+    <col min="87" max="87" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="146.81640625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="15" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="12" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="17" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="8" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="14" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="5" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:96" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1695,15 +1689,15 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>280</v>
+        <v>189</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>279</v>
+        <v>190</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1761,7 +1755,7 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1832,7 +1826,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1898,7 +1892,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:96" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:96" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1955,7 +1949,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:96" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:96" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2013,7 +2007,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2070,7 +2064,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2127,7 +2121,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2178,7 +2172,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2205,7 +2199,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2229,7 +2223,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2286,7 +2280,7 @@
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:96" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2311,7 +2305,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2377,7 +2371,7 @@
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2416,7 +2410,7 @@
       </c>
       <c r="BZ15" s="4"/>
     </row>
-    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2424,7 +2418,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2435,7 +2429,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2451,7 +2445,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2553,7 +2547,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>277</v>
       </c>
@@ -2605,7 +2599,7 @@
       <c r="CB20" s="5"/>
       <c r="CC20" s="5"/>
     </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>234</v>
       </c>
@@ -2719,7 +2713,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2797,7 +2791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -2877,7 +2871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -2963,7 +2957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -3102,7 +3096,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>183</v>
       </c>
@@ -3230,7 +3224,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>184</v>
       </c>
@@ -3343,7 +3337,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>187</v>
       </c>
@@ -3450,7 +3444,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>188</v>
       </c>
@@ -3502,7 +3496,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>198</v>
       </c>
@@ -3544,7 +3538,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>210</v>
       </c>
@@ -3586,7 +3580,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>212</v>
       </c>
@@ -3625,7 +3619,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>213</v>
       </c>
@@ -3664,7 +3658,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>216</v>
       </c>
@@ -3681,7 +3675,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>217</v>
       </c>
@@ -3739,7 +3733,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>218</v>
       </c>
@@ -3756,7 +3750,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>198</v>
       </c>
@@ -3791,7 +3785,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>271</v>
       </c>
@@ -3817,37 +3811,37 @@
     <hyperlink ref="BY30:BY33" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
     <hyperlink ref="AH26" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
     <hyperlink ref="AH25" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{C530F640-5A3A-45E7-800F-3A1EC68A3189}"/>
-    <hyperlink ref="Y21" r:id="rId5" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
-    <hyperlink ref="BY21" r:id="rId6" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
-    <hyperlink ref="BY32" r:id="rId7" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="BY29:BY31" r:id="rId8" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
-    <hyperlink ref="CG24" r:id="rId9" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
-    <hyperlink ref="Y19" r:id="rId10" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BY26" r:id="rId11" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
-    <hyperlink ref="BY28" r:id="rId12" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BY27" r:id="rId13" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BY25" r:id="rId14" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
-    <hyperlink ref="B3" r:id="rId15" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="Y26" r:id="rId16" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
-    <hyperlink ref="Y27" r:id="rId17" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
-    <hyperlink ref="Y25" r:id="rId18" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
-    <hyperlink ref="BY24" r:id="rId19" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="BY22" r:id="rId20" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
-    <hyperlink ref="BY15" r:id="rId21" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="BY19" r:id="rId22" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="F14" r:id="rId23" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
-    <hyperlink ref="B4" r:id="rId24" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="C4" r:id="rId25" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
-    <hyperlink ref="F5" r:id="rId26" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="F6" r:id="rId27" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="B5" r:id="rId28" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="BZ26" r:id="rId29" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
-    <hyperlink ref="BZ25" r:id="rId30" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
-    <hyperlink ref="CG37" r:id="rId31" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
-    <hyperlink ref="BY23" r:id="rId32" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
-    <hyperlink ref="BZ20" r:id="rId33" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
-    <hyperlink ref="BY20" r:id="rId34" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
+    <hyperlink ref="Y21" r:id="rId4" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
+    <hyperlink ref="BY21" r:id="rId5" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
+    <hyperlink ref="BY32" r:id="rId6" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="BY29:BY31" r:id="rId7" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="CG24" r:id="rId8" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="Y19" r:id="rId9" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
+    <hyperlink ref="BY26" r:id="rId10" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BY28" r:id="rId11" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BY27" r:id="rId12" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BY25" r:id="rId13" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
+    <hyperlink ref="Y26" r:id="rId15" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="Y27" r:id="rId16" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y25" r:id="rId17" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="BY24" r:id="rId18" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="BY22" r:id="rId19" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="BY15" r:id="rId20" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="BY19" r:id="rId21" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="F14" r:id="rId22" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
+    <hyperlink ref="B4" r:id="rId23" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
+    <hyperlink ref="C4" r:id="rId24" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="F5" r:id="rId25" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="F6" r:id="rId26" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="B5" r:id="rId27" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
+    <hyperlink ref="BZ26" r:id="rId28" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
+    <hyperlink ref="BZ25" r:id="rId29" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
+    <hyperlink ref="CG37" r:id="rId30" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
+    <hyperlink ref="BY23" r:id="rId31" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
+    <hyperlink ref="BZ20" r:id="rId32" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
+    <hyperlink ref="BY20" r:id="rId33" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
+    <hyperlink ref="B2" r:id="rId34" xr:uid="{A45A2FC1-0756-4996-B77E-C3738CB0981D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId35"/>

</xml_diff>

<commit_message>
Testimonial Admin test case for Hydroflask
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{B94DF1F2-8C07-418A-B8C2-FA55AA97501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FB74BA2-03DB-4C7E-A47B-4BAB3F25452D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F633C7-C61E-4B23-9340-430D007632B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="285">
   <si>
     <t>DataSet</t>
   </si>
@@ -857,6 +857,24 @@
   </si>
   <si>
     <t>QATESTINGLOTUSWAVEpromocontent1</t>
+  </si>
+  <si>
+    <t>TestmonialProductcard</t>
+  </si>
+  <si>
+    <t>#21ffff</t>
+  </si>
+  <si>
+    <t>Qatester</t>
+  </si>
+  <si>
+    <t>QaTester</t>
+  </si>
+  <si>
+    <t>spanem@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Aonqkziplddf1!</t>
   </si>
 </sst>
 </file>
@@ -1278,128 +1296,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR38"/>
+  <dimension ref="A1:CT39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7265625" customWidth="1"/>
-    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.77734375" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.44140625" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
-    <col min="13" max="15" width="30.7265625" customWidth="1"/>
-    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7265625" customWidth="1"/>
-    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.77734375" customWidth="1"/>
+    <col min="16" max="16" width="89.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.77734375" customWidth="1"/>
+    <col min="21" max="21" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.5546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.54296875" customWidth="1"/>
-    <col min="31" max="31" width="17.54296875" customWidth="1"/>
-    <col min="32" max="32" width="14.7265625" customWidth="1"/>
+    <col min="25" max="25" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.5546875" customWidth="1"/>
+    <col min="31" max="31" width="17.5546875" customWidth="1"/>
+    <col min="32" max="32" width="14.77734375" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="21" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="37.5546875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.7265625" customWidth="1"/>
-    <col min="41" max="41" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.7265625" customWidth="1"/>
-    <col min="43" max="43" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="17.1796875" customWidth="1"/>
-    <col min="48" max="48" width="45.81640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="60.54296875" customWidth="1"/>
-    <col min="50" max="50" width="26.26953125" customWidth="1"/>
+    <col min="40" max="40" width="15.77734375" customWidth="1"/>
+    <col min="41" max="41" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.77734375" customWidth="1"/>
+    <col min="43" max="43" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="17.21875" customWidth="1"/>
+    <col min="48" max="48" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.5546875" customWidth="1"/>
+    <col min="50" max="50" width="26.21875" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="11.26953125" customWidth="1"/>
-    <col min="62" max="62" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.21875" customWidth="1"/>
+    <col min="62" max="62" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.1796875" customWidth="1"/>
-    <col min="68" max="68" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="49.54296875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="13.1796875" customWidth="1"/>
-    <col min="73" max="73" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="42.81640625" customWidth="1"/>
-    <col min="77" max="77" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7265625" customWidth="1"/>
-    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.54296875" customWidth="1"/>
-    <col min="87" max="87" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="146.81640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="15" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="12" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="17" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="8" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="14" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="5" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.21875" customWidth="1"/>
+    <col min="68" max="68" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="13.21875" customWidth="1"/>
+    <col min="73" max="73" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="42.77734375" customWidth="1"/>
+    <col min="77" max="77" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.77734375" customWidth="1"/>
+    <col min="79" max="79" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.5546875" customWidth="1"/>
+    <col min="87" max="87" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="35.44140625" customWidth="1"/>
+    <col min="98" max="98" width="146.77734375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="15" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="17" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="8" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="14" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="5" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:98" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1686,18 +1705,24 @@
         <v>209</v>
       </c>
       <c r="CR1" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="CS1" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="CT1" s="17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>189</v>
+        <v>283</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>190</v>
+        <v>284</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1755,7 +1780,7 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1826,7 +1851,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1892,7 +1917,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:96" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:98" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1949,7 +1974,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:96" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2007,7 +2032,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2064,7 +2089,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2121,7 +2146,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2172,7 +2197,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2199,7 +2224,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2223,7 +2248,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2280,7 +2305,7 @@
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:96" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2305,7 +2330,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2371,7 +2396,7 @@
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2410,7 +2435,7 @@
       </c>
       <c r="BZ15" s="4"/>
     </row>
-    <row r="16" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2418,7 +2443,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2429,7 +2454,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2445,7 +2470,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2547,7 +2572,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>277</v>
       </c>
@@ -2599,7 +2624,7 @@
       <c r="CB20" s="5"/>
       <c r="CC20" s="5"/>
     </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>234</v>
       </c>
@@ -2713,7 +2738,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2791,7 +2816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -2871,7 +2896,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -2957,7 +2982,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -3096,105 +3121,51 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>279</v>
       </c>
       <c r="L26" s="4"/>
-      <c r="Q26" t="s">
-        <v>145</v>
-      </c>
-      <c r="R26" t="s">
-        <v>146</v>
-      </c>
-      <c r="S26" t="s">
-        <v>147</v>
-      </c>
-      <c r="T26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="U26" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="V26" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="W26" t="s">
-        <v>151</v>
-      </c>
-      <c r="X26" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y26" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z26" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-      <c r="AD26" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="AE26" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF26" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG26" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="AH26" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="AI26" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="AJ26" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="AK26" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="AL26" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="AM26" s="4">
-        <v>3</v>
-      </c>
-      <c r="AN26" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO26" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AP26" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AQ26" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AT26" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AU26" s="4" t="s">
-        <v>256</v>
-      </c>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="15"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="18"/>
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="4"/>
+      <c r="AN26" s="4"/>
+      <c r="AO26" s="4"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="4"/>
+      <c r="AT26" s="4"/>
+      <c r="AU26" s="4"/>
       <c r="AY26" s="4"/>
+      <c r="BQ26" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="BU26" s="4" t="s">
-        <v>164</v>
+        <v>280</v>
       </c>
       <c r="BW26" s="6"/>
       <c r="BX26" s="4" t="s">
-        <v>154</v>
+        <v>281</v>
       </c>
       <c r="BY26" s="4" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="BZ26" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CI26">
         <v>25</v>
@@ -3223,29 +3194,42 @@
       <c r="CQ26" t="s">
         <v>77</v>
       </c>
+      <c r="CR26" t="s">
+        <v>282</v>
+      </c>
+      <c r="CS26" t="s">
+        <v>281</v>
+      </c>
     </row>
-    <row r="27" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L27" s="4"/>
-      <c r="P27" s="4"/>
       <c r="Q27" t="s">
         <v>145</v>
       </c>
       <c r="R27" t="s">
         <v>146</v>
       </c>
-      <c r="S27" s="4" t="s">
-        <v>165</v>
+      <c r="S27" t="s">
+        <v>147</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="U27" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="V27" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="W27" t="s">
+        <v>151</v>
+      </c>
+      <c r="X27" t="s">
+        <v>152</v>
+      </c>
       <c r="Y27" s="4" t="s">
         <v>153</v>
       </c>
@@ -3255,59 +3239,67 @@
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
-      <c r="AD27" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
-      <c r="AG27" s="4"/>
-      <c r="AH27" s="4"/>
-      <c r="AI27" s="4"/>
-      <c r="AJ27" s="4"/>
-      <c r="AK27" s="4"/>
-      <c r="AL27" s="4"/>
-      <c r="AM27" s="4"/>
-      <c r="AN27" s="4"/>
+      <c r="AD27" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE27" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG27" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="AH27" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AI27" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ27" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="AK27" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL27" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="AM27" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN27" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="AO27" s="4" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="AP27" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="AQ27" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AR27" s="4"/>
-      <c r="AS27" s="4"/>
+        <v>162</v>
+      </c>
       <c r="AT27" s="4" t="s">
         <v>255</v>
       </c>
       <c r="AU27" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="AV27" s="4"/>
-      <c r="AW27" s="4"/>
-      <c r="AX27" s="4"/>
       <c r="AY27" s="4"/>
-      <c r="AZ27" s="4"/>
-      <c r="BA27" s="4"/>
-      <c r="BB27" s="4"/>
-      <c r="BC27" s="4"/>
-      <c r="BD27" s="4"/>
-      <c r="BE27" s="4"/>
-      <c r="BF27" s="4"/>
+      <c r="BU27" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="BW27" s="6"/>
       <c r="BX27" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY27" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ27" s="4"/>
-      <c r="CA27" t="s">
-        <v>185</v>
-      </c>
-      <c r="CB27" t="s">
-        <v>186</v>
+        <v>163</v>
+      </c>
+      <c r="BZ27" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="CI27">
         <v>25</v>
@@ -3337,37 +3329,39 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>187</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>176</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="L28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" t="s">
         <v>145</v>
       </c>
-      <c r="R28" s="4"/>
+      <c r="R28" t="s">
+        <v>146</v>
+      </c>
       <c r="S28" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
+      <c r="Y28" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="Z28" s="4" t="s">
         <v>155</v>
       </c>
       <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
-      <c r="AD28" s="4" t="s">
-        <v>172</v>
+      <c r="AD28" t="s">
+        <v>167</v>
       </c>
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
@@ -3380,25 +3374,24 @@
       <c r="AM28" s="4"/>
       <c r="AN28" s="4"/>
       <c r="AO28" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AP28" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="AQ28" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AR28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AS28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AT28" s="4"/>
-      <c r="AU28" s="4"/>
-      <c r="AW28" s="4" t="s">
-        <v>181</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="AR28" s="4"/>
+      <c r="AS28" s="4"/>
+      <c r="AT28" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AU28" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="AV28" s="4"/>
+      <c r="AW28" s="4"/>
       <c r="AX28" s="4"/>
       <c r="AY28" s="4"/>
       <c r="AZ28" s="4"/>
@@ -3408,7 +3401,6 @@
       <c r="BD28" s="4"/>
       <c r="BE28" s="4"/>
       <c r="BF28" s="4"/>
-      <c r="BW28" s="9"/>
       <c r="BX28" s="4" t="s">
         <v>154</v>
       </c>
@@ -3416,6 +3408,12 @@
         <v>103</v>
       </c>
       <c r="BZ28" s="4"/>
+      <c r="CA28" t="s">
+        <v>185</v>
+      </c>
+      <c r="CB28" t="s">
+        <v>186</v>
+      </c>
       <c r="CI28">
         <v>25</v>
       </c>
@@ -3444,23 +3442,78 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>176</v>
       </c>
+      <c r="P29" s="4"/>
       <c r="Q29" t="s">
         <v>145</v>
       </c>
+      <c r="R29" s="4"/>
       <c r="S29" s="4" t="s">
         <v>171</v>
       </c>
       <c r="T29" s="4" t="s">
         <v>171</v>
       </c>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
+      <c r="AK29" s="4"/>
+      <c r="AL29" s="4"/>
+      <c r="AM29" s="4"/>
+      <c r="AN29" s="4"/>
+      <c r="AO29" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP29" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AQ29" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AR29" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AS29" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AT29" s="4"/>
+      <c r="AU29" s="4"/>
+      <c r="AW29" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX29" s="4"/>
       <c r="AY29" s="4"/>
+      <c r="AZ29" s="4"/>
+      <c r="BA29" s="4"/>
+      <c r="BB29" s="4"/>
+      <c r="BC29" s="4"/>
+      <c r="BD29" s="4"/>
+      <c r="BE29" s="4"/>
+      <c r="BF29" s="4"/>
+      <c r="BW29" s="9"/>
       <c r="BX29" s="4" t="s">
         <v>154</v>
       </c>
@@ -3496,10 +3549,23 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>198</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>145</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AY30" s="4"/>
       <c r="BX30" s="4" t="s">
         <v>154</v>
       </c>
@@ -3507,9 +3573,6 @@
         <v>103</v>
       </c>
       <c r="BZ30" s="4"/>
-      <c r="CH30" t="s">
-        <v>200</v>
-      </c>
       <c r="CI30">
         <v>25</v>
       </c>
@@ -3538,12 +3601,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>210</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="BX31" s="4" t="s">
         <v>154</v>
@@ -3552,6 +3612,9 @@
         <v>103</v>
       </c>
       <c r="BZ31" s="4"/>
+      <c r="CH31" t="s">
+        <v>200</v>
+      </c>
       <c r="CI31">
         <v>25</v>
       </c>
@@ -3580,250 +3643,292 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>212</v>
+        <v>210</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>211</v>
       </c>
       <c r="BX32" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY32" s="4" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="BZ32" s="4"/>
       <c r="CI32">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="CJ32">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="CK32">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="CL32">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="CM32">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="CN32">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="CO32">
         <v>32</v>
       </c>
       <c r="CP32">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="CQ32" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:96" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BX33" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BY33" s="4" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="BZ33" s="4"/>
       <c r="CI33">
+        <v>12</v>
+      </c>
+      <c r="CJ33">
         <v>32</v>
       </c>
-      <c r="CJ33">
+      <c r="CK33">
+        <v>22</v>
+      </c>
+      <c r="CL33">
+        <v>12</v>
+      </c>
+      <c r="CM33">
+        <v>23</v>
+      </c>
+      <c r="CN33">
+        <v>20</v>
+      </c>
+      <c r="CO33">
+        <v>32</v>
+      </c>
+      <c r="CP33">
+        <v>21</v>
+      </c>
+      <c r="CQ33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>213</v>
+      </c>
+      <c r="BX34" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY34" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BZ34" s="4"/>
+      <c r="CI34">
+        <v>32</v>
+      </c>
+      <c r="CJ34">
         <v>34</v>
       </c>
-      <c r="CK33">
+      <c r="CK34">
         <v>54</v>
       </c>
-      <c r="CL33">
+      <c r="CL34">
         <v>21</v>
       </c>
-      <c r="CM33">
+      <c r="CM34">
         <v>13</v>
       </c>
-      <c r="CN33">
+      <c r="CN34">
         <v>5</v>
       </c>
-      <c r="CO33">
+      <c r="CO34">
         <v>2</v>
       </c>
-      <c r="CP33">
+      <c r="CP34">
         <v>12</v>
       </c>
-      <c r="CQ33" t="s">
+      <c r="CQ34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:96" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="35" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>216</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AA35" t="s">
         <v>222</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AB35" t="s">
         <v>223</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AC35" t="s">
         <v>224</v>
       </c>
-      <c r="BU34" t="s">
+      <c r="BU35" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:96" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="36" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>217</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-      <c r="AA35" t="s">
+      <c r="C36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" t="s">
         <v>225</v>
       </c>
-      <c r="AB35" t="s">
+      <c r="AB36" t="s">
         <v>226</v>
       </c>
-      <c r="AC35" t="s">
+      <c r="AC36" t="s">
         <v>227</v>
       </c>
-      <c r="AD35" s="4"/>
-      <c r="AE35" s="4"/>
-      <c r="AF35" s="4"/>
-      <c r="AG35" s="4"/>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="4"/>
-      <c r="AJ35" s="4"/>
-      <c r="AK35" s="4"/>
-      <c r="AL35" s="4"/>
-      <c r="AM35" s="4"/>
-      <c r="AN35" s="4"/>
-      <c r="AO35" s="4"/>
-      <c r="AP35" s="4"/>
-      <c r="AQ35" s="4"/>
-      <c r="AR35" s="4"/>
-      <c r="AS35" s="4"/>
-      <c r="AT35" s="4"/>
-      <c r="AU35" s="4"/>
-      <c r="AV35" s="4"/>
-      <c r="BU35" t="s">
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4"/>
+      <c r="AF36" s="4"/>
+      <c r="AG36" s="4"/>
+      <c r="AH36" s="4"/>
+      <c r="AI36" s="4"/>
+      <c r="AJ36" s="4"/>
+      <c r="AK36" s="4"/>
+      <c r="AL36" s="4"/>
+      <c r="AM36" s="4"/>
+      <c r="AN36" s="4"/>
+      <c r="AO36" s="4"/>
+      <c r="AP36" s="4"/>
+      <c r="AQ36" s="4"/>
+      <c r="AR36" s="4"/>
+      <c r="AS36" s="4"/>
+      <c r="AT36" s="4"/>
+      <c r="AU36" s="4"/>
+      <c r="AV36" s="4"/>
+      <c r="BU36" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:96" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>218</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AA37" t="s">
         <v>228</v>
       </c>
-      <c r="AB36" t="s">
+      <c r="AB37" t="s">
         <v>229</v>
       </c>
-      <c r="AC36" t="s">
+      <c r="AC37" t="s">
         <v>230</v>
       </c>
-      <c r="BU36" t="s">
+      <c r="BU37" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:96" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>198</v>
       </c>
-      <c r="U37" t="s">
+      <c r="U38" t="s">
         <v>152</v>
       </c>
-      <c r="V37" t="s">
+      <c r="V38" t="s">
         <v>268</v>
       </c>
-      <c r="AE37" t="s">
+      <c r="AE38" t="s">
         <v>197</v>
       </c>
-      <c r="AG37" t="s">
+      <c r="AG38" t="s">
         <v>158</v>
       </c>
-      <c r="AR37" t="s">
+      <c r="AR38" t="s">
         <v>269</v>
       </c>
-      <c r="AW37" t="s">
+      <c r="AW38" t="s">
         <v>270</v>
       </c>
-      <c r="AX37" t="s">
+      <c r="AX38" t="s">
         <v>276</v>
       </c>
-      <c r="CB37" t="s">
+      <c r="CB38" t="s">
         <v>194</v>
       </c>
-      <c r="CG37" s="14" t="s">
+      <c r="CG38" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="CH37" t="s">
+      <c r="CH38" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:96" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>271</v>
       </c>
-      <c r="U38" t="s">
+      <c r="U39" t="s">
         <v>272</v>
       </c>
-      <c r="AW38" t="s">
+      <c r="AW39" t="s">
         <v>273</v>
       </c>
-      <c r="AX38" t="s">
+      <c r="AX39" t="s">
         <v>274</v>
       </c>
-      <c r="BX38" t="s">
+      <c r="BX39" t="s">
         <v>233</v>
       </c>
-      <c r="CR38" t="s">
+      <c r="CT39" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="BY30:BY33" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
-    <hyperlink ref="AH26" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
+    <hyperlink ref="BY31:BY34" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="AH27" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
     <hyperlink ref="AH25" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
     <hyperlink ref="Y21" r:id="rId4" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
     <hyperlink ref="BY21" r:id="rId5" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
-    <hyperlink ref="BY32" r:id="rId6" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="BY29:BY31" r:id="rId7" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="BY33" r:id="rId6" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="BY30:BY32" r:id="rId7" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
     <hyperlink ref="CG24" r:id="rId8" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
     <hyperlink ref="Y19" r:id="rId9" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BY26" r:id="rId10" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
-    <hyperlink ref="BY28" r:id="rId11" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BY27" r:id="rId12" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BY27" r:id="rId10" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BY29" r:id="rId11" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BY28" r:id="rId12" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
     <hyperlink ref="BY25" r:id="rId13" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
     <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="Y26" r:id="rId15" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
-    <hyperlink ref="Y27" r:id="rId16" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y27" r:id="rId15" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="Y28" r:id="rId16" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
     <hyperlink ref="Y25" r:id="rId17" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
     <hyperlink ref="BY24" r:id="rId18" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
     <hyperlink ref="BY22" r:id="rId19" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
@@ -3835,15 +3940,17 @@
     <hyperlink ref="F5" r:id="rId25" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
     <hyperlink ref="F6" r:id="rId26" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="B5" r:id="rId27" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="BZ26" r:id="rId28" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
+    <hyperlink ref="BZ27" r:id="rId28" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
     <hyperlink ref="BZ25" r:id="rId29" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
-    <hyperlink ref="CG37" r:id="rId30" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
+    <hyperlink ref="CG38" r:id="rId30" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
     <hyperlink ref="BY23" r:id="rId31" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
     <hyperlink ref="BZ20" r:id="rId32" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
     <hyperlink ref="BY20" r:id="rId33" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
     <hyperlink ref="B2" r:id="rId34" xr:uid="{A45A2FC1-0756-4996-B77E-C3738CB0981D}"/>
+    <hyperlink ref="BY26" r:id="rId35" xr:uid="{118B4519-9553-4B2D-8F17-5D5CD3CCF7A6}"/>
+    <hyperlink ref="BZ26" r:id="rId36" xr:uid="{591C1FDE-188C-4B4E-B1F5-78AD3F842631}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId35"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Admin regrression testcases commit - Customer Create, update, Delete
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6FAECE-945D-4AA0-86FA-5FA716359658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A61156D-D0BC-4525-93D3-EECD94FF43DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -871,16 +871,16 @@
     <t>QaTester</t>
   </si>
   <si>
-    <t>spanem@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Aonqkziplddf1!</t>
-  </si>
-  <si>
     <t>ChooseCondition</t>
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>vraikanti@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Baprvtyfaqtt2!</t>
   </si>
 </sst>
 </file>
@@ -1304,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CR22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CT39" sqref="CT39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,7 +1720,7 @@
         <v>275</v>
       </c>
       <c r="CU1" s="17" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
@@ -1728,10 +1728,10 @@
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -3925,7 +3925,7 @@
         <v>274</v>
       </c>
       <c r="CU39" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Admin login details update test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A61156D-D0BC-4525-93D3-EECD94FF43DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA465BE4-914A-411D-A305-0A1F3D342DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="285">
   <si>
     <t>DataSet</t>
   </si>
@@ -592,9 +592,6 @@
     <t>mkoppanadam@helenoftroy.com</t>
   </si>
   <si>
-    <t>Acyqadtkonic1!</t>
-  </si>
-  <si>
     <t>Stacked</t>
   </si>
   <si>
@@ -877,10 +874,7 @@
     <t>Price</t>
   </si>
   <si>
-    <t>vraikanti@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Baprvtyfaqtt2!</t>
+    <t>Amtlmcflmipq1!</t>
   </si>
 </sst>
 </file>
@@ -1305,126 +1299,126 @@
   <dimension ref="A1:CU39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7265625" customWidth="1"/>
+    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.453125" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
-    <col min="13" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7265625" customWidth="1"/>
+    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7265625" customWidth="1"/>
+    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.5703125" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.54296875" customWidth="1"/>
+    <col min="31" max="31" width="17.54296875" customWidth="1"/>
+    <col min="32" max="32" width="14.7265625" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="21" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.7109375" customWidth="1"/>
-    <col min="41" max="41" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.7109375" customWidth="1"/>
-    <col min="43" max="43" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="17.28515625" customWidth="1"/>
-    <col min="48" max="48" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="60.5703125" customWidth="1"/>
-    <col min="50" max="50" width="26.28515625" customWidth="1"/>
+    <col min="40" max="40" width="15.7265625" customWidth="1"/>
+    <col min="41" max="41" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.7265625" customWidth="1"/>
+    <col min="43" max="43" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="17.26953125" customWidth="1"/>
+    <col min="48" max="48" width="45.7265625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.54296875" customWidth="1"/>
+    <col min="50" max="50" width="26.26953125" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="11.28515625" customWidth="1"/>
-    <col min="62" max="62" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.26953125" customWidth="1"/>
+    <col min="62" max="62" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.28515625" customWidth="1"/>
-    <col min="68" max="68" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="13.28515625" customWidth="1"/>
-    <col min="73" max="73" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="42.7109375" customWidth="1"/>
-    <col min="77" max="77" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7109375" customWidth="1"/>
-    <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.5703125" customWidth="1"/>
-    <col min="87" max="87" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="96" max="97" width="35.42578125" customWidth="1"/>
-    <col min="98" max="98" width="146.7109375" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.26953125" customWidth="1"/>
+    <col min="68" max="68" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="13.26953125" customWidth="1"/>
+    <col min="73" max="73" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="42.7265625" customWidth="1"/>
+    <col min="77" max="77" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.7265625" customWidth="1"/>
+    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.54296875" customWidth="1"/>
+    <col min="87" max="87" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="35.453125" customWidth="1"/>
+    <col min="98" max="98" width="146.7265625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="15" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="12" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="17" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="118" max="118" width="8" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="14" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="5" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1504,13 +1498,13 @@
         <v>134</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>135</v>
@@ -1525,16 +1519,16 @@
         <v>138</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="AL1" s="3" t="s">
         <v>139</v>
@@ -1561,10 +1555,10 @@
         <v>179</v>
       </c>
       <c r="AT1" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="AU1" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>16</v>
@@ -1573,7 +1567,7 @@
         <v>17</v>
       </c>
       <c r="AX1" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AY1" s="3" t="s">
         <v>18</v>
@@ -1636,10 +1630,10 @@
         <v>34</v>
       </c>
       <c r="BS1" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="BT1" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="BU1" s="3" t="s">
         <v>35</v>
@@ -1657,7 +1651,7 @@
         <v>39</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="CA1" s="3" t="s">
         <v>104</v>
@@ -1681,57 +1675,57 @@
         <v>124</v>
       </c>
       <c r="CH1" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="CI1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="CJ1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="CJ1" s="16" t="s">
+      <c r="CK1" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="CK1" s="16" t="s">
+      <c r="CL1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="CL1" s="16" t="s">
+      <c r="CM1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="CM1" s="16" t="s">
+      <c r="CN1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="CN1" s="16" t="s">
+      <c r="CO1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="CO1" s="16" t="s">
+      <c r="CP1" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="CP1" s="16" t="s">
+      <c r="CQ1" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="CQ1" s="17" t="s">
-        <v>209</v>
-      </c>
       <c r="CR1" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="CS1" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CT1" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="CU1" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>285</v>
+        <v>189</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1789,7 +1783,7 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1797,7 +1791,7 @@
         <v>189</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>190</v>
+        <v>284</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1860,7 +1854,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1926,7 +1920,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1983,7 +1977,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2041,7 +2035,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2098,7 +2092,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2155,7 +2149,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2206,7 +2200,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2233,7 +2227,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2257,7 +2251,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2314,7 +2308,7 @@
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2339,7 +2333,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2405,7 +2399,7 @@
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2444,7 +2438,7 @@
       </c>
       <c r="BZ15" s="4"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2452,7 +2446,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2463,7 +2457,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2479,7 +2473,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2520,7 +2514,7 @@
       <c r="AQ19" s="4"/>
       <c r="AV19" s="4"/>
       <c r="AW19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AY19" s="4"/>
       <c r="BR19" s="1"/>
@@ -2536,22 +2530,22 @@
         <v>102</v>
       </c>
       <c r="BX19" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="BY19" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BZ19" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="CA19" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="CB19" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="CB19" s="5" t="s">
+      <c r="CC19" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="CC19" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="CI19">
         <v>25</v>
@@ -2581,9 +2575,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2621,21 +2615,21 @@
       <c r="BS20" s="1"/>
       <c r="BT20" s="1"/>
       <c r="BX20" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="BY20" s="4" t="s">
         <v>163</v>
       </c>
       <c r="BZ20" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CA20" s="5"/>
       <c r="CB20" s="5"/>
       <c r="CC20" s="5"/>
     </row>
-    <row r="21" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2644,7 +2638,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2677,22 +2671,22 @@
       <c r="AP21" s="4"/>
       <c r="AQ21" s="4"/>
       <c r="AR21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AV21" s="4"/>
       <c r="AW21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AX21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AY21" s="4"/>
       <c r="BR21" s="1"/>
       <c r="BS21" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="BT21" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="BU21" t="s">
         <v>100</v>
@@ -2704,20 +2698,20 @@
         <v>102</v>
       </c>
       <c r="BX21" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BY21" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BZ21" s="4"/>
       <c r="CA21" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="CB21" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="CB21" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="CC21" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="CI21">
         <v>25</v>
@@ -2747,7 +2741,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2789,10 +2783,10 @@
       </c>
       <c r="BZ22" s="14"/>
       <c r="CA22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="CB22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CD22" t="s">
         <v>115</v>
@@ -2825,7 +2819,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -2872,7 +2866,7 @@
       <c r="AU23" s="4"/>
       <c r="AV23" s="4"/>
       <c r="AW23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BX23" s="4" t="s">
         <v>154</v>
@@ -2905,7 +2899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -2954,14 +2948,14 @@
       <c r="BN24" s="9"/>
       <c r="BO24" s="9"/>
       <c r="BX24" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BY24" s="14" t="s">
         <v>103</v>
       </c>
       <c r="BZ24" s="14"/>
       <c r="CF24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="CG24" s="14" t="s">
         <v>118</v>
@@ -2991,7 +2985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -3017,7 +3011,7 @@
         <v>149</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="W25" t="s">
         <v>151</v>
@@ -3035,7 +3029,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AE25" s="15" t="s">
         <v>157</v>
@@ -3047,19 +3041,19 @@
         <v>158</v>
       </c>
       <c r="AH25" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="AI25" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="AI25" s="18" t="s">
+      <c r="AJ25" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="AJ25" s="18" t="s">
-        <v>252</v>
-      </c>
       <c r="AK25" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AL25" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="AL25" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="AM25" s="4">
         <v>3</v>
@@ -3077,10 +3071,10 @@
         <v>162</v>
       </c>
       <c r="AT25" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AU25" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="AU25" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="AY25" s="4"/>
       <c r="BB25" t="s">
@@ -3100,7 +3094,7 @@
         <v>103</v>
       </c>
       <c r="BZ25" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="CI25">
         <v>25</v>
@@ -3130,9 +3124,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L26" s="4"/>
       <c r="T26" s="4"/>
@@ -3164,17 +3158,17 @@
         <v>119</v>
       </c>
       <c r="BU26" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="BW26" s="6"/>
       <c r="BX26" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="BY26" s="4" t="s">
         <v>103</v>
       </c>
       <c r="BZ26" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="CI26">
         <v>25</v>
@@ -3204,13 +3198,13 @@
         <v>77</v>
       </c>
       <c r="CR26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="CS26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
-    <row r="27" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>183</v>
       </c>
@@ -3231,7 +3225,7 @@
         <v>149</v>
       </c>
       <c r="V27" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W27" t="s">
         <v>151</v>
@@ -3249,7 +3243,7 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
       <c r="AD27" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AE27" s="15" t="s">
         <v>157</v>
@@ -3258,22 +3252,22 @@
         <v>115</v>
       </c>
       <c r="AG27" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AH27" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AI27" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="AI27" s="18" t="s">
-        <v>254</v>
-      </c>
       <c r="AJ27" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AK27" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AL27" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AM27" s="4">
         <v>3</v>
@@ -3291,10 +3285,10 @@
         <v>162</v>
       </c>
       <c r="AT27" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AU27" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="AU27" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="AY27" s="4"/>
       <c r="BU27" s="4" t="s">
@@ -3308,7 +3302,7 @@
         <v>163</v>
       </c>
       <c r="BZ27" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CI27">
         <v>25</v>
@@ -3338,7 +3332,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>184</v>
       </c>
@@ -3394,10 +3388,10 @@
       <c r="AR28" s="4"/>
       <c r="AS28" s="4"/>
       <c r="AT28" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AU28" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="AU28" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="AV28" s="4"/>
       <c r="AW28" s="4"/>
@@ -3451,7 +3445,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>187</v>
       </c>
@@ -3558,7 +3552,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>188</v>
       </c>
@@ -3610,9 +3604,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BX31" s="4" t="s">
         <v>154</v>
@@ -3622,7 +3616,7 @@
       </c>
       <c r="BZ31" s="4"/>
       <c r="CH31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="CI31">
         <v>25</v>
@@ -3652,12 +3646,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD32" t="s">
         <v>210</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>211</v>
       </c>
       <c r="BX32" s="4" t="s">
         <v>154</v>
@@ -3694,9 +3688,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BX33" s="4" t="s">
         <v>154</v>
@@ -3730,12 +3724,12 @@
         <v>21</v>
       </c>
       <c r="CQ33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="BX34" s="4" t="s">
         <v>154</v>
@@ -3769,29 +3763,29 @@
         <v>12</v>
       </c>
       <c r="CQ34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>215</v>
       </c>
+      <c r="AA35" t="s">
+        <v>221</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>223</v>
+      </c>
+      <c r="BU35" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>216</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>222</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>223</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>224</v>
-      </c>
-      <c r="BU35" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>217</v>
       </c>
       <c r="C36" s="4"/>
       <c r="F36" s="4"/>
@@ -3816,13 +3810,13 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
       <c r="AA36" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB36" t="s">
         <v>225</v>
       </c>
-      <c r="AB36" t="s">
+      <c r="AC36" t="s">
         <v>226</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>227</v>
       </c>
       <c r="AD36" s="4"/>
       <c r="AE36" s="4"/>
@@ -3844,88 +3838,88 @@
       <c r="AU36" s="4"/>
       <c r="AV36" s="4"/>
       <c r="BU36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AA37" t="s">
+        <v>227</v>
+      </c>
+      <c r="AB37" t="s">
         <v>228</v>
       </c>
-      <c r="AB37" t="s">
+      <c r="AC37" t="s">
         <v>229</v>
       </c>
-      <c r="AC37" t="s">
+      <c r="BU37" t="s">
         <v>230</v>
       </c>
-      <c r="BU37" t="s">
-        <v>231</v>
-      </c>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U38" t="s">
         <v>152</v>
       </c>
       <c r="V38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AE38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AG38" t="s">
         <v>158</v>
       </c>
       <c r="AR38" t="s">
+        <v>268</v>
+      </c>
+      <c r="AW38" t="s">
         <v>269</v>
       </c>
-      <c r="AW38" t="s">
-        <v>270</v>
-      </c>
       <c r="AX38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="CB38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CG38" s="14" t="s">
         <v>103</v>
       </c>
       <c r="CH38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="CI38">
         <v>40</v>
       </c>
       <c r="CT38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>270</v>
+      </c>
+      <c r="U39" t="s">
         <v>271</v>
       </c>
-      <c r="U39" t="s">
+      <c r="AW39" t="s">
         <v>272</v>
       </c>
-      <c r="AW39" t="s">
+      <c r="AX39" t="s">
         <v>273</v>
       </c>
-      <c r="AX39" t="s">
-        <v>274</v>
-      </c>
       <c r="BX39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="CT39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="CU39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create update and delete hydroflask for admin
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA465BE4-914A-411D-A305-0A1F3D342DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F155AF-DA5C-4524-8831-E4EB37C3A1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="285">
   <si>
     <t>DataSet</t>
   </si>
@@ -1299,126 +1299,126 @@
   <dimension ref="A1:CU39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7265625" customWidth="1"/>
-    <col min="9" max="9" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.42578125" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
-    <col min="13" max="15" width="30.7265625" customWidth="1"/>
-    <col min="16" max="16" width="89.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7265625" customWidth="1"/>
-    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.54296875" customWidth="1"/>
-    <col min="31" max="31" width="17.54296875" customWidth="1"/>
-    <col min="32" max="32" width="14.7265625" customWidth="1"/>
+    <col min="25" max="25" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.5703125" customWidth="1"/>
+    <col min="31" max="31" width="17.5703125" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="21" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.7265625" customWidth="1"/>
-    <col min="41" max="41" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.7265625" customWidth="1"/>
-    <col min="43" max="43" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="17.26953125" customWidth="1"/>
-    <col min="48" max="48" width="45.7265625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="60.54296875" customWidth="1"/>
-    <col min="50" max="50" width="26.26953125" customWidth="1"/>
+    <col min="40" max="40" width="15.7109375" customWidth="1"/>
+    <col min="41" max="41" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.7109375" customWidth="1"/>
+    <col min="43" max="43" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="17.28515625" customWidth="1"/>
+    <col min="48" max="48" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.5703125" customWidth="1"/>
+    <col min="50" max="50" width="26.28515625" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="11.26953125" customWidth="1"/>
-    <col min="62" max="62" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.28515625" customWidth="1"/>
+    <col min="62" max="62" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.26953125" customWidth="1"/>
-    <col min="68" max="68" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="49.54296875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="13.26953125" customWidth="1"/>
-    <col min="73" max="73" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="42.7265625" customWidth="1"/>
-    <col min="77" max="77" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7265625" customWidth="1"/>
-    <col min="79" max="79" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.54296875" customWidth="1"/>
-    <col min="87" max="87" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="96" max="97" width="35.453125" customWidth="1"/>
-    <col min="98" max="98" width="146.7265625" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.28515625" customWidth="1"/>
+    <col min="68" max="68" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="13.28515625" customWidth="1"/>
+    <col min="73" max="73" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="42.7109375" customWidth="1"/>
+    <col min="77" max="77" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.7109375" customWidth="1"/>
+    <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.5703125" customWidth="1"/>
+    <col min="87" max="87" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="35.42578125" customWidth="1"/>
+    <col min="98" max="98" width="146.7109375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="15" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="12" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="17" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="118" max="118" width="8" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="14" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="5" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1854,7 +1854,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1920,7 +1920,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1977,7 +1977,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2092,7 +2092,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2308,7 +2308,7 @@
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2333,7 +2333,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2345,6 +2345,9 @@
       </c>
       <c r="F14" s="4" t="s">
         <v>79</v>
+      </c>
+      <c r="I14" t="s">
+        <v>72</v>
       </c>
       <c r="Q14" s="4"/>
       <c r="S14" s="4"/>
@@ -2399,7 +2402,7 @@
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2438,7 +2441,7 @@
       </c>
       <c r="BZ15" s="4"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2446,7 +2449,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2457,7 +2460,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2473,7 +2476,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>276</v>
       </c>
@@ -2627,7 +2630,7 @@
       <c r="CB20" s="5"/>
       <c r="CC20" s="5"/>
     </row>
-    <row r="21" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>233</v>
       </c>
@@ -2741,7 +2744,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2819,7 +2822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -2985,7 +2988,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -3124,7 +3127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>278</v>
       </c>
@@ -3204,7 +3207,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="27" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>183</v>
       </c>
@@ -3332,7 +3335,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>184</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>187</v>
       </c>
@@ -3552,7 +3555,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>188</v>
       </c>
@@ -3604,7 +3607,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>197</v>
       </c>
@@ -3646,7 +3649,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>209</v>
       </c>
@@ -3688,7 +3691,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -3727,7 +3730,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>212</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -3783,7 +3786,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>216</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>217</v>
       </c>
@@ -3858,7 +3861,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>197</v>
       </c>
@@ -3899,7 +3902,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>270</v>
       </c>

</xml_diff>

<commit_message>
oxo drybar and osprey us admin for create update and delete customer
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F155AF-DA5C-4524-8831-E4EB37C3A1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A2058D-8A23-4F74-B240-FF92D4743548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="312" yWindow="312" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="294">
   <si>
     <t>DataSet</t>
   </si>
@@ -250,9 +250,6 @@
     <t>Test Test</t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>testing</t>
   </si>
   <si>
@@ -875,6 +872,36 @@
   </si>
   <si>
     <t>Amtlmcflmipq1!</t>
+  </si>
+  <si>
+    <t>HYFCustomer</t>
+  </si>
+  <si>
+    <t>OxoCustomer</t>
+  </si>
+  <si>
+    <t>OXO Website</t>
+  </si>
+  <si>
+    <t>8 cup coffee</t>
+  </si>
+  <si>
+    <t>OSPUSCustomer</t>
+  </si>
+  <si>
+    <t>Osprey US</t>
+  </si>
+  <si>
+    <t>VOLT 45</t>
+  </si>
+  <si>
+    <t>DRYCustomer</t>
+  </si>
+  <si>
+    <t>Drybar Website</t>
+  </si>
+  <si>
+    <t>Hair</t>
   </si>
 </sst>
 </file>
@@ -1296,129 +1323,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU39"/>
+  <dimension ref="A1:CU42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="32.44140625" customWidth="1"/>
     <col min="12" max="12" width="52" customWidth="1"/>
-    <col min="13" max="15" width="30.7109375" customWidth="1"/>
-    <col min="16" max="16" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="30.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="30.6640625" customWidth="1"/>
+    <col min="16" max="16" width="89.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="30.6640625" customWidth="1"/>
+    <col min="21" max="21" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.5546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.5703125" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.5546875" customWidth="1"/>
+    <col min="31" max="31" width="17.5546875" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="21" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="37.5546875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.7109375" customWidth="1"/>
-    <col min="41" max="41" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.7109375" customWidth="1"/>
-    <col min="43" max="43" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="17.28515625" customWidth="1"/>
-    <col min="48" max="48" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="60.5703125" customWidth="1"/>
-    <col min="50" max="50" width="26.28515625" customWidth="1"/>
+    <col min="40" max="40" width="15.6640625" customWidth="1"/>
+    <col min="41" max="41" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.6640625" customWidth="1"/>
+    <col min="43" max="43" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="17.33203125" customWidth="1"/>
+    <col min="48" max="48" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="60.5546875" customWidth="1"/>
+    <col min="50" max="50" width="26.33203125" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="11.28515625" customWidth="1"/>
-    <col min="62" max="62" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.33203125" customWidth="1"/>
+    <col min="62" max="62" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.28515625" customWidth="1"/>
-    <col min="68" max="68" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="13.28515625" customWidth="1"/>
-    <col min="73" max="73" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="42.7109375" customWidth="1"/>
-    <col min="77" max="77" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="54.7109375" customWidth="1"/>
-    <col min="79" max="79" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14.5703125" customWidth="1"/>
-    <col min="87" max="87" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="96" max="97" width="35.42578125" customWidth="1"/>
-    <col min="98" max="98" width="146.7109375" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.33203125" customWidth="1"/>
+    <col min="68" max="68" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="13.33203125" customWidth="1"/>
+    <col min="73" max="73" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="42.6640625" customWidth="1"/>
+    <col min="77" max="77" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.6640625" customWidth="1"/>
+    <col min="79" max="79" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="14.5546875" customWidth="1"/>
+    <col min="87" max="87" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="35.44140625" customWidth="1"/>
+    <col min="98" max="98" width="146.6640625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="15" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="12" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="17" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="118" max="118" width="8" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="14" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="5" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1468,97 +1495,97 @@
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AL1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="AT1" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="AL1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>16</v>
@@ -1567,7 +1594,7 @@
         <v>17</v>
       </c>
       <c r="AX1" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AY1" s="3" t="s">
         <v>18</v>
@@ -1597,10 +1624,10 @@
         <v>26</v>
       </c>
       <c r="BH1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI1" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="BJ1" s="3" t="s">
         <v>27</v>
@@ -1618,7 +1645,7 @@
         <v>31</v>
       </c>
       <c r="BO1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BP1" s="3" t="s">
         <v>32</v>
@@ -1630,10 +1657,10 @@
         <v>34</v>
       </c>
       <c r="BS1" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="BT1" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="BU1" s="3" t="s">
         <v>35</v>
@@ -1651,81 +1678,81 @@
         <v>39</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="CA1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="CB1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="CC1" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="CD1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="CE1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="CF1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="CG1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="CG1" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="CH1" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="CI1" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="CJ1" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="CJ1" s="16" t="s">
+      <c r="CK1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="CK1" s="16" t="s">
+      <c r="CL1" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="CL1" s="16" t="s">
+      <c r="CM1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="CM1" s="16" t="s">
+      <c r="CN1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="CN1" s="16" t="s">
+      <c r="CO1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="CO1" s="16" t="s">
+      <c r="CP1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="CP1" s="16" t="s">
+      <c r="CQ1" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="CQ1" s="17" t="s">
-        <v>208</v>
-      </c>
       <c r="CR1" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="CS1" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="CT1" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="CU1" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1783,15 +1810,15 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1854,7 +1881,7 @@
       <c r="BO3" s="6"/>
       <c r="BP3" s="7"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1920,7 +1947,7 @@
       <c r="BO4" s="6"/>
       <c r="BP4" s="7"/>
     </row>
-    <row r="5" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1977,7 +2004,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="8"/>
     </row>
-    <row r="6" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2035,7 +2062,7 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2092,7 +2119,7 @@
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2149,7 +2176,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="4"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2200,7 +2227,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="4"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2227,7 +2254,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2251,7 +2278,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2308,7 +2335,7 @@
       <c r="AX12" s="4"/>
       <c r="AY12" s="4"/>
     </row>
-    <row r="13" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2333,18 +2360,18 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="8"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>284</v>
+      </c>
+      <c r="D14" t="s">
         <v>76</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>77</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="I14" t="s">
         <v>72</v>
@@ -2379,423 +2406,401 @@
         <v>72</v>
       </c>
       <c r="BA14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="BB14" s="11" t="s">
+      <c r="BC14" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="BC14" s="12" t="s">
+      <c r="BD14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="BD14" s="12" t="s">
+      <c r="BE14" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="BE14" s="12" t="s">
+      <c r="BF14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="BF14" s="12" t="s">
+      <c r="BG14" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="BG14" s="11" t="s">
-        <v>86</v>
       </c>
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
+      <c r="BP14" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ14" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>285</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="4"/>
+      <c r="AJ15" s="4"/>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="4"/>
+      <c r="AN15" s="4"/>
+      <c r="AO15" s="4"/>
+      <c r="AP15" s="4"/>
+      <c r="AQ15" s="4"/>
+      <c r="AZ15" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="BA15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB15" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE15" s="12"/>
+      <c r="BF15" s="12"/>
+      <c r="BG15" s="11"/>
+      <c r="BH15" s="11"/>
+      <c r="BI15" s="11"/>
+      <c r="BP15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BR15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>288</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="4"/>
+      <c r="AL16" s="4"/>
+      <c r="AM16" s="4"/>
+      <c r="AN16" s="4"/>
+      <c r="AO16" s="4"/>
+      <c r="AP16" s="4"/>
+      <c r="AQ16" s="4"/>
+      <c r="AZ16" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="BA16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE16" s="12"/>
+      <c r="BF16" s="12"/>
+      <c r="BG16" s="11"/>
+      <c r="BH16" s="11"/>
+      <c r="BI16" s="11"/>
+      <c r="BP16" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BR16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>291</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="4"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="4"/>
+      <c r="AN17" s="4"/>
+      <c r="AO17" s="4"/>
+      <c r="AP17" s="4"/>
+      <c r="AQ17" s="4"/>
+      <c r="AZ17" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="BA17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE17" s="12"/>
+      <c r="BF17" s="12"/>
+      <c r="BG17" s="11"/>
+      <c r="BH17" s="11"/>
+      <c r="BI17" s="11"/>
+      <c r="BP17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ17" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BR17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC18" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="I15" t="s">
-        <v>72</v>
-      </c>
-      <c r="BC15" s="12" t="s">
+      <c r="BH18" t="s">
+        <v>108</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>109</v>
+      </c>
+      <c r="BJ18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="BH15" t="s">
-        <v>109</v>
-      </c>
-      <c r="BI15" t="s">
-        <v>110</v>
-      </c>
-      <c r="BJ15" s="5" t="s">
+      <c r="BK18" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="BK15" s="5" t="s">
+      <c r="BL18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="BL15" s="9" t="s">
+      <c r="BM18" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="BM15" s="13" t="s">
+      <c r="BN18" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BO18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="BY18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="BZ18" s="4"/>
+    </row>
+    <row r="19" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>92</v>
       </c>
-      <c r="BN15" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="BO15" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="BY15" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="BZ15" s="4"/>
+      <c r="BP19" s="9" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>93</v>
-      </c>
-      <c r="BP16" s="9" t="s">
+    <row r="20" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>94</v>
       </c>
+      <c r="BQ20" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BX20" s="4" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="17" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>95</v>
-      </c>
-      <c r="BQ17" s="9" t="s">
+    <row r="21" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>96</v>
       </c>
-      <c r="BX17" s="4" t="s">
-        <v>154</v>
+      <c r="C21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="BR21" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU21" s="8"/>
+      <c r="BX21" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="L18" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="BR18" t="s">
+    <row r="22" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>98</v>
       </c>
-      <c r="BU18" s="8"/>
-      <c r="BX18" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" t="s">
-        <v>177</v>
-      </c>
-      <c r="P19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="Y19" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="4"/>
-      <c r="AD19" s="4"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="4"/>
-      <c r="AG19" s="4"/>
-      <c r="AL19" s="4"/>
-      <c r="AM19" s="4"/>
-      <c r="AN19" s="4"/>
-      <c r="AO19" s="4"/>
-      <c r="AP19" s="4"/>
-      <c r="AQ19" s="4"/>
-      <c r="AV19" s="4"/>
-      <c r="AW19" t="s">
-        <v>194</v>
-      </c>
-      <c r="AY19" s="4"/>
-      <c r="BR19" s="1"/>
-      <c r="BS19" s="1"/>
-      <c r="BT19" s="1"/>
-      <c r="BU19" t="s">
-        <v>100</v>
-      </c>
-      <c r="BV19" t="s">
-        <v>101</v>
-      </c>
-      <c r="BW19" t="s">
-        <v>102</v>
-      </c>
-      <c r="BX19" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="BY19" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ19" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="CA19" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="CB19" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="CC19" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="CI19">
-        <v>25</v>
-      </c>
-      <c r="CJ19">
-        <v>27</v>
-      </c>
-      <c r="CK19">
-        <v>15</v>
-      </c>
-      <c r="CL19">
-        <v>10</v>
-      </c>
-      <c r="CM19">
-        <v>30</v>
-      </c>
-      <c r="CN19">
-        <v>35</v>
-      </c>
-      <c r="CO19">
-        <v>32</v>
-      </c>
-      <c r="CP19">
-        <v>23</v>
-      </c>
-      <c r="CQ19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>276</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
-      <c r="AD20" s="4"/>
-      <c r="AE20" s="15"/>
-      <c r="AF20" s="4"/>
-      <c r="AG20" s="4"/>
-      <c r="AL20" s="4"/>
-      <c r="AM20" s="4"/>
-      <c r="AN20" s="4"/>
-      <c r="AO20" s="4"/>
-      <c r="AP20" s="4"/>
-      <c r="AQ20" s="4"/>
-      <c r="AV20" s="4"/>
-      <c r="AY20" s="4"/>
-      <c r="BR20" s="1"/>
-      <c r="BS20" s="1"/>
-      <c r="BT20" s="1"/>
-      <c r="BX20" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="BY20" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="BZ20" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="CA20" s="5"/>
-      <c r="CB20" s="5"/>
-      <c r="CC20" s="5"/>
-    </row>
-    <row r="21" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>233</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" t="s">
-        <v>177</v>
-      </c>
-      <c r="P21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="Y21" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="4"/>
-      <c r="AG21" s="4"/>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
-      <c r="AJ21" s="4"/>
-      <c r="AK21" s="4"/>
-      <c r="AL21" s="4"/>
-      <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
-      <c r="AO21" s="4"/>
-      <c r="AP21" s="4"/>
-      <c r="AQ21" s="4"/>
-      <c r="AR21" t="s">
-        <v>237</v>
-      </c>
-      <c r="AV21" s="4"/>
-      <c r="AW21" t="s">
-        <v>240</v>
-      </c>
-      <c r="AX21" t="s">
-        <v>242</v>
-      </c>
-      <c r="AY21" s="4"/>
-      <c r="BR21" s="1"/>
-      <c r="BS21" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="BT21" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="BU21" t="s">
-        <v>100</v>
-      </c>
-      <c r="BV21" t="s">
-        <v>101</v>
-      </c>
-      <c r="BW21" t="s">
-        <v>102</v>
-      </c>
-      <c r="BX21" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="BY21" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ21" s="4"/>
-      <c r="CA21" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="CB21" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="CC21" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="CI21">
-        <v>25</v>
-      </c>
-      <c r="CJ21">
-        <v>27</v>
-      </c>
-      <c r="CK21">
-        <v>15</v>
-      </c>
-      <c r="CL21">
-        <v>10</v>
-      </c>
-      <c r="CM21">
-        <v>30</v>
-      </c>
-      <c r="CN21">
-        <v>35</v>
-      </c>
-      <c r="CO21">
-        <v>32</v>
-      </c>
-      <c r="CP21">
-        <v>23</v>
-      </c>
-      <c r="CQ21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>117</v>
-      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" t="s">
+        <v>176</v>
+      </c>
+      <c r="P22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-      <c r="Y22" s="5" t="s">
-        <v>39</v>
+      <c r="Y22" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
-      <c r="AD22" s="15"/>
+      <c r="AD22" s="4"/>
       <c r="AE22" s="15"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
-      <c r="AH22" s="4"/>
-      <c r="AI22" s="4"/>
-      <c r="AJ22" s="4"/>
-      <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
       <c r="AM22" s="4"/>
       <c r="AN22" s="4"/>
       <c r="AO22" s="4"/>
       <c r="AP22" s="4"/>
       <c r="AQ22" s="4"/>
-      <c r="BN22" s="6"/>
-      <c r="BO22" s="6"/>
-      <c r="BP22" s="7"/>
-      <c r="BQ22" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="BX22" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BY22" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="BZ22" s="14"/>
-      <c r="CA22" t="s">
+      <c r="AV22" s="4"/>
+      <c r="AW22" t="s">
+        <v>193</v>
+      </c>
+      <c r="AY22" s="4"/>
+      <c r="BR22" s="1"/>
+      <c r="BS22" s="1"/>
+      <c r="BT22" s="1"/>
+      <c r="BU22" t="s">
+        <v>99</v>
+      </c>
+      <c r="BV22" t="s">
+        <v>100</v>
+      </c>
+      <c r="BW22" t="s">
+        <v>101</v>
+      </c>
+      <c r="BX22" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="BY22" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ22" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="CA22" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="CB22" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="CB22" t="s">
-        <v>193</v>
-      </c>
-      <c r="CD22" t="s">
-        <v>115</v>
-      </c>
-      <c r="CE22" t="s">
-        <v>39</v>
+      <c r="CC22" s="5" t="s">
+        <v>191</v>
       </c>
       <c r="CI22">
         <v>25</v>
@@ -2821,10 +2826,13 @@
       <c r="CP22">
         <v>23</v>
       </c>
+      <c r="CQ22" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="23" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>275</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2833,78 +2841,50 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="S23" s="4"/>
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
-      <c r="AE23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="15"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
-      <c r="AH23" s="4"/>
-      <c r="AI23" s="4"/>
-      <c r="AJ23" s="4"/>
-      <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
       <c r="AM23" s="4"/>
       <c r="AN23" s="4"/>
       <c r="AO23" s="4"/>
       <c r="AP23" s="4"/>
       <c r="AQ23" s="4"/>
-      <c r="AR23" s="4"/>
-      <c r="AS23" s="4"/>
-      <c r="AT23" s="4"/>
-      <c r="AU23" s="4"/>
       <c r="AV23" s="4"/>
-      <c r="AW23" t="s">
-        <v>195</v>
-      </c>
-      <c r="BX23" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BY23" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="CI23">
-        <v>25</v>
-      </c>
-      <c r="CJ23">
-        <v>27</v>
-      </c>
-      <c r="CK23">
-        <v>15</v>
-      </c>
-      <c r="CL23">
-        <v>10</v>
-      </c>
-      <c r="CM23">
-        <v>30</v>
-      </c>
-      <c r="CN23">
-        <v>35</v>
-      </c>
-      <c r="CO23">
-        <v>32</v>
-      </c>
-      <c r="CP23">
-        <v>23</v>
-      </c>
+      <c r="AY23" s="4"/>
+      <c r="BR23" s="1"/>
+      <c r="BS23" s="1"/>
+      <c r="BT23" s="1"/>
+      <c r="BX23" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="BY23" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="BZ23" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="CA23" s="5"/>
+      <c r="CB23" s="5"/>
+      <c r="CC23" s="5"/>
     </row>
-    <row r="24" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>232</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2912,25 +2892,27 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
+      <c r="O24" t="s">
+        <v>176</v>
+      </c>
       <c r="P24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
+      <c r="Y24" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="4"/>
-      <c r="AE24" s="4"/>
+      <c r="AE24" s="15"/>
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
       <c r="AH24" s="4"/>
@@ -2943,25 +2925,48 @@
       <c r="AO24" s="4"/>
       <c r="AP24" s="4"/>
       <c r="AQ24" s="4"/>
-      <c r="AR24" s="4"/>
-      <c r="AS24" s="4"/>
-      <c r="AT24" s="4"/>
-      <c r="AU24" s="4"/>
+      <c r="AR24" t="s">
+        <v>236</v>
+      </c>
       <c r="AV24" s="4"/>
-      <c r="BN24" s="9"/>
-      <c r="BO24" s="9"/>
+      <c r="AW24" t="s">
+        <v>239</v>
+      </c>
+      <c r="AX24" t="s">
+        <v>241</v>
+      </c>
+      <c r="AY24" s="4"/>
+      <c r="BR24" s="1"/>
+      <c r="BS24" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="BT24" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="BU24" t="s">
+        <v>99</v>
+      </c>
+      <c r="BV24" t="s">
+        <v>100</v>
+      </c>
+      <c r="BW24" t="s">
+        <v>101</v>
+      </c>
       <c r="BX24" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="BY24" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ24" s="14"/>
-      <c r="CF24" t="s">
-        <v>196</v>
-      </c>
-      <c r="CG24" s="14" t="s">
-        <v>118</v>
+        <v>231</v>
+      </c>
+      <c r="BY24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ24" s="4"/>
+      <c r="CA24" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="CB24" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="CC24" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="CI24">
         <v>25</v>
@@ -2987,117 +2992,62 @@
       <c r="CP24">
         <v>23</v>
       </c>
+      <c r="CQ24" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="25" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>182</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="O25" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>145</v>
-      </c>
-      <c r="R25" t="s">
-        <v>146</v>
-      </c>
-      <c r="S25" t="s">
-        <v>147</v>
-      </c>
-      <c r="T25" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="U25" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="V25" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="W25" t="s">
-        <v>151</v>
-      </c>
-      <c r="X25" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y25" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z25" s="4" t="s">
-        <v>155</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="Y25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
-      <c r="AD25" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="AE25" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF25" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG25" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH25" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="AI25" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="AJ25" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="AK25" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="AL25" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="AM25" s="4">
-        <v>3</v>
-      </c>
-      <c r="AN25" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO25" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AP25" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AQ25" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AT25" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AU25" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AY25" s="4"/>
-      <c r="BB25" t="s">
-        <v>177</v>
-      </c>
-      <c r="BQ25" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="BU25" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="BW25" s="6"/>
+      <c r="AD25" s="15"/>
+      <c r="AE25" s="15"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="4"/>
+      <c r="AI25" s="4"/>
+      <c r="AJ25" s="4"/>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="4"/>
+      <c r="AN25" s="4"/>
+      <c r="AO25" s="4"/>
+      <c r="AP25" s="4"/>
+      <c r="AQ25" s="4"/>
+      <c r="BN25" s="6"/>
+      <c r="BO25" s="6"/>
+      <c r="BP25" s="7"/>
+      <c r="BQ25" s="9" t="s">
+        <v>118</v>
+      </c>
       <c r="BX25" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BY25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ25" s="4" t="s">
-        <v>259</v>
+        <v>153</v>
+      </c>
+      <c r="BY25" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="BZ25" s="14"/>
+      <c r="CA25" t="s">
+        <v>189</v>
+      </c>
+      <c r="CB25" t="s">
+        <v>192</v>
+      </c>
+      <c r="CD25" t="s">
+        <v>114</v>
+      </c>
+      <c r="CE25" t="s">
+        <v>39</v>
       </c>
       <c r="CI25">
         <v>25</v>
@@ -3123,30 +3073,41 @@
       <c r="CP25">
         <v>23</v>
       </c>
-      <c r="CQ25" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="26" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>278</v>
-      </c>
-      <c r="L26" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-      <c r="AD26" s="15"/>
-      <c r="AE26" s="15"/>
+      <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4"/>
-      <c r="AI26" s="18"/>
-      <c r="AJ26" s="18"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
       <c r="AM26" s="4"/>
@@ -3154,24 +3115,19 @@
       <c r="AO26" s="4"/>
       <c r="AP26" s="4"/>
       <c r="AQ26" s="4"/>
+      <c r="AR26" s="4"/>
+      <c r="AS26" s="4"/>
       <c r="AT26" s="4"/>
       <c r="AU26" s="4"/>
-      <c r="AY26" s="4"/>
-      <c r="BQ26" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="BU26" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="BW26" s="6"/>
+      <c r="AV26" s="4"/>
+      <c r="AW26" t="s">
+        <v>194</v>
+      </c>
       <c r="BX26" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="BY26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ26" s="4" t="s">
-        <v>259</v>
+        <v>153</v>
+      </c>
+      <c r="BY26" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="CI26">
         <v>25</v>
@@ -3197,115 +3153,67 @@
       <c r="CP26">
         <v>23</v>
       </c>
-      <c r="CQ26" t="s">
-        <v>77</v>
-      </c>
-      <c r="CR26" t="s">
-        <v>281</v>
-      </c>
-      <c r="CS26" t="s">
-        <v>280</v>
-      </c>
     </row>
-    <row r="27" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>183</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="Q27" t="s">
-        <v>145</v>
-      </c>
-      <c r="R27" t="s">
-        <v>146</v>
-      </c>
-      <c r="S27" t="s">
-        <v>147</v>
-      </c>
-      <c r="T27" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="U27" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="V27" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W27" t="s">
-        <v>151</v>
-      </c>
-      <c r="X27" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y27" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z27" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
-      <c r="AD27" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE27" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF27" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG27" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="AH27" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="AI27" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="AJ27" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="AK27" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="AL27" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="AM27" s="4">
-        <v>3</v>
-      </c>
-      <c r="AN27" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO27" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AP27" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AQ27" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AT27" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AU27" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AY27" s="4"/>
-      <c r="BU27" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="BW27" s="6"/>
-      <c r="BX27" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BY27" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="BZ27" s="4" t="s">
-        <v>260</v>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
+      <c r="AO27" s="4"/>
+      <c r="AP27" s="4"/>
+      <c r="AQ27" s="4"/>
+      <c r="AR27" s="4"/>
+      <c r="AS27" s="4"/>
+      <c r="AT27" s="4"/>
+      <c r="AU27" s="4"/>
+      <c r="AV27" s="4"/>
+      <c r="BN27" s="9"/>
+      <c r="BO27" s="9"/>
+      <c r="BX27" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="BY27" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ27" s="14"/>
+      <c r="CF27" t="s">
+        <v>195</v>
+      </c>
+      <c r="CG27" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="CI27">
         <v>25</v>
@@ -3331,94 +3239,117 @@
       <c r="CP27">
         <v>23</v>
       </c>
-      <c r="CQ27" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="28" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>184</v>
-      </c>
-      <c r="L28" s="4"/>
-      <c r="P28" s="4"/>
+        <v>181</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O28" t="s">
+        <v>176</v>
+      </c>
       <c r="Q28" t="s">
+        <v>144</v>
+      </c>
+      <c r="R28" t="s">
         <v>145</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>146</v>
       </c>
-      <c r="S28" s="4" t="s">
-        <v>165</v>
-      </c>
       <c r="T28" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
+        <v>147</v>
+      </c>
+      <c r="U28" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="V28" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="W28" t="s">
+        <v>150</v>
+      </c>
+      <c r="X28" t="s">
+        <v>151</v>
+      </c>
       <c r="Y28" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z28" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
-      <c r="AD28" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
-      <c r="AG28" s="4"/>
-      <c r="AH28" s="4"/>
-      <c r="AI28" s="4"/>
-      <c r="AJ28" s="4"/>
-      <c r="AK28" s="4"/>
-      <c r="AL28" s="4"/>
-      <c r="AM28" s="4"/>
-      <c r="AN28" s="4"/>
+      <c r="AD28" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="AE28" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG28" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AH28" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="AI28" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="AJ28" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="AK28" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="AL28" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AM28" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN28" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="AO28" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AP28" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AQ28" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AR28" s="4"/>
-      <c r="AS28" s="4"/>
+        <v>161</v>
+      </c>
       <c r="AT28" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU28" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="AU28" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AV28" s="4"/>
-      <c r="AW28" s="4"/>
-      <c r="AX28" s="4"/>
       <c r="AY28" s="4"/>
-      <c r="AZ28" s="4"/>
-      <c r="BA28" s="4"/>
-      <c r="BB28" s="4"/>
-      <c r="BC28" s="4"/>
-      <c r="BD28" s="4"/>
-      <c r="BE28" s="4"/>
-      <c r="BF28" s="4"/>
+      <c r="BB28" t="s">
+        <v>176</v>
+      </c>
+      <c r="BQ28" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="BU28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BW28" s="6"/>
       <c r="BX28" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ28" s="4"/>
-      <c r="CA28" t="s">
-        <v>185</v>
-      </c>
-      <c r="CB28" t="s">
-        <v>186</v>
+        <v>102</v>
+      </c>
+      <c r="BZ28" s="4" t="s">
+        <v>258</v>
       </c>
       <c r="CI28">
         <v>25</v>
@@ -3445,88 +3376,55 @@
         <v>23</v>
       </c>
       <c r="CQ28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>187</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="P29" s="4"/>
-      <c r="Q29" t="s">
-        <v>145</v>
-      </c>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>171</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="L29" s="4"/>
+      <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
-      <c r="Z29" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="Z29" s="4"/>
       <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
-      <c r="AD29" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AE29" s="4"/>
+      <c r="AD29" s="15"/>
+      <c r="AE29" s="15"/>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
       <c r="AH29" s="4"/>
-      <c r="AI29" s="4"/>
-      <c r="AJ29" s="4"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="18"/>
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
       <c r="AM29" s="4"/>
       <c r="AN29" s="4"/>
-      <c r="AO29" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="AP29" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AQ29" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AR29" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AS29" s="4" t="s">
-        <v>180</v>
-      </c>
+      <c r="AO29" s="4"/>
+      <c r="AP29" s="4"/>
+      <c r="AQ29" s="4"/>
       <c r="AT29" s="4"/>
       <c r="AU29" s="4"/>
-      <c r="AW29" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="AX29" s="4"/>
       <c r="AY29" s="4"/>
-      <c r="AZ29" s="4"/>
-      <c r="BA29" s="4"/>
-      <c r="BB29" s="4"/>
-      <c r="BC29" s="4"/>
-      <c r="BD29" s="4"/>
-      <c r="BE29" s="4"/>
-      <c r="BF29" s="4"/>
-      <c r="BW29" s="9"/>
+      <c r="BQ29" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="BU29" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="BW29" s="6"/>
       <c r="BX29" s="4" t="s">
-        <v>154</v>
+        <v>279</v>
       </c>
       <c r="BY29" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ29" s="4"/>
+        <v>102</v>
+      </c>
+      <c r="BZ29" s="4" t="s">
+        <v>258</v>
+      </c>
       <c r="CI29">
         <v>25</v>
       </c>
@@ -3552,33 +3450,115 @@
         <v>23</v>
       </c>
       <c r="CQ29" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="CR29" t="s">
+        <v>280</v>
+      </c>
+      <c r="CS29" t="s">
+        <v>279</v>
       </c>
     </row>
-    <row r="30" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>188</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>176</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="L30" s="4"/>
       <c r="Q30" t="s">
+        <v>144</v>
+      </c>
+      <c r="R30" t="s">
         <v>145</v>
       </c>
-      <c r="S30" s="4" t="s">
-        <v>171</v>
+      <c r="S30" t="s">
+        <v>146</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>171</v>
+        <v>147</v>
+      </c>
+      <c r="U30" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="W30" t="s">
+        <v>150</v>
+      </c>
+      <c r="X30" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y30" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AE30" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF30" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG30" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH30" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="AI30" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="AJ30" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="AK30" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="AL30" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="AM30" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO30" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AP30" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ30" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT30" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU30" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="AY30" s="4"/>
+      <c r="BU30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="BW30" s="6"/>
       <c r="BX30" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY30" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ30" s="4"/>
+        <v>162</v>
+      </c>
+      <c r="BZ30" s="4" t="s">
+        <v>259</v>
+      </c>
       <c r="CI30">
         <v>25</v>
       </c>
@@ -3604,22 +3584,93 @@
         <v>23</v>
       </c>
       <c r="CQ30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>197</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="L31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" t="s">
+        <v>144</v>
+      </c>
+      <c r="R31" t="s">
+        <v>145</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z31" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE31" s="4"/>
+      <c r="AF31" s="4"/>
+      <c r="AG31" s="4"/>
+      <c r="AH31" s="4"/>
+      <c r="AI31" s="4"/>
+      <c r="AJ31" s="4"/>
+      <c r="AK31" s="4"/>
+      <c r="AL31" s="4"/>
+      <c r="AM31" s="4"/>
+      <c r="AN31" s="4"/>
+      <c r="AO31" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AP31" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AQ31" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AR31" s="4"/>
+      <c r="AS31" s="4"/>
+      <c r="AT31" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU31" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AV31" s="4"/>
+      <c r="AW31" s="4"/>
+      <c r="AX31" s="4"/>
+      <c r="AY31" s="4"/>
+      <c r="AZ31" s="4"/>
+      <c r="BA31" s="4"/>
+      <c r="BB31" s="4"/>
+      <c r="BC31" s="4"/>
+      <c r="BD31" s="4"/>
+      <c r="BE31" s="4"/>
+      <c r="BF31" s="4"/>
       <c r="BX31" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY31" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BZ31" s="4"/>
-      <c r="CH31" t="s">
-        <v>199</v>
+      <c r="CA31" t="s">
+        <v>184</v>
+      </c>
+      <c r="CB31" t="s">
+        <v>185</v>
       </c>
       <c r="CI31">
         <v>25</v>
@@ -3646,21 +3697,86 @@
         <v>23</v>
       </c>
       <c r="CQ31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>209</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>210</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P32" s="4"/>
+      <c r="Q32" t="s">
+        <v>144</v>
+      </c>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="4"/>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="4"/>
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="4"/>
+      <c r="AI32" s="4"/>
+      <c r="AJ32" s="4"/>
+      <c r="AK32" s="4"/>
+      <c r="AL32" s="4"/>
+      <c r="AM32" s="4"/>
+      <c r="AN32" s="4"/>
+      <c r="AO32" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AP32" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AQ32" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR32" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AS32" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT32" s="4"/>
+      <c r="AU32" s="4"/>
+      <c r="AW32" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX32" s="4"/>
+      <c r="AY32" s="4"/>
+      <c r="AZ32" s="4"/>
+      <c r="BA32" s="4"/>
+      <c r="BB32" s="4"/>
+      <c r="BC32" s="4"/>
+      <c r="BD32" s="4"/>
+      <c r="BE32" s="4"/>
+      <c r="BF32" s="4"/>
+      <c r="BW32" s="9"/>
       <c r="BX32" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY32" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BZ32" s="4"/>
       <c r="CI32">
@@ -3688,284 +3804,423 @@
         <v>23</v>
       </c>
       <c r="CQ32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>211</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>144</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AY33" s="4"/>
       <c r="BX33" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BY33" s="4" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
       <c r="BZ33" s="4"/>
       <c r="CI33">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="CJ33">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="CK33">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="CL33">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="CM33">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="CN33">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="CO33">
         <v>32</v>
       </c>
       <c r="CP33">
+        <v>23</v>
+      </c>
+      <c r="CQ33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>196</v>
+      </c>
+      <c r="BX34" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="BY34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ34" s="4"/>
+      <c r="CH34" t="s">
+        <v>198</v>
+      </c>
+      <c r="CI34">
+        <v>25</v>
+      </c>
+      <c r="CJ34">
+        <v>27</v>
+      </c>
+      <c r="CK34">
+        <v>15</v>
+      </c>
+      <c r="CL34">
+        <v>10</v>
+      </c>
+      <c r="CM34">
+        <v>30</v>
+      </c>
+      <c r="CN34">
+        <v>35</v>
+      </c>
+      <c r="CO34">
+        <v>32</v>
+      </c>
+      <c r="CP34">
+        <v>23</v>
+      </c>
+      <c r="CQ34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>209</v>
+      </c>
+      <c r="BX35" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="BY35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ35" s="4"/>
+      <c r="CI35">
+        <v>25</v>
+      </c>
+      <c r="CJ35">
+        <v>27</v>
+      </c>
+      <c r="CK35">
+        <v>15</v>
+      </c>
+      <c r="CL35">
+        <v>10</v>
+      </c>
+      <c r="CM35">
+        <v>30</v>
+      </c>
+      <c r="CN35">
+        <v>35</v>
+      </c>
+      <c r="CO35">
+        <v>32</v>
+      </c>
+      <c r="CP35">
+        <v>23</v>
+      </c>
+      <c r="CQ35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>210</v>
+      </c>
+      <c r="BX36" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="BY36" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="BZ36" s="4"/>
+      <c r="CI36">
+        <v>12</v>
+      </c>
+      <c r="CJ36">
+        <v>32</v>
+      </c>
+      <c r="CK36">
+        <v>22</v>
+      </c>
+      <c r="CL36">
+        <v>12</v>
+      </c>
+      <c r="CM36">
+        <v>23</v>
+      </c>
+      <c r="CN36">
+        <v>20</v>
+      </c>
+      <c r="CO36">
+        <v>32</v>
+      </c>
+      <c r="CP36">
         <v>21</v>
       </c>
-      <c r="CQ33" t="s">
+      <c r="CQ36" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>211</v>
+      </c>
+      <c r="BX37" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="BY37" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ37" s="4"/>
+      <c r="CI37">
+        <v>32</v>
+      </c>
+      <c r="CJ37">
+        <v>34</v>
+      </c>
+      <c r="CK37">
+        <v>54</v>
+      </c>
+      <c r="CL37">
+        <v>21</v>
+      </c>
+      <c r="CM37">
+        <v>13</v>
+      </c>
+      <c r="CN37">
+        <v>5</v>
+      </c>
+      <c r="CO37">
+        <v>2</v>
+      </c>
+      <c r="CP37">
+        <v>12</v>
+      </c>
+      <c r="CQ37" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>212</v>
-      </c>
-      <c r="BX34" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="BY34" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ34" s="4"/>
-      <c r="CI34">
-        <v>32</v>
-      </c>
-      <c r="CJ34">
-        <v>34</v>
-      </c>
-      <c r="CK34">
-        <v>54</v>
-      </c>
-      <c r="CL34">
-        <v>21</v>
-      </c>
-      <c r="CM34">
-        <v>13</v>
-      </c>
-      <c r="CN34">
-        <v>5</v>
-      </c>
-      <c r="CO34">
-        <v>2</v>
-      </c>
-      <c r="CP34">
-        <v>12</v>
-      </c>
-      <c r="CQ34" t="s">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>214</v>
       </c>
+      <c r="AA38" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>222</v>
+      </c>
+      <c r="BU38" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>215</v>
       </c>
-      <c r="AA35" t="s">
-        <v>221</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>222</v>
-      </c>
-      <c r="AC35" t="s">
+      <c r="C39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" t="s">
         <v>223</v>
       </c>
-      <c r="BU35" t="s">
+      <c r="AB39" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD39" s="4"/>
+      <c r="AE39" s="4"/>
+      <c r="AF39" s="4"/>
+      <c r="AG39" s="4"/>
+      <c r="AH39" s="4"/>
+      <c r="AI39" s="4"/>
+      <c r="AJ39" s="4"/>
+      <c r="AK39" s="4"/>
+      <c r="AL39" s="4"/>
+      <c r="AM39" s="4"/>
+      <c r="AN39" s="4"/>
+      <c r="AO39" s="4"/>
+      <c r="AP39" s="4"/>
+      <c r="AQ39" s="4"/>
+      <c r="AR39" s="4"/>
+      <c r="AS39" s="4"/>
+      <c r="AT39" s="4"/>
+      <c r="AU39" s="4"/>
+      <c r="AV39" s="4"/>
+      <c r="BU39" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>216</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-      <c r="AA36" t="s">
-        <v>224</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>225</v>
-      </c>
-      <c r="AC36" t="s">
+      <c r="AA40" t="s">
         <v>226</v>
       </c>
-      <c r="AD36" s="4"/>
-      <c r="AE36" s="4"/>
-      <c r="AF36" s="4"/>
-      <c r="AG36" s="4"/>
-      <c r="AH36" s="4"/>
-      <c r="AI36" s="4"/>
-      <c r="AJ36" s="4"/>
-      <c r="AK36" s="4"/>
-      <c r="AL36" s="4"/>
-      <c r="AM36" s="4"/>
-      <c r="AN36" s="4"/>
-      <c r="AO36" s="4"/>
-      <c r="AP36" s="4"/>
-      <c r="AQ36" s="4"/>
-      <c r="AR36" s="4"/>
-      <c r="AS36" s="4"/>
-      <c r="AT36" s="4"/>
-      <c r="AU36" s="4"/>
-      <c r="AV36" s="4"/>
-      <c r="BU36" t="s">
+      <c r="AB40" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>228</v>
+      </c>
+      <c r="BU40" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>196</v>
+      </c>
+      <c r="U41" t="s">
+        <v>151</v>
+      </c>
+      <c r="V41" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>195</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR41" t="s">
+        <v>267</v>
+      </c>
+      <c r="AW41" t="s">
+        <v>268</v>
+      </c>
+      <c r="AX41" t="s">
+        <v>274</v>
+      </c>
+      <c r="CB41" t="s">
+        <v>192</v>
+      </c>
+      <c r="CG41" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="CH41" t="s">
+        <v>198</v>
+      </c>
+      <c r="CI41">
+        <v>40</v>
+      </c>
+      <c r="CT41" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>269</v>
+      </c>
+      <c r="U42" t="s">
+        <v>270</v>
+      </c>
+      <c r="AW42" t="s">
+        <v>271</v>
+      </c>
+      <c r="AX42" t="s">
+        <v>272</v>
+      </c>
+      <c r="BX42" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>217</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>227</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC37" t="s">
-        <v>229</v>
-      </c>
-      <c r="BU37" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>197</v>
-      </c>
-      <c r="U38" t="s">
-        <v>152</v>
-      </c>
-      <c r="V38" t="s">
-        <v>267</v>
-      </c>
-      <c r="AE38" t="s">
-        <v>196</v>
-      </c>
-      <c r="AG38" t="s">
-        <v>158</v>
-      </c>
-      <c r="AR38" t="s">
-        <v>268</v>
-      </c>
-      <c r="AW38" t="s">
-        <v>269</v>
-      </c>
-      <c r="AX38" t="s">
-        <v>275</v>
-      </c>
-      <c r="CB38" t="s">
-        <v>193</v>
-      </c>
-      <c r="CG38" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="CH38" t="s">
-        <v>199</v>
-      </c>
-      <c r="CI38">
-        <v>40</v>
-      </c>
-      <c r="CT38" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>270</v>
-      </c>
-      <c r="U39" t="s">
-        <v>271</v>
-      </c>
-      <c r="AW39" t="s">
+      <c r="CT42" t="s">
         <v>272</v>
       </c>
-      <c r="AX39" t="s">
-        <v>273</v>
-      </c>
-      <c r="BX39" t="s">
-        <v>232</v>
-      </c>
-      <c r="CT39" t="s">
-        <v>273</v>
-      </c>
-      <c r="CU39" t="s">
-        <v>283</v>
+      <c r="CU42" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="BY31:BY34" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
-    <hyperlink ref="AH27" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
-    <hyperlink ref="AH25" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
-    <hyperlink ref="Y21" r:id="rId4" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
-    <hyperlink ref="BY21" r:id="rId5" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
-    <hyperlink ref="BY33" r:id="rId6" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="BY30:BY32" r:id="rId7" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
-    <hyperlink ref="CG24" r:id="rId8" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
-    <hyperlink ref="Y19" r:id="rId9" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BY27" r:id="rId10" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
-    <hyperlink ref="BY29" r:id="rId11" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BY28" r:id="rId12" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BY25" r:id="rId13" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="BY34:BY37" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="AH30" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
+    <hyperlink ref="AH28" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
+    <hyperlink ref="Y24" r:id="rId4" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
+    <hyperlink ref="BY24" r:id="rId5" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
+    <hyperlink ref="BY36" r:id="rId6" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="BY33:BY35" r:id="rId7" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="CG27" r:id="rId8" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="Y22" r:id="rId9" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
+    <hyperlink ref="BY30" r:id="rId10" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BY32" r:id="rId11" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BY31" r:id="rId12" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BY28" r:id="rId13" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
     <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="Y27" r:id="rId15" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
-    <hyperlink ref="Y28" r:id="rId16" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
-    <hyperlink ref="Y25" r:id="rId17" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
-    <hyperlink ref="BY24" r:id="rId18" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="BY22" r:id="rId19" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
-    <hyperlink ref="BY15" r:id="rId20" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="BY19" r:id="rId21" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="Y30" r:id="rId15" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="Y31" r:id="rId16" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y28" r:id="rId17" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="BY27" r:id="rId18" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="BY25" r:id="rId19" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="BY18" r:id="rId20" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="BY22" r:id="rId21" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
     <hyperlink ref="F14" r:id="rId22" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
     <hyperlink ref="B4" r:id="rId23" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
     <hyperlink ref="C4" r:id="rId24" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="F5" r:id="rId25" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
     <hyperlink ref="F6" r:id="rId26" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="B5" r:id="rId27" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="BZ27" r:id="rId28" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
-    <hyperlink ref="BZ25" r:id="rId29" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
-    <hyperlink ref="CG38" r:id="rId30" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
-    <hyperlink ref="BY23" r:id="rId31" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
-    <hyperlink ref="BZ20" r:id="rId32" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
-    <hyperlink ref="BY20" r:id="rId33" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
+    <hyperlink ref="BZ30" r:id="rId28" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
+    <hyperlink ref="BZ28" r:id="rId29" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
+    <hyperlink ref="CG41" r:id="rId30" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
+    <hyperlink ref="BY26" r:id="rId31" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
+    <hyperlink ref="BZ23" r:id="rId32" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
+    <hyperlink ref="BY23" r:id="rId33" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
     <hyperlink ref="B2" r:id="rId34" xr:uid="{A45A2FC1-0756-4996-B77E-C3738CB0981D}"/>
-    <hyperlink ref="BY26" r:id="rId35" xr:uid="{118B4519-9553-4B2D-8F17-5D5CD3CCF7A6}"/>
-    <hyperlink ref="BZ26" r:id="rId36" xr:uid="{591C1FDE-188C-4B4E-B1F5-78AD3F842631}"/>
+    <hyperlink ref="BY29" r:id="rId35" xr:uid="{118B4519-9553-4B2D-8F17-5D5CD3CCF7A6}"/>
+    <hyperlink ref="BZ29" r:id="rId36" xr:uid="{591C1FDE-188C-4B4E-B1F5-78AD3F842631}"/>
+    <hyperlink ref="F15" r:id="rId37" xr:uid="{7FF82608-09D3-4690-A1C1-AACFF7C86E9B}"/>
+    <hyperlink ref="F16" r:id="rId38" xr:uid="{E4722610-7662-41AA-A24D-6A3E09EB03CA}"/>
+    <hyperlink ref="F17" r:id="rId39" xr:uid="{7C3664F1-DCC7-4B88-971D-CCE87E75E636}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
emea changes for the create update and delete admin testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/AdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/AdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A2058D-8A23-4F74-B240-FF92D4743548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74D08BD-C3B5-4791-991D-F03E186FED39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="312" yWindow="312" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="302">
   <si>
     <t>DataSet</t>
   </si>
@@ -280,9 +280,6 @@
     <t>7/8/2022</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Connecticut</t>
   </si>
   <si>
@@ -902,6 +899,33 @@
   </si>
   <si>
     <t>Hair</t>
+  </si>
+  <si>
+    <t>USAddress</t>
+  </si>
+  <si>
+    <t>OPSUKCustomer</t>
+  </si>
+  <si>
+    <t>Osprey Europe</t>
+  </si>
+  <si>
+    <t>UKAddress</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Nord</t>
+  </si>
+  <si>
+    <t>68 rue de l'Epeule</t>
+  </si>
+  <si>
+    <t>Roubaix</t>
+  </si>
+  <si>
+    <t>59100</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU42"/>
+  <dimension ref="A1:CU44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,97 +1519,97 @@
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AH1" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AT1" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="AL1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>16</v>
@@ -1594,7 +1618,7 @@
         <v>17</v>
       </c>
       <c r="AX1" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AY1" s="3" t="s">
         <v>18</v>
@@ -1624,10 +1648,10 @@
         <v>26</v>
       </c>
       <c r="BH1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BI1" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="BJ1" s="3" t="s">
         <v>27</v>
@@ -1645,7 +1669,7 @@
         <v>31</v>
       </c>
       <c r="BO1" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="BP1" s="3" t="s">
         <v>32</v>
@@ -1657,10 +1681,10 @@
         <v>34</v>
       </c>
       <c r="BS1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="BT1" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="BU1" s="3" t="s">
         <v>35</v>
@@ -1678,70 +1702,70 @@
         <v>39</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="CA1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="CB1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="CC1" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="CD1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="CE1" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="CF1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="CG1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="CG1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="CH1" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="CI1" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="CJ1" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="CJ1" s="16" t="s">
+      <c r="CK1" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="CK1" s="16" t="s">
+      <c r="CL1" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="CL1" s="16" t="s">
+      <c r="CM1" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="CM1" s="16" t="s">
+      <c r="CN1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="CN1" s="16" t="s">
+      <c r="CO1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="CO1" s="16" t="s">
+      <c r="CP1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="CP1" s="16" t="s">
+      <c r="CQ1" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="CQ1" s="17" t="s">
-        <v>207</v>
-      </c>
       <c r="CR1" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="CS1" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="CT1" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="CU1" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.3">
@@ -1749,10 +1773,10 @@
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1815,10 +1839,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -2362,7 +2386,7 @@
     </row>
     <row r="14" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D14" t="s">
         <v>76</v>
@@ -2428,19 +2452,34 @@
       </c>
       <c r="BH14" s="11"/>
       <c r="BI14" s="11"/>
+      <c r="BJ14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="BL14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM14" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BN14" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="BP14" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BQ14" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="BR14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
         <v>76</v>
@@ -2452,7 +2491,7 @@
         <v>78</v>
       </c>
       <c r="I15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q15" s="4"/>
       <c r="S15" s="4"/>
@@ -2481,7 +2520,7 @@
       <c r="AP15" s="4"/>
       <c r="AQ15" s="4"/>
       <c r="AZ15" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BA15" s="5" t="s">
         <v>79</v>
@@ -2500,19 +2539,34 @@
       <c r="BG15" s="11"/>
       <c r="BH15" s="11"/>
       <c r="BI15" s="11"/>
+      <c r="BJ15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="BL15" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM15" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BN15" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="BP15" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BQ15" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="BR15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D16" t="s">
         <v>76</v>
@@ -2524,7 +2578,7 @@
         <v>78</v>
       </c>
       <c r="I16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q16" s="4"/>
       <c r="S16" s="4"/>
@@ -2553,7 +2607,7 @@
       <c r="AP16" s="4"/>
       <c r="AQ16" s="4"/>
       <c r="AZ16" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="BA16" s="5" t="s">
         <v>79</v>
@@ -2572,19 +2626,34 @@
       <c r="BG16" s="11"/>
       <c r="BH16" s="11"/>
       <c r="BI16" s="11"/>
+      <c r="BJ16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="BL16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM16" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BN16" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="BP16" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BQ16" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="BR16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D17" t="s">
         <v>76</v>
@@ -2596,7 +2665,7 @@
         <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="S17" s="4"/>
@@ -2625,7 +2694,7 @@
       <c r="AP17" s="4"/>
       <c r="AQ17" s="4"/>
       <c r="AZ17" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BA17" s="5" t="s">
         <v>79</v>
@@ -2644,247 +2713,209 @@
       <c r="BG17" s="11"/>
       <c r="BH17" s="11"/>
       <c r="BI17" s="11"/>
+      <c r="BJ17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="BL17" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM17" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BN17" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="BP17" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BQ17" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="BR17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>294</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
-      </c>
-      <c r="BC18" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH18" t="s">
-        <v>108</v>
-      </c>
-      <c r="BI18" t="s">
-        <v>109</v>
-      </c>
-      <c r="BJ18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="BK18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="BL18" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="BM18" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN18" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="BO18" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="BY18" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="BZ18" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="Q18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="4"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+      <c r="AN18" s="4"/>
+      <c r="AO18" s="4"/>
+      <c r="AP18" s="4"/>
+      <c r="AQ18" s="4"/>
+      <c r="AZ18" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="BA18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC18" s="12"/>
+      <c r="BD18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE18" s="12"/>
+      <c r="BF18" s="12"/>
+      <c r="BG18" s="11"/>
+      <c r="BH18" s="11"/>
+      <c r="BI18" s="11"/>
+      <c r="BJ18" s="5"/>
+      <c r="BK18" s="5"/>
+      <c r="BL18" s="9"/>
+      <c r="BM18" s="13"/>
+      <c r="BN18" s="12"/>
+      <c r="BP18" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="BQ18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="BR18" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="19" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>92</v>
-      </c>
-      <c r="BP19" s="9" t="s">
-        <v>93</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="I19" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC19" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH19" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI19" t="s">
+        <v>108</v>
+      </c>
+      <c r="BJ19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="BL19" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM19" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BN19" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BO19" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="BZ19" s="4"/>
     </row>
     <row r="20" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>94</v>
-      </c>
-      <c r="BQ20" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="BX20" s="4" t="s">
-        <v>153</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="BC20" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="BJ20" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="BK20" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="BL20" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="BM20" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BN20" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="BO20" s="12"/>
+      <c r="BY20" s="4"/>
+      <c r="BZ20" s="4"/>
     </row>
-    <row r="21" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="L21" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="BR21" t="s">
-        <v>97</v>
-      </c>
-      <c r="BU21" s="8"/>
-      <c r="BX21" s="4" t="s">
-        <v>153</v>
+        <v>91</v>
+      </c>
+      <c r="BP21" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" t="s">
-        <v>176</v>
-      </c>
-      <c r="P22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="Y22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BQ22" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="BX22" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="4"/>
-      <c r="AD22" s="4"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="4"/>
-      <c r="AG22" s="4"/>
-      <c r="AL22" s="4"/>
-      <c r="AM22" s="4"/>
-      <c r="AN22" s="4"/>
-      <c r="AO22" s="4"/>
-      <c r="AP22" s="4"/>
-      <c r="AQ22" s="4"/>
-      <c r="AV22" s="4"/>
-      <c r="AW22" t="s">
-        <v>193</v>
-      </c>
-      <c r="AY22" s="4"/>
-      <c r="BR22" s="1"/>
-      <c r="BS22" s="1"/>
-      <c r="BT22" s="1"/>
-      <c r="BU22" t="s">
-        <v>99</v>
-      </c>
-      <c r="BV22" t="s">
-        <v>100</v>
-      </c>
-      <c r="BW22" t="s">
-        <v>101</v>
-      </c>
-      <c r="BX22" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="BY22" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BZ22" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="CA22" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="CB22" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="CC22" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="CI22">
-        <v>25</v>
-      </c>
-      <c r="CJ22">
-        <v>27</v>
-      </c>
-      <c r="CK22">
-        <v>15</v>
-      </c>
-      <c r="CL22">
-        <v>10</v>
-      </c>
-      <c r="CM22">
-        <v>30</v>
-      </c>
-      <c r="CN22">
-        <v>35</v>
-      </c>
-      <c r="CO22">
-        <v>32</v>
-      </c>
-      <c r="CP22">
-        <v>23</v>
-      </c>
-      <c r="CQ22" t="s">
-        <v>76</v>
-      </c>
     </row>
-    <row r="23" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>275</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="C23" s="4"/>
       <c r="L23" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="4"/>
-      <c r="AC23" s="4"/>
-      <c r="AD23" s="4"/>
-      <c r="AE23" s="15"/>
-      <c r="AF23" s="4"/>
-      <c r="AG23" s="4"/>
-      <c r="AL23" s="4"/>
-      <c r="AM23" s="4"/>
-      <c r="AN23" s="4"/>
-      <c r="AO23" s="4"/>
-      <c r="AP23" s="4"/>
-      <c r="AQ23" s="4"/>
-      <c r="AV23" s="4"/>
-      <c r="AY23" s="4"/>
-      <c r="BR23" s="1"/>
-      <c r="BS23" s="1"/>
-      <c r="BT23" s="1"/>
-      <c r="BX23" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="BY23" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="BZ23" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="CA23" s="5"/>
-      <c r="CB23" s="5"/>
-      <c r="CC23" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="BR23" t="s">
+        <v>96</v>
+      </c>
+      <c r="BU23" s="8"/>
+      <c r="BX23" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="24" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>232</v>
+        <v>97</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2893,19 +2924,19 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4" t="s">
-        <v>237</v>
+        <v>119</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
       <c r="Y24" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
@@ -2915,58 +2946,46 @@
       <c r="AE24" s="15"/>
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
-      <c r="AH24" s="4"/>
-      <c r="AI24" s="4"/>
-      <c r="AJ24" s="4"/>
-      <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
       <c r="AM24" s="4"/>
       <c r="AN24" s="4"/>
       <c r="AO24" s="4"/>
       <c r="AP24" s="4"/>
       <c r="AQ24" s="4"/>
-      <c r="AR24" t="s">
-        <v>236</v>
-      </c>
       <c r="AV24" s="4"/>
       <c r="AW24" t="s">
-        <v>239</v>
-      </c>
-      <c r="AX24" t="s">
-        <v>241</v>
+        <v>192</v>
       </c>
       <c r="AY24" s="4"/>
       <c r="BR24" s="1"/>
-      <c r="BS24" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="BT24" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="BS24" s="1"/>
+      <c r="BT24" s="1"/>
       <c r="BU24" t="s">
+        <v>98</v>
+      </c>
+      <c r="BV24" t="s">
         <v>99</v>
       </c>
-      <c r="BV24" t="s">
+      <c r="BW24" t="s">
         <v>100</v>
       </c>
-      <c r="BW24" t="s">
+      <c r="BX24" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="BY24" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="BX24" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="BY24" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BZ24" s="4"/>
+      <c r="BZ24" s="4" t="s">
+        <v>257</v>
+      </c>
       <c r="CA24" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="CB24" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="CC24" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="CI24">
         <v>25</v>
@@ -2998,85 +3017,59 @@
     </row>
     <row r="25" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>116</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="P25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
-      <c r="Y25" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
-      <c r="AD25" s="15"/>
+      <c r="AD25" s="4"/>
       <c r="AE25" s="15"/>
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AJ25" s="4"/>
-      <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
       <c r="AM25" s="4"/>
       <c r="AN25" s="4"/>
       <c r="AO25" s="4"/>
       <c r="AP25" s="4"/>
       <c r="AQ25" s="4"/>
-      <c r="BN25" s="6"/>
-      <c r="BO25" s="6"/>
-      <c r="BP25" s="7"/>
-      <c r="BQ25" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="BX25" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="BY25" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="BZ25" s="14"/>
-      <c r="CA25" t="s">
-        <v>189</v>
-      </c>
-      <c r="CB25" t="s">
-        <v>192</v>
-      </c>
-      <c r="CD25" t="s">
-        <v>114</v>
-      </c>
-      <c r="CE25" t="s">
-        <v>39</v>
-      </c>
-      <c r="CI25">
-        <v>25</v>
-      </c>
-      <c r="CJ25">
-        <v>27</v>
-      </c>
-      <c r="CK25">
-        <v>15</v>
-      </c>
-      <c r="CL25">
-        <v>10</v>
-      </c>
-      <c r="CM25">
-        <v>30</v>
-      </c>
-      <c r="CN25">
-        <v>35</v>
-      </c>
-      <c r="CO25">
-        <v>32</v>
-      </c>
-      <c r="CP25">
-        <v>23</v>
-      </c>
+      <c r="AV25" s="4"/>
+      <c r="AY25" s="4"/>
+      <c r="BR25" s="1"/>
+      <c r="BS25" s="1"/>
+      <c r="BT25" s="1"/>
+      <c r="BX25" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="BY25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="BZ25" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="CA25" s="5"/>
+      <c r="CB25" s="5"/>
+      <c r="CC25" s="5"/>
     </row>
     <row r="26" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>231</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -3085,24 +3078,26 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4" t="s">
-        <v>120</v>
+        <v>236</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
+      <c r="O26" t="s">
+        <v>175</v>
+      </c>
       <c r="P26" s="4"/>
-      <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
+      <c r="Y26" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="Z26" s="4"/>
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
-      <c r="AE26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="15"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4"/>
@@ -3115,19 +3110,48 @@
       <c r="AO26" s="4"/>
       <c r="AP26" s="4"/>
       <c r="AQ26" s="4"/>
-      <c r="AR26" s="4"/>
-      <c r="AS26" s="4"/>
-      <c r="AT26" s="4"/>
-      <c r="AU26" s="4"/>
+      <c r="AR26" t="s">
+        <v>235</v>
+      </c>
       <c r="AV26" s="4"/>
       <c r="AW26" t="s">
-        <v>194</v>
-      </c>
-      <c r="BX26" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="BY26" s="14" t="s">
-        <v>162</v>
+        <v>238</v>
+      </c>
+      <c r="AX26" t="s">
+        <v>240</v>
+      </c>
+      <c r="AY26" s="4"/>
+      <c r="BR26" s="1"/>
+      <c r="BS26" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="BT26" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="BU26" t="s">
+        <v>98</v>
+      </c>
+      <c r="BV26" t="s">
+        <v>99</v>
+      </c>
+      <c r="BW26" t="s">
+        <v>100</v>
+      </c>
+      <c r="BX26" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="BY26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="BZ26" s="4"/>
+      <c r="CA26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="CB26" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="CC26" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="CI26">
         <v>25</v>
@@ -3152,37 +3176,27 @@
       </c>
       <c r="CP26">
         <v>23</v>
+      </c>
+      <c r="CQ26" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>121</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
+        <v>115</v>
+      </c>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
+      <c r="Y27" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="4"/>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="15"/>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
       <c r="AH27" s="4"/>
@@ -3195,25 +3209,30 @@
       <c r="AO27" s="4"/>
       <c r="AP27" s="4"/>
       <c r="AQ27" s="4"/>
-      <c r="AR27" s="4"/>
-      <c r="AS27" s="4"/>
-      <c r="AT27" s="4"/>
-      <c r="AU27" s="4"/>
-      <c r="AV27" s="4"/>
-      <c r="BN27" s="9"/>
-      <c r="BO27" s="9"/>
-      <c r="BX27" s="5" t="s">
-        <v>231</v>
+      <c r="BN27" s="6"/>
+      <c r="BO27" s="6"/>
+      <c r="BP27" s="7"/>
+      <c r="BQ27" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="BX27" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="BY27" s="14" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="BZ27" s="14"/>
-      <c r="CF27" t="s">
-        <v>195</v>
-      </c>
-      <c r="CG27" s="14" t="s">
-        <v>117</v>
+      <c r="CA27" t="s">
+        <v>188</v>
+      </c>
+      <c r="CB27" t="s">
+        <v>191</v>
+      </c>
+      <c r="CD27" t="s">
+        <v>113</v>
+      </c>
+      <c r="CE27" t="s">
+        <v>39</v>
       </c>
       <c r="CI27">
         <v>25</v>
@@ -3242,114 +3261,58 @@
     </row>
     <row r="28" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>181</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
       <c r="L28" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="O28" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>144</v>
-      </c>
-      <c r="R28" t="s">
-        <v>145</v>
-      </c>
-      <c r="S28" t="s">
-        <v>146</v>
-      </c>
-      <c r="T28" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="U28" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="V28" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="W28" t="s">
-        <v>150</v>
-      </c>
-      <c r="X28" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y28" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z28" s="4" t="s">
-        <v>154</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
-      <c r="AD28" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="AE28" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF28" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG28" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="AH28" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="AI28" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="AJ28" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="AK28" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="AL28" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="AM28" s="4">
-        <v>3</v>
-      </c>
-      <c r="AN28" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AO28" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AP28" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AQ28" s="4" t="s">
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="4"/>
+      <c r="AI28" s="4"/>
+      <c r="AJ28" s="4"/>
+      <c r="AK28" s="4"/>
+      <c r="AL28" s="4"/>
+      <c r="AM28" s="4"/>
+      <c r="AN28" s="4"/>
+      <c r="AO28" s="4"/>
+      <c r="AP28" s="4"/>
+      <c r="AQ28" s="4"/>
+      <c r="AR28" s="4"/>
+      <c r="AS28" s="4"/>
+      <c r="AT28" s="4"/>
+      <c r="AU28" s="4"/>
+      <c r="AV28" s="4"/>
+      <c r="AW28" t="s">
+        <v>193</v>
+      </c>
+      <c r="BX28" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="BY28" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="AT28" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="AU28" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AY28" s="4"/>
-      <c r="BB28" t="s">
-        <v>176</v>
-      </c>
-      <c r="BQ28" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="BU28" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="BW28" s="6"/>
-      <c r="BX28" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="BY28" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BZ28" s="4" t="s">
-        <v>258</v>
       </c>
       <c r="CI28">
         <v>25</v>
@@ -3374,31 +3337,42 @@
       </c>
       <c r="CP28">
         <v>23</v>
-      </c>
-      <c r="CQ28" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>277</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
       <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
       <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
-      <c r="AD29" s="15"/>
-      <c r="AE29" s="15"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
       <c r="AH29" s="4"/>
-      <c r="AI29" s="18"/>
-      <c r="AJ29" s="18"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
       <c r="AM29" s="4"/>
@@ -3406,24 +3380,25 @@
       <c r="AO29" s="4"/>
       <c r="AP29" s="4"/>
       <c r="AQ29" s="4"/>
+      <c r="AR29" s="4"/>
+      <c r="AS29" s="4"/>
       <c r="AT29" s="4"/>
       <c r="AU29" s="4"/>
-      <c r="AY29" s="4"/>
-      <c r="BQ29" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="BU29" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="BW29" s="6"/>
-      <c r="BX29" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="BY29" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BZ29" s="4" t="s">
-        <v>258</v>
+      <c r="AV29" s="4"/>
+      <c r="BN29" s="9"/>
+      <c r="BO29" s="9"/>
+      <c r="BX29" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="BY29" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="BZ29" s="14"/>
+      <c r="CF29" t="s">
+        <v>194</v>
+      </c>
+      <c r="CG29" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="CI29">
         <v>25</v>
@@ -3448,116 +3423,118 @@
       </c>
       <c r="CP29">
         <v>23</v>
-      </c>
-      <c r="CQ29" t="s">
-        <v>76</v>
-      </c>
-      <c r="CR29" t="s">
-        <v>280</v>
-      </c>
-      <c r="CS29" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>182</v>
-      </c>
-      <c r="L30" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="O30" t="s">
+        <v>175</v>
+      </c>
       <c r="Q30" t="s">
+        <v>143</v>
+      </c>
+      <c r="R30" t="s">
         <v>144</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>145</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="T30" s="4" t="s">
+      <c r="U30" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="U30" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="V30" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="W30" t="s">
+        <v>149</v>
+      </c>
+      <c r="X30" t="s">
         <v>150</v>
       </c>
-      <c r="X30" t="s">
+      <c r="Y30" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="Y30" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="Z30" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
       <c r="AC30" s="4"/>
       <c r="AD30" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="AE30" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF30" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG30" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH30" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI30" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="AJ30" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="AK30" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="AE30" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF30" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG30" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="AH30" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="AI30" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="AJ30" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="AK30" s="4" t="s">
+      <c r="AL30" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="AL30" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="AM30" s="4">
         <v>3</v>
       </c>
       <c r="AN30" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AO30" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AO30" s="4" t="s">
+      <c r="AP30" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AP30" s="4" t="s">
+      <c r="AQ30" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AQ30" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="AT30" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AU30" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="AU30" s="4" t="s">
-        <v>254</v>
-      </c>
       <c r="AY30" s="4"/>
+      <c r="BB30" t="s">
+        <v>175</v>
+      </c>
+      <c r="BQ30" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="BU30" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="BW30" s="6"/>
       <c r="BX30" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BY30" s="4" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
       <c r="BZ30" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="CI30">
         <v>25</v>
@@ -3589,88 +3566,49 @@
     </row>
     <row r="31" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>183</v>
+        <v>276</v>
       </c>
       <c r="L31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" t="s">
-        <v>144</v>
-      </c>
-      <c r="R31" t="s">
-        <v>145</v>
-      </c>
-      <c r="S31" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="T31" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="T31" s="4"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z31" s="4" t="s">
-        <v>154</v>
-      </c>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
       <c r="AA31" s="4"/>
       <c r="AB31" s="4"/>
       <c r="AC31" s="4"/>
-      <c r="AD31" t="s">
-        <v>166</v>
-      </c>
-      <c r="AE31" s="4"/>
+      <c r="AD31" s="15"/>
+      <c r="AE31" s="15"/>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
       <c r="AH31" s="4"/>
-      <c r="AI31" s="4"/>
-      <c r="AJ31" s="4"/>
+      <c r="AI31" s="18"/>
+      <c r="AJ31" s="18"/>
       <c r="AK31" s="4"/>
       <c r="AL31" s="4"/>
       <c r="AM31" s="4"/>
       <c r="AN31" s="4"/>
-      <c r="AO31" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="AP31" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ31" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AR31" s="4"/>
-      <c r="AS31" s="4"/>
-      <c r="AT31" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="AU31" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AV31" s="4"/>
-      <c r="AW31" s="4"/>
-      <c r="AX31" s="4"/>
+      <c r="AO31" s="4"/>
+      <c r="AP31" s="4"/>
+      <c r="AQ31" s="4"/>
+      <c r="AT31" s="4"/>
+      <c r="AU31" s="4"/>
       <c r="AY31" s="4"/>
-      <c r="AZ31" s="4"/>
-      <c r="BA31" s="4"/>
-      <c r="BB31" s="4"/>
-      <c r="BC31" s="4"/>
-      <c r="BD31" s="4"/>
-      <c r="BE31" s="4"/>
-      <c r="BF31" s="4"/>
+      <c r="BQ31" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU31" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="BW31" s="6"/>
       <c r="BX31" s="4" t="s">
-        <v>153</v>
+        <v>278</v>
       </c>
       <c r="BY31" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BZ31" s="4"/>
-      <c r="CA31" t="s">
-        <v>184</v>
-      </c>
-      <c r="CB31" t="s">
-        <v>185</v>
+        <v>101</v>
+      </c>
+      <c r="BZ31" s="4" t="s">
+        <v>257</v>
       </c>
       <c r="CI31">
         <v>25</v>
@@ -3698,87 +3636,114 @@
       </c>
       <c r="CQ31" t="s">
         <v>76</v>
+      </c>
+      <c r="CR31" t="s">
+        <v>279</v>
+      </c>
+      <c r="CS31" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>186</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="P32" s="4"/>
+        <v>181</v>
+      </c>
+      <c r="L32" s="4"/>
       <c r="Q32" t="s">
+        <v>143</v>
+      </c>
+      <c r="R32" t="s">
         <v>144</v>
       </c>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4" t="s">
-        <v>170</v>
+      <c r="S32" t="s">
+        <v>145</v>
       </c>
       <c r="T32" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="V32" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="W32" t="s">
+        <v>149</v>
+      </c>
+      <c r="X32" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y32" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="Z32" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA32" s="4"/>
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
-      <c r="AD32" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="AE32" s="4"/>
-      <c r="AF32" s="4"/>
-      <c r="AG32" s="4"/>
-      <c r="AH32" s="4"/>
-      <c r="AI32" s="4"/>
-      <c r="AJ32" s="4"/>
-      <c r="AK32" s="4"/>
-      <c r="AL32" s="4"/>
-      <c r="AM32" s="4"/>
-      <c r="AN32" s="4"/>
+      <c r="AD32" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="AE32" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF32" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG32" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH32" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI32" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ32" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="AK32" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="AL32" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AM32" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN32" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="AO32" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="AP32" s="4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="AQ32" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="AR32" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="AS32" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="AT32" s="4"/>
-      <c r="AU32" s="4"/>
-      <c r="AW32" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AX32" s="4"/>
+        <v>160</v>
+      </c>
+      <c r="AT32" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AU32" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="AY32" s="4"/>
-      <c r="AZ32" s="4"/>
-      <c r="BA32" s="4"/>
-      <c r="BB32" s="4"/>
-      <c r="BC32" s="4"/>
-      <c r="BD32" s="4"/>
-      <c r="BE32" s="4"/>
-      <c r="BF32" s="4"/>
-      <c r="BW32" s="9"/>
+      <c r="BU32" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="BW32" s="6"/>
       <c r="BX32" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BY32" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BZ32" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="BZ32" s="4" t="s">
+        <v>258</v>
+      </c>
       <c r="CI32">
         <v>25</v>
       </c>
@@ -3809,28 +3774,89 @@
     </row>
     <row r="33" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>187</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>175</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="P33" s="4"/>
       <c r="Q33" t="s">
+        <v>143</v>
+      </c>
+      <c r="R33" t="s">
         <v>144</v>
       </c>
       <c r="S33" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="T33" s="4" t="s">
-        <v>170</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z33" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="4"/>
+      <c r="AI33" s="4"/>
+      <c r="AJ33" s="4"/>
+      <c r="AK33" s="4"/>
+      <c r="AL33" s="4"/>
+      <c r="AM33" s="4"/>
+      <c r="AN33" s="4"/>
+      <c r="AO33" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP33" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AQ33" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AR33" s="4"/>
+      <c r="AS33" s="4"/>
+      <c r="AT33" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AU33" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AV33" s="4"/>
+      <c r="AW33" s="4"/>
+      <c r="AX33" s="4"/>
       <c r="AY33" s="4"/>
+      <c r="AZ33" s="4"/>
+      <c r="BA33" s="4"/>
+      <c r="BB33" s="4"/>
+      <c r="BC33" s="4"/>
+      <c r="BD33" s="4"/>
+      <c r="BE33" s="4"/>
+      <c r="BF33" s="4"/>
       <c r="BX33" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BY33" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BZ33" s="4"/>
+      <c r="CA33" t="s">
+        <v>183</v>
+      </c>
+      <c r="CB33" t="s">
+        <v>184</v>
+      </c>
       <c r="CI33">
         <v>25</v>
       </c>
@@ -3861,18 +3887,83 @@
     </row>
     <row r="34" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>196</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="P34" s="4"/>
+      <c r="Q34" t="s">
+        <v>143</v>
+      </c>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="4"/>
+      <c r="AJ34" s="4"/>
+      <c r="AK34" s="4"/>
+      <c r="AL34" s="4"/>
+      <c r="AM34" s="4"/>
+      <c r="AN34" s="4"/>
+      <c r="AO34" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP34" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ34" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AR34" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AS34" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AT34" s="4"/>
+      <c r="AU34" s="4"/>
+      <c r="AW34" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AX34" s="4"/>
+      <c r="AY34" s="4"/>
+      <c r="AZ34" s="4"/>
+      <c r="BA34" s="4"/>
+      <c r="BB34" s="4"/>
+      <c r="BC34" s="4"/>
+      <c r="BD34" s="4"/>
+      <c r="BE34" s="4"/>
+      <c r="BF34" s="4"/>
+      <c r="BW34" s="9"/>
       <c r="BX34" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BY34" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BZ34" s="4"/>
-      <c r="CH34" t="s">
-        <v>198</v>
-      </c>
       <c r="CI34">
         <v>25</v>
       </c>
@@ -3903,16 +3994,26 @@
     </row>
     <row r="35" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD35" t="s">
-        <v>209</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>143</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AY35" s="4"/>
       <c r="BX35" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BY35" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BZ35" s="4"/>
       <c r="CI35">
@@ -3945,282 +4046,367 @@
     </row>
     <row r="36" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="BX36" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BY36" s="4" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
       <c r="BZ36" s="4"/>
+      <c r="CH36" t="s">
+        <v>197</v>
+      </c>
       <c r="CI36">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="CJ36">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="CK36">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="CL36">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="CM36">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="CN36">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="CO36">
         <v>32</v>
       </c>
       <c r="CP36">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="CQ36" t="s">
-        <v>212</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>207</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>208</v>
       </c>
       <c r="BX37" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BY37" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BZ37" s="4"/>
       <c r="CI37">
+        <v>25</v>
+      </c>
+      <c r="CJ37">
+        <v>27</v>
+      </c>
+      <c r="CK37">
+        <v>15</v>
+      </c>
+      <c r="CL37">
+        <v>10</v>
+      </c>
+      <c r="CM37">
+        <v>30</v>
+      </c>
+      <c r="CN37">
+        <v>35</v>
+      </c>
+      <c r="CO37">
         <v>32</v>
       </c>
-      <c r="CJ37">
-        <v>34</v>
-      </c>
-      <c r="CK37">
-        <v>54</v>
-      </c>
-      <c r="CL37">
-        <v>21</v>
-      </c>
-      <c r="CM37">
-        <v>13</v>
-      </c>
-      <c r="CN37">
-        <v>5</v>
-      </c>
-      <c r="CO37">
-        <v>2</v>
-      </c>
       <c r="CP37">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="CQ37" t="s">
-        <v>213</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>214</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>220</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>221</v>
-      </c>
-      <c r="AC38" t="s">
-        <v>222</v>
-      </c>
-      <c r="BU38" t="s">
-        <v>229</v>
+        <v>209</v>
+      </c>
+      <c r="BX38" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="BY38" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="BZ38" s="4"/>
+      <c r="CI38">
+        <v>12</v>
+      </c>
+      <c r="CJ38">
+        <v>32</v>
+      </c>
+      <c r="CK38">
+        <v>22</v>
+      </c>
+      <c r="CL38">
+        <v>12</v>
+      </c>
+      <c r="CM38">
+        <v>23</v>
+      </c>
+      <c r="CN38">
+        <v>20</v>
+      </c>
+      <c r="CO38">
+        <v>32</v>
+      </c>
+      <c r="CP38">
+        <v>21</v>
+      </c>
+      <c r="CQ38" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>215</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-      <c r="AA39" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>224</v>
-      </c>
-      <c r="AC39" t="s">
-        <v>225</v>
-      </c>
-      <c r="AD39" s="4"/>
-      <c r="AE39" s="4"/>
-      <c r="AF39" s="4"/>
-      <c r="AG39" s="4"/>
-      <c r="AH39" s="4"/>
-      <c r="AI39" s="4"/>
-      <c r="AJ39" s="4"/>
-      <c r="AK39" s="4"/>
-      <c r="AL39" s="4"/>
-      <c r="AM39" s="4"/>
-      <c r="AN39" s="4"/>
-      <c r="AO39" s="4"/>
-      <c r="AP39" s="4"/>
-      <c r="AQ39" s="4"/>
-      <c r="AR39" s="4"/>
-      <c r="AS39" s="4"/>
-      <c r="AT39" s="4"/>
-      <c r="AU39" s="4"/>
-      <c r="AV39" s="4"/>
-      <c r="BU39" t="s">
-        <v>230</v>
+        <v>210</v>
+      </c>
+      <c r="BX39" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="BY39" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="BZ39" s="4"/>
+      <c r="CI39">
+        <v>32</v>
+      </c>
+      <c r="CJ39">
+        <v>34</v>
+      </c>
+      <c r="CK39">
+        <v>54</v>
+      </c>
+      <c r="CL39">
+        <v>21</v>
+      </c>
+      <c r="CM39">
+        <v>13</v>
+      </c>
+      <c r="CN39">
+        <v>5</v>
+      </c>
+      <c r="CO39">
+        <v>2</v>
+      </c>
+      <c r="CP39">
+        <v>12</v>
+      </c>
+      <c r="CQ39" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AA40" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="AB40" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="AC40" t="s">
+        <v>221</v>
+      </c>
+      <c r="BU40" t="s">
         <v>228</v>
-      </c>
-      <c r="BU40" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>196</v>
-      </c>
-      <c r="U41" t="s">
-        <v>151</v>
-      </c>
-      <c r="V41" t="s">
-        <v>266</v>
-      </c>
-      <c r="AE41" t="s">
-        <v>195</v>
-      </c>
-      <c r="AG41" t="s">
-        <v>157</v>
-      </c>
-      <c r="AR41" t="s">
-        <v>267</v>
-      </c>
-      <c r="AW41" t="s">
-        <v>268</v>
-      </c>
-      <c r="AX41" t="s">
-        <v>274</v>
-      </c>
-      <c r="CB41" t="s">
-        <v>192</v>
-      </c>
-      <c r="CG41" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="CH41" t="s">
-        <v>198</v>
-      </c>
-      <c r="CI41">
-        <v>40</v>
-      </c>
-      <c r="CT41" t="s">
-        <v>274</v>
+        <v>214</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD41" s="4"/>
+      <c r="AE41" s="4"/>
+      <c r="AF41" s="4"/>
+      <c r="AG41" s="4"/>
+      <c r="AH41" s="4"/>
+      <c r="AI41" s="4"/>
+      <c r="AJ41" s="4"/>
+      <c r="AK41" s="4"/>
+      <c r="AL41" s="4"/>
+      <c r="AM41" s="4"/>
+      <c r="AN41" s="4"/>
+      <c r="AO41" s="4"/>
+      <c r="AP41" s="4"/>
+      <c r="AQ41" s="4"/>
+      <c r="AR41" s="4"/>
+      <c r="AS41" s="4"/>
+      <c r="AT41" s="4"/>
+      <c r="AU41" s="4"/>
+      <c r="AV41" s="4"/>
+      <c r="BU41" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>227</v>
+      </c>
+      <c r="BU42" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>195</v>
+      </c>
+      <c r="U43" t="s">
+        <v>150</v>
+      </c>
+      <c r="V43" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>194</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>266</v>
+      </c>
+      <c r="AW43" t="s">
+        <v>267</v>
+      </c>
+      <c r="AX43" t="s">
+        <v>273</v>
+      </c>
+      <c r="CB43" t="s">
+        <v>191</v>
+      </c>
+      <c r="CG43" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="CH43" t="s">
+        <v>197</v>
+      </c>
+      <c r="CI43">
+        <v>40</v>
+      </c>
+      <c r="CT43" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="1:99" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>268</v>
+      </c>
+      <c r="U44" t="s">
         <v>269</v>
       </c>
-      <c r="U42" t="s">
+      <c r="AW44" t="s">
         <v>270</v>
       </c>
-      <c r="AW42" t="s">
+      <c r="AX44" t="s">
         <v>271</v>
       </c>
-      <c r="AX42" t="s">
-        <v>272</v>
-      </c>
-      <c r="BX42" t="s">
-        <v>231</v>
-      </c>
-      <c r="CT42" t="s">
-        <v>272</v>
-      </c>
-      <c r="CU42" t="s">
-        <v>282</v>
+      <c r="BX44" t="s">
+        <v>230</v>
+      </c>
+      <c r="CT44" t="s">
+        <v>271</v>
+      </c>
+      <c r="CU44" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="BY34:BY37" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
-    <hyperlink ref="AH30" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
-    <hyperlink ref="AH28" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
-    <hyperlink ref="Y24" r:id="rId4" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
-    <hyperlink ref="BY24" r:id="rId5" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
-    <hyperlink ref="BY36" r:id="rId6" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
-    <hyperlink ref="BY33:BY35" r:id="rId7" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
-    <hyperlink ref="CG27" r:id="rId8" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
-    <hyperlink ref="Y22" r:id="rId9" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="BY30" r:id="rId10" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
-    <hyperlink ref="BY32" r:id="rId11" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
-    <hyperlink ref="BY31" r:id="rId12" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
-    <hyperlink ref="BY28" r:id="rId13" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
+    <hyperlink ref="BY36:BY39" r:id="rId1" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{EB5CA8C2-1562-4119-9F73-A9538DBCB59F}"/>
+    <hyperlink ref="AH32" r:id="rId2" xr:uid="{01EF0CE5-9B58-4433-9ABF-637664271D4A}"/>
+    <hyperlink ref="AH30" r:id="rId3" xr:uid="{8D00A604-39CB-4F0D-8570-A13B62ED5B4B}"/>
+    <hyperlink ref="Y26" r:id="rId4" xr:uid="{985288ED-AB06-4F73-A462-75C48E9CE552}"/>
+    <hyperlink ref="BY26" r:id="rId5" xr:uid="{713BFF2A-4E60-4EA4-AC01-3C19A2256FD8}"/>
+    <hyperlink ref="BY38" r:id="rId6" xr:uid="{A23ABB53-5727-42D8-8E0C-D85C2F423A01}"/>
+    <hyperlink ref="BY35:BY37" r:id="rId7" display="https://mcloud-na-stage.hydroflask.com/" xr:uid="{13786534-6D7A-418B-83F3-7683D4DA3272}"/>
+    <hyperlink ref="CG29" r:id="rId8" xr:uid="{A7326925-D24E-45A3-B30B-B17CA2EAC70F}"/>
+    <hyperlink ref="Y24" r:id="rId9" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
+    <hyperlink ref="BY32" r:id="rId10" xr:uid="{ADB86528-09A6-4882-AFCD-DF420D5D0BCC}"/>
+    <hyperlink ref="BY34" r:id="rId11" xr:uid="{7736404F-437A-4EE4-8F8C-7BEE74482B41}"/>
+    <hyperlink ref="BY33" r:id="rId12" xr:uid="{FC2D7836-3655-4FA9-BFF8-A8F465A50638}"/>
+    <hyperlink ref="BY30" r:id="rId13" xr:uid="{0B7C4113-A9F2-47CB-AEF4-71888DD42C4E}"/>
     <hyperlink ref="B3" r:id="rId14" xr:uid="{6B3D8009-A111-4E7B-9461-B134713DC69A}"/>
-    <hyperlink ref="Y30" r:id="rId15" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
-    <hyperlink ref="Y31" r:id="rId16" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
-    <hyperlink ref="Y28" r:id="rId17" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
-    <hyperlink ref="BY27" r:id="rId18" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
-    <hyperlink ref="BY25" r:id="rId19" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
-    <hyperlink ref="BY18" r:id="rId20" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
-    <hyperlink ref="BY22" r:id="rId21" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
+    <hyperlink ref="Y32" r:id="rId15" xr:uid="{E128BB24-CB82-4C21-9C71-14C6C15DCBF2}"/>
+    <hyperlink ref="Y33" r:id="rId16" xr:uid="{CFD5C950-2660-4740-945F-00CCEA503FA7}"/>
+    <hyperlink ref="Y30" r:id="rId17" xr:uid="{016DC2B7-E706-4737-B1F2-C90DB9A8141B}"/>
+    <hyperlink ref="BY29" r:id="rId18" xr:uid="{C8939988-54E9-4E39-A7C5-8B5A7BEE9838}"/>
+    <hyperlink ref="BY27" r:id="rId19" xr:uid="{C3E36BD8-A58A-435F-AEE0-D77C29B8BAFC}"/>
+    <hyperlink ref="BY19" r:id="rId20" xr:uid="{59F06CFA-4A9A-442F-820B-8DB95BEDB399}"/>
+    <hyperlink ref="BY24" r:id="rId21" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
     <hyperlink ref="F14" r:id="rId22" xr:uid="{385388DF-8463-40F4-A1DF-56EF41731726}"/>
     <hyperlink ref="B4" r:id="rId23" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
     <hyperlink ref="C4" r:id="rId24" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="F5" r:id="rId25" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
     <hyperlink ref="F6" r:id="rId26" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="B5" r:id="rId27" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="BZ30" r:id="rId28" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
-    <hyperlink ref="BZ28" r:id="rId29" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
-    <hyperlink ref="CG41" r:id="rId30" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
-    <hyperlink ref="BY26" r:id="rId31" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
-    <hyperlink ref="BZ23" r:id="rId32" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
-    <hyperlink ref="BY23" r:id="rId33" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
+    <hyperlink ref="BZ32" r:id="rId28" xr:uid="{E6803652-51DC-4D3E-ACC7-78FD44AECEA2}"/>
+    <hyperlink ref="BZ30" r:id="rId29" xr:uid="{568B9388-2529-4A5E-8BE2-FDB6634E32BD}"/>
+    <hyperlink ref="CG43" r:id="rId30" xr:uid="{6E8A49C1-8542-4410-B4F6-5E9AB5507439}"/>
+    <hyperlink ref="BY28" r:id="rId31" xr:uid="{9CC67629-DCE9-471E-8A66-73F5FCEDACE6}"/>
+    <hyperlink ref="BZ25" r:id="rId32" xr:uid="{2C3124E1-8E57-401F-BF4D-BB27CCCB62A4}"/>
+    <hyperlink ref="BY25" r:id="rId33" xr:uid="{E9715A60-7CAD-4F74-A49B-6ECF31016FBD}"/>
     <hyperlink ref="B2" r:id="rId34" xr:uid="{A45A2FC1-0756-4996-B77E-C3738CB0981D}"/>
-    <hyperlink ref="BY29" r:id="rId35" xr:uid="{118B4519-9553-4B2D-8F17-5D5CD3CCF7A6}"/>
-    <hyperlink ref="BZ29" r:id="rId36" xr:uid="{591C1FDE-188C-4B4E-B1F5-78AD3F842631}"/>
+    <hyperlink ref="BY31" r:id="rId35" xr:uid="{118B4519-9553-4B2D-8F17-5D5CD3CCF7A6}"/>
+    <hyperlink ref="BZ31" r:id="rId36" xr:uid="{591C1FDE-188C-4B4E-B1F5-78AD3F842631}"/>
     <hyperlink ref="F15" r:id="rId37" xr:uid="{7FF82608-09D3-4690-A1C1-AACFF7C86E9B}"/>
     <hyperlink ref="F16" r:id="rId38" xr:uid="{E4722610-7662-41AA-A24D-6A3E09EB03CA}"/>
     <hyperlink ref="F17" r:id="rId39" xr:uid="{7C3664F1-DCC7-4B88-971D-CCE87E75E636}"/>
+    <hyperlink ref="F18" r:id="rId40" xr:uid="{203B4BDF-61BF-4CA5-B715-63F89C0CE046}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>